<commit_message>
Initial character and starting relic setup
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7950CDC-A80E-AE47-BCA7-F74BC9717164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABD2079-B909-A548-8DE6-968DC57EB0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="204">
   <si>
     <t>Card</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>Deal 11 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Broken Watch</t>
   </si>
 </sst>
 </file>
@@ -757,6 +760,16 @@
   </cellStyles>
   <dxfs count="40">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -776,6 +789,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -795,26 +821,17 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -913,20 +930,6 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -941,16 +944,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A0365BF5-8AEF-1541-8A73-1FAFC18B3000}" name="Table5" displayName="Table5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A0365BF5-8AEF-1541-8A73-1FAFC18B3000}" name="Table5" displayName="Table5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{34504B4D-C4C2-9A41-B374-E8AAE8CE5F50}" name="Type Distribution" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{A000506B-CF71-5E40-9E19-3283EB9AB6A5}" name="Attack" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{34504B4D-C4C2-9A41-B374-E8AAE8CE5F50}" name="Type Distribution" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{A000506B-CF71-5E40-9E19-3283EB9AB6A5}" name="Attack" dataDxfId="36">
       <calculatedColumnFormula>COUNTIF(Attack!B:B, "Attack")+2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E4910042-1C4F-7241-AF97-15EAE0ED3526}" name="Skill" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{E4910042-1C4F-7241-AF97-15EAE0ED3526}" name="Skill" dataDxfId="35">
       <calculatedColumnFormula>COUNTIF(Skill!B:B, "Skill")+2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{ACD01204-B8A4-A94E-9713-ED0AAFE7864A}" name="Power" dataDxfId="29">
+    <tableColumn id="4" xr3:uid="{ACD01204-B8A4-A94E-9713-ED0AAFE7864A}" name="Power" dataDxfId="34">
       <calculatedColumnFormula>COUNTIF(Power!B:B, "Power")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{C4A535F2-9151-CD4A-B7A5-B26959DE0891}" name="Total" dataDxfId="33">
@@ -962,20 +965,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FBC4ED66-205A-2B4B-8038-24BE55587C8B}" name="Table6" displayName="Table6" ref="A4:F5" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FBC4ED66-205A-2B4B-8038-24BE55587C8B}" name="Table6" displayName="Table6" ref="A4:F5" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{723025F6-8AC8-A54C-B8BF-62EFE06A88F3}" name="Rarity Distribution" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{5873556F-3E30-8C41-A882-5F91FF21B2CD}" name="Starter" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{97A168A8-6B9F-D544-81CC-2F6894EAA3BD}" name="Common" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{723025F6-8AC8-A54C-B8BF-62EFE06A88F3}" name="Rarity Distribution" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{5873556F-3E30-8C41-A882-5F91FF21B2CD}" name="Starter" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{97A168A8-6B9F-D544-81CC-2F6894EAA3BD}" name="Common" dataDxfId="28">
       <calculatedColumnFormula>COUNTIF(Attack!C:C, "1 - Common") + COUNTIF(Skill!C:C, "1 - Common")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CC9EE848-AEB4-F64C-885E-A1555CBCEB7E}" name="Uncommon" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{CC9EE848-AEB4-F64C-885E-A1555CBCEB7E}" name="Uncommon" dataDxfId="27">
       <calculatedColumnFormula>COUNTIF(Attack!C:C, "2 - Uncommon") + COUNTIF(Skill!C:C, "2 - Uncommon") + COUNTIF(Power!C:C, "2 - Uncommon")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2125D09F-2585-0A4E-BC5B-5316265C0FEE}" name="Rare" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{2125D09F-2585-0A4E-BC5B-5316265C0FEE}" name="Rare" dataDxfId="26">
       <calculatedColumnFormula>COUNTIF(Attack!C:C, "3 - Rare") + COUNTIF(Skill!C:C, "3 - Rare") + COUNTIF(Power!C:C, "3 - Rare")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F99C6110-6813-294F-8E6C-4A873016DDF9}" name="Total" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{F99C6110-6813-294F-8E6C-4A873016DDF9}" name="Total" dataDxfId="25">
       <calculatedColumnFormula>SUM(Table6[[#This Row],[Starter]:[Rare]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -984,31 +987,31 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{61E7CF1C-5F0E-754C-AAD2-411AA0D4C832}" name="Table7" displayName="Table7" ref="A7:I8" totalsRowShown="0" headerRowDxfId="28" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{61E7CF1C-5F0E-754C-AAD2-411AA0D4C832}" name="Table7" displayName="Table7" ref="A7:I8" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{40AE5186-ED5B-7A43-B70B-C74345C2BF59}" name="Energy Distribution" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{6311906F-96D9-1444-8E4B-387C2346C3E9}" name="0" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{40AE5186-ED5B-7A43-B70B-C74345C2BF59}" name="Energy Distribution" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{6311906F-96D9-1444-8E4B-387C2346C3E9}" name="0" dataDxfId="21">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{70A46805-952A-8341-9D29-48388A36F6AD}" name="1" dataDxfId="17">
+    <tableColumn id="3" xr3:uid="{70A46805-952A-8341-9D29-48388A36F6AD}" name="1" dataDxfId="20">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7C55F4FE-B98F-7048-B862-BD96E32386C7}" name="2" dataDxfId="16">
+    <tableColumn id="4" xr3:uid="{7C55F4FE-B98F-7048-B862-BD96E32386C7}" name="2" dataDxfId="19">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DAABB23E-D56D-004E-A811-01E3D4E05C18}" name="3" dataDxfId="15">
+    <tableColumn id="5" xr3:uid="{DAABB23E-D56D-004E-A811-01E3D4E05C18}" name="3" dataDxfId="18">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 3) + COUNTIF(Skill!D:D, 3) + COUNTIF(Power!D:D, 3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{48BE9FBD-CD55-934B-AE03-FEE3B5119F04}" name="4+" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{48BE9FBD-CD55-934B-AE03-FEE3B5119F04}" name="4+" dataDxfId="17">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 4) + COUNTIF(Skill!D:D, 4) + COUNTIF(Power!D:D, 4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4BD6AD74-51C2-9C4D-8E88-D51309874FDA}" name="X" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{4BD6AD74-51C2-9C4D-8E88-D51309874FDA}" name="X" dataDxfId="16">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, "X") + COUNTIF(Skill!D:D, "X") + COUNTIF(Power!D:D, "X") + 1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{623CD9FD-C1D3-F744-9B45-1427C108460C}" name="-" dataDxfId="12">
+    <tableColumn id="8" xr3:uid="{623CD9FD-C1D3-F744-9B45-1427C108460C}" name="-" dataDxfId="15">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, "-") + COUNTIF(Skill!D:D, "-") + COUNTIF(Power!D:D, "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9780DADF-B233-7D42-BDCD-4E234335988C}" name="Total" dataDxfId="11">
+    <tableColumn id="9" xr3:uid="{9780DADF-B233-7D42-BDCD-4E234335988C}" name="Total" dataDxfId="14">
       <calculatedColumnFormula>SUM(Table7[[#This Row],[0]:[-]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1017,7 +1020,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7C756C6-3086-B84D-8124-5C5A39DD6F88}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7C756C6-3086-B84D-8124-5C5A39DD6F88}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:H30" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
     <sortCondition ref="C2:C30"/>
@@ -1029,10 +1032,10 @@
     <tableColumn id="1" xr3:uid="{1F29B09D-D19E-FA48-9E7F-BAC34439E0F8}" name="Card"/>
     <tableColumn id="2" xr3:uid="{3322A061-A8AA-9A47-91E6-099290785AE1}" name="Type"/>
     <tableColumn id="3" xr3:uid="{11B78D21-A734-1B49-955F-3EFE17677D89}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{C9BCFEFD-AE44-1148-97DD-210162048243}" name="Cost" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{2B64A65A-AD66-494F-9CFA-EF4A4DC964EF}" name="Effect" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{DF6D6DB9-A817-3340-9D8F-068D1C0EE55F}" name="Cost+" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{B016A6E3-657B-0E41-93E9-11821589C0D1}" name="Effect+" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C9BCFEFD-AE44-1148-97DD-210162048243}" name="Cost" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{2B64A65A-AD66-494F-9CFA-EF4A4DC964EF}" name="Effect" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{DF6D6DB9-A817-3340-9D8F-068D1C0EE55F}" name="Cost+" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{B016A6E3-657B-0E41-93E9-11821589C0D1}" name="Effect+" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{414D4855-A6B0-5141-92D1-574196120D8E}" name="Archtype"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1040,7 +1043,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E0050C6-5A96-0D4F-8EE8-DB1A30499FA5}" name="Table13" displayName="Table13" ref="A1:H31" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E0050C6-5A96-0D4F-8EE8-DB1A30499FA5}" name="Table13" displayName="Table13" ref="A1:H31" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:H31" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
     <sortCondition ref="C2:C31"/>
@@ -1052,10 +1055,10 @@
     <tableColumn id="1" xr3:uid="{D7BAF323-FB19-DE4E-8241-E8A673166D79}" name="Card"/>
     <tableColumn id="2" xr3:uid="{78259434-0171-D54A-98EB-47FDC48418DC}" name="Type"/>
     <tableColumn id="3" xr3:uid="{6BE0F913-4927-B548-8967-D2D5E241F539}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{4D4696EF-29FA-4648-A3F9-21E237630332}" name="Cost" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{17B7585E-F4A9-8A4E-A271-B6ADA1156BC1}" name="Effect" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{6DC7B496-C382-6046-8D6B-16011788E342}" name="Cost+" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{0544E40D-5A08-6543-9402-BF8DCAF50A36}" name="Effect+" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4D4696EF-29FA-4648-A3F9-21E237630332}" name="Cost" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{17B7585E-F4A9-8A4E-A271-B6ADA1156BC1}" name="Effect" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{6DC7B496-C382-6046-8D6B-16011788E342}" name="Cost+" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{0544E40D-5A08-6543-9402-BF8DCAF50A36}" name="Effect+" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{6AAC3F2A-041E-9340-A123-6AC70156CDE0}" name="Archtype"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1063,7 +1066,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:H13" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:H13" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:H13" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
     <sortCondition ref="C1:C13"/>
@@ -1072,10 +1075,10 @@
     <tableColumn id="1" xr3:uid="{4ED489C4-F350-1D4A-86C7-32EE92042A1C}" name="Card"/>
     <tableColumn id="2" xr3:uid="{AA19D34C-C869-0D44-BE2A-5180F578A4AD}" name="Type"/>
     <tableColumn id="3" xr3:uid="{AFFE9C0B-45EB-924B-9F20-5928238A8A58}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{C1331125-4439-BB41-88D7-CE7B6D51C545}" name="Cost" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{9CE4A36D-0360-6E40-8CBA-FD0E723CC355}" name="Effect" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{C1331125-4439-BB41-88D7-CE7B6D51C545}" name="Cost" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9CE4A36D-0360-6E40-8CBA-FD0E723CC355}" name="Effect" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{73F1147E-E7F4-A14F-A50E-BDFDDFB67163}" name="Cost+"/>
-    <tableColumn id="7" xr3:uid="{FF6644A0-523B-644F-B790-49B0344226F1}" name="Effect+" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{FF6644A0-523B-644F-B790-49B0344226F1}" name="Effect+" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{C57FAEB9-782E-3445-A11D-AAACD258DFFF}" name="Archtype"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1381,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878F93DA-FDEA-9E49-BD7F-EE4A9783DC48}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1720,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2396E-0670-B44C-B534-C216CC78A82B}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1747,6 +1750,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
       <c r="B2" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Implement jade mechanice and add test card
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABD2079-B909-A548-8DE6-968DC57EB0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24C2CA5-F132-FD45-894B-B9A9D0DCD09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="208">
   <si>
     <t>Card</t>
   </si>
@@ -246,9 +246,6 @@
     <t>At the end of your turn, gain 2 Block for each Jade that you have.</t>
   </si>
   <si>
-    <t>For the next 3 turns, the first card you play each turn costs 0.</t>
-  </si>
-  <si>
     <t>Gain 1 E and draw 1 card at the start of your next X turns. Exhaust.</t>
   </si>
   <si>
@@ -439,9 +436,6 @@
     <t>At the end of your turn, you can choose to place 1 card from your hand onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>The first time you consume Jade each combat, gain 1 Dexterity and 8 Block.</t>
-  </si>
-  <si>
     <t>Deal 8 damage 1 time. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
   <si>
@@ -643,12 +637,6 @@
     <t>Deal 14 damage. Place this card on top of your draw pile.</t>
   </si>
   <si>
-    <t>Deal 7 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 11 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 8 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
   </si>
   <si>
@@ -656,6 +644,30 @@
   </si>
   <si>
     <t>Broken Watch</t>
+  </si>
+  <si>
+    <t>The first time you consume Jade each combat, gain 1 E.</t>
+  </si>
+  <si>
+    <t>The next three times you consume Jade each combat, gain 1 E.</t>
+  </si>
+  <si>
+    <t>Ancient Watch</t>
+  </si>
+  <si>
+    <t>Goggles</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Twilight Assault</t>
+  </si>
+  <si>
+    <t>Deal 6 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 9 damage. Gain 1 E and 1 Jade.</t>
   </si>
 </sst>
 </file>
@@ -1020,15 +1032,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7C756C6-3086-B84D-8124-5C5A39DD6F88}" name="Table1" displayName="Table1" ref="A1:H30" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A1:H30" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7C756C6-3086-B84D-8124-5C5A39DD6F88}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A1:I30" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
     <sortCondition ref="C2:C30"/>
     <sortCondition ref="H2:H30"/>
     <sortCondition ref="D2:D30"/>
     <sortCondition ref="E2:E30"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{1F29B09D-D19E-FA48-9E7F-BAC34439E0F8}" name="Card"/>
     <tableColumn id="2" xr3:uid="{3322A061-A8AA-9A47-91E6-099290785AE1}" name="Type"/>
     <tableColumn id="3" xr3:uid="{11B78D21-A734-1B49-955F-3EFE17677D89}" name="Rarity"/>
@@ -1037,6 +1049,7 @@
     <tableColumn id="6" xr3:uid="{DF6D6DB9-A817-3340-9D8F-068D1C0EE55F}" name="Cost+" dataDxfId="10"/>
     <tableColumn id="7" xr3:uid="{B016A6E3-657B-0E41-93E9-11821589C0D1}" name="Effect+" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{414D4855-A6B0-5141-92D1-574196120D8E}" name="Archtype"/>
+    <tableColumn id="9" xr3:uid="{439B6A21-C7EA-2946-A0F2-B9310052717D}" name="Done"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1397,7 +1410,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1409,7 +1422,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1449,10 +1462,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1464,7 +1477,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1505,31 +1518,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1672,13 +1685,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1695,13 +1708,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1721,10 +1734,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2396E-0670-B44C-B534-C216CC78A82B}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,9 +1746,10 @@
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="80.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -1748,55 +1762,58 @@
       <c r="D1" s="14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>59</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1807,7 +1824,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -1818,29 +1835,35 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -1851,7 +1874,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1862,29 +1885,32 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>202</v>
+      </c>
       <c r="B13" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>55</v>
       </c>
@@ -1895,7 +1921,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>55</v>
       </c>
@@ -1906,12 +1932,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
         <v>63</v>
@@ -1931,10 +1957,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1946,9 +1972,10 @@
     <col min="6" max="6" width="12.83203125" style="10" customWidth="1"/>
     <col min="7" max="7" width="40.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1973,8 +2000,14 @@
       <c r="H1" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I1" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1985,19 +2018,22 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -2008,19 +2044,19 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -2031,19 +2067,19 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -2054,19 +2090,19 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2077,19 +2113,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -2106,13 +2142,13 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2123,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2135,7 +2171,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -2158,7 +2194,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -2169,19 +2205,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -2192,19 +2228,19 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -2215,19 +2251,19 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -2238,19 +2274,19 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2261,19 +2297,19 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -2284,19 +2320,19 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -2307,13 +2343,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -2353,13 +2389,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -2376,13 +2412,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -2399,13 +2435,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" s="10">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>44</v>
@@ -2419,13 +2455,13 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>39</v>
@@ -2442,16 +2478,16 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H22" t="s">
         <v>37</v>
@@ -2465,16 +2501,16 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H23" t="s">
         <v>37</v>
@@ -2488,16 +2524,16 @@
         <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>41</v>
@@ -2514,13 +2550,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>35</v>
@@ -2537,16 +2573,16 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="34" x14ac:dyDescent="0.2">
@@ -2560,13 +2596,13 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F27" s="2">
         <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H27" t="s">
         <v>36</v>
@@ -2583,13 +2619,13 @@
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>48</v>
@@ -2603,16 +2639,16 @@
         <v>46</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
@@ -2626,13 +2662,13 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>43</v>
@@ -2712,13 +2748,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -2735,13 +2771,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -2758,13 +2794,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -2781,13 +2817,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
@@ -2804,13 +2840,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
@@ -2827,13 +2863,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -2850,13 +2886,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -2873,13 +2909,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" t="s">
         <v>36</v>
@@ -2896,13 +2932,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H10" t="s">
         <v>37</v>
@@ -2965,13 +3001,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -2988,13 +3024,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -3011,13 +3047,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -3031,16 +3067,16 @@
         <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -3057,16 +3093,16 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="10">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="H17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="34" x14ac:dyDescent="0.2">
@@ -3080,13 +3116,13 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -3103,13 +3139,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -3123,16 +3159,16 @@
         <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>48</v>
@@ -3146,16 +3182,16 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H21" t="s">
         <v>37</v>
@@ -3169,16 +3205,16 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>37</v>
@@ -3192,16 +3228,16 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>41</v>
@@ -3218,13 +3254,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F24" s="10">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
@@ -3241,13 +3277,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
@@ -3284,19 +3320,19 @@
         <v>46</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="34" x14ac:dyDescent="0.2">
@@ -3310,13 +3346,13 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H28" t="s">
         <v>36</v>
@@ -3353,16 +3389,16 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>37</v>
@@ -3376,16 +3412,16 @@
         <v>46</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="H31" t="s">
         <v>37</v>
@@ -3455,13 +3491,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -3478,13 +3514,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -3501,13 +3537,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>35</v>
@@ -3524,13 +3560,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>38</v>
@@ -3547,13 +3583,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>38</v>
@@ -3570,13 +3606,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -3593,13 +3629,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -3639,13 +3675,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>35</v>
@@ -3685,13 +3721,13 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>36</v>
@@ -3708,13 +3744,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Fix jade, implement recall effect, and add starter deck
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24C2CA5-F132-FD45-894B-B9A9D0DCD09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BE2510-334F-DD48-AE06-8044853807A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="229">
   <si>
     <t>Card</t>
   </si>
@@ -668,6 +668,69 @@
   </si>
   <si>
     <t>Deal 9 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Star Surge</t>
+  </si>
+  <si>
+    <t>Rewind</t>
+  </si>
+  <si>
+    <t>Memento</t>
+  </si>
+  <si>
+    <t>Parallel Universe</t>
+  </si>
+  <si>
+    <t>Wormhole</t>
+  </si>
+  <si>
+    <t>Time Dilation</t>
+  </si>
+  <si>
+    <t>Temporal Paradox</t>
+  </si>
+  <si>
+    <t>Ring Singularity</t>
+  </si>
+  <si>
+    <t>Cosmic Binding</t>
+  </si>
+  <si>
+    <t>Tempered Fate</t>
+  </si>
+  <si>
+    <t>Essence Flux</t>
+  </si>
+  <si>
+    <t>Mystic Shot</t>
+  </si>
+  <si>
+    <t>Arcane Barrage</t>
+  </si>
+  <si>
+    <t>Mystic Shift</t>
+  </si>
+  <si>
+    <t>Mimic</t>
+  </si>
+  <si>
+    <t>Distorted Reality</t>
+  </si>
+  <si>
+    <t>Inherit Wisdom</t>
+  </si>
+  <si>
+    <t>Parallel Convergence</t>
+  </si>
+  <si>
+    <t>Time Bomb</t>
+  </si>
+  <si>
+    <t>Time Warp</t>
+  </si>
+  <si>
+    <t>Mystic Blast</t>
   </si>
 </sst>
 </file>
@@ -1594,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DEF958-860E-CA46-81B7-63BF564B50D2}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,6 +1741,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -1698,6 +1764,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1959,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,6 +2103,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -2355,7 +2427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -2378,7 +2450,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>208</v>
+      </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -2401,7 +2476,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>215</v>
+      </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -2424,7 +2502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -2447,7 +2525,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -2470,7 +2548,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>216</v>
+      </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -2493,7 +2574,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -2516,7 +2597,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -2539,7 +2623,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -2562,7 +2646,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>220</v>
+      </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
@@ -2585,7 +2672,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>226</v>
+      </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -2608,7 +2698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -2631,7 +2721,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>7</v>
       </c>
@@ -2654,7 +2744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>7</v>
       </c>
@@ -2697,7 +2787,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2876,6 +2966,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>213</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -2899,6 +2992,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>209</v>
+      </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -3014,6 +3110,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>211</v>
+      </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -3082,7 +3181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -3105,7 +3204,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>221</v>
+      </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -3128,7 +3230,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -3151,7 +3253,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>225</v>
+      </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -3174,7 +3279,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -3197,7 +3302,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>10</v>
       </c>
@@ -3220,7 +3325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -3243,7 +3348,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -3266,7 +3371,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -3289,7 +3394,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>222</v>
+      </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
@@ -3312,7 +3420,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>212</v>
+      </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -3335,7 +3446,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -3358,7 +3469,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>217</v>
+      </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -3381,7 +3495,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>10</v>
       </c>
@@ -3404,7 +3518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>10</v>
       </c>
@@ -3440,7 +3554,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3550,6 +3664,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -3596,6 +3713,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>224</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -3619,6 +3739,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>223</v>
+      </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -3734,6 +3857,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>214</v>
+      </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Fix starter relic and add mystic shot card
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BE2510-334F-DD48-AE06-8044853807A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A95557C-CD0E-F740-8B27-FB8DBF32F2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="258">
   <si>
     <t>Card</t>
   </si>
@@ -673,9 +673,6 @@
     <t>Star Surge</t>
   </si>
   <si>
-    <t>Rewind</t>
-  </si>
-  <si>
     <t>Memento</t>
   </si>
   <si>
@@ -697,9 +694,6 @@
     <t>Cosmic Binding</t>
   </si>
   <si>
-    <t>Tempered Fate</t>
-  </si>
-  <si>
     <t>Essence Flux</t>
   </si>
   <si>
@@ -712,12 +706,6 @@
     <t>Mystic Shift</t>
   </si>
   <si>
-    <t>Mimic</t>
-  </si>
-  <si>
-    <t>Distorted Reality</t>
-  </si>
-  <si>
     <t>Inherit Wisdom</t>
   </si>
   <si>
@@ -731,6 +719,105 @@
   </si>
   <si>
     <t>Mystic Blast</t>
+  </si>
+  <si>
+    <t>Borrowed Time</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Surge</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>Malefice</t>
+  </si>
+  <si>
+    <t>Glimpse</t>
+  </si>
+  <si>
+    <t>Boomerang Blade</t>
+  </si>
+  <si>
+    <t>Fortune's End</t>
+  </si>
+  <si>
+    <t>Fate's Edict</t>
+  </si>
+  <si>
+    <t>False Promise</t>
+  </si>
+  <si>
+    <t>Arcane Bolt</t>
+  </si>
+  <si>
+    <t>Mystic Flare</t>
+  </si>
+  <si>
+    <t>Deja Vu</t>
+  </si>
+  <si>
+    <t>Rewinder</t>
+  </si>
+  <si>
+    <t>Split Second</t>
+  </si>
+  <si>
+    <t>Time Sink</t>
+  </si>
+  <si>
+    <t>Continuum Split</t>
+  </si>
+  <si>
+    <t>Tides of Time</t>
+  </si>
+  <si>
+    <t>Distort Reality</t>
+  </si>
+  <si>
+    <t>Precognition</t>
+  </si>
+  <si>
+    <t>Temper Fate</t>
+  </si>
+  <si>
+    <t>Back in Time</t>
+  </si>
+  <si>
+    <t>Singularity</t>
+  </si>
+  <si>
+    <t>Event Horizon</t>
+  </si>
+  <si>
+    <t>While Loop</t>
+  </si>
+  <si>
+    <t>For Loop</t>
+  </si>
+  <si>
+    <t>Predestination</t>
+  </si>
+  <si>
+    <t>Butterfly Effect</t>
+  </si>
+  <si>
+    <t>Arrow of Time</t>
+  </si>
+  <si>
+    <t>Mana Ball</t>
+  </si>
+  <si>
+    <t>Mana Shield</t>
+  </si>
+  <si>
+    <t>Causality</t>
+  </si>
+  <si>
+    <t>Eternal Form</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DEF958-860E-CA46-81B7-63BF564B50D2}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1742,7 +1829,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1765,7 +1852,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2028,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2104,7 +2191,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2127,8 +2214,14 @@
       <c r="H3" t="s">
         <v>35</v>
       </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -2198,6 +2291,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -2221,6 +2317,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2290,6 +2389,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>239</v>
+      </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -2336,6 +2438,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>235</v>
+      </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -2359,6 +2464,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>253</v>
+      </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2382,6 +2490,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>254</v>
+      </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -2478,7 +2589,7 @@
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2526,6 +2637,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>250</v>
+      </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -2550,7 +2664,7 @@
     </row>
     <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2575,6 +2689,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>233</v>
+      </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -2599,7 +2716,7 @@
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2624,6 +2741,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>232</v>
+      </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -2648,7 +2768,7 @@
     </row>
     <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2674,7 +2794,7 @@
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2699,6 +2819,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -2745,6 +2868,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>228</v>
+      </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
@@ -2786,8 +2912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2828,6 +2954,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>227</v>
+      </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -2897,6 +3026,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -2920,6 +3052,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>243</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2967,7 +3102,7 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -2993,7 +3128,7 @@
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3041,6 +3176,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>256</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -3087,6 +3225,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>244</v>
+      </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -3111,7 +3252,7 @@
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3136,6 +3277,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>255</v>
+      </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -3159,6 +3303,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>248</v>
+      </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -3182,6 +3329,9 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>245</v>
+      </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -3206,7 +3356,7 @@
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3231,6 +3381,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>241</v>
+      </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -3255,7 +3408,7 @@
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3280,6 +3433,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -3303,6 +3459,9 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>249</v>
+      </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
@@ -3396,7 +3555,7 @@
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3422,7 +3581,7 @@
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3447,6 +3606,9 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>252</v>
+      </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -3471,7 +3633,7 @@
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3496,6 +3658,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>251</v>
+      </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
@@ -3665,7 +3830,7 @@
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -3690,6 +3855,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>247</v>
+      </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -3714,7 +3882,7 @@
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -3740,7 +3908,7 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -3788,6 +3956,9 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -3811,6 +3982,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>257</v>
+      </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -3834,6 +4008,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>225</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -3858,7 +4035,7 @@
     </row>
     <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Implement recall block and draw power, add 4 new cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A95557C-CD0E-F740-8B27-FB8DBF32F2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DBEBCD-6A14-D842-9C52-EF3F3EA24CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="269">
   <si>
     <t>Card</t>
   </si>
@@ -793,12 +793,6 @@
     <t>Event Horizon</t>
   </si>
   <si>
-    <t>While Loop</t>
-  </si>
-  <si>
-    <t>For Loop</t>
-  </si>
-  <si>
     <t>Predestination</t>
   </si>
   <si>
@@ -818,6 +812,45 @@
   </si>
   <si>
     <t>Eternal Form</t>
+  </si>
+  <si>
+    <t>Mystic Barrier</t>
+  </si>
+  <si>
+    <t>Lucid Dream</t>
+  </si>
+  <si>
+    <t>Flashback</t>
+  </si>
+  <si>
+    <t>Flash Forward</t>
+  </si>
+  <si>
+    <t>Big Bang</t>
+  </si>
+  <si>
+    <t>Timestream Shift</t>
+  </si>
+  <si>
+    <t>Astral Banishment</t>
+  </si>
+  <si>
+    <t>Dark Matter</t>
+  </si>
+  <si>
+    <t>Defensive Loop</t>
+  </si>
+  <si>
+    <t>Offensive Loop</t>
+  </si>
+  <si>
+    <t>Accelerate</t>
+  </si>
+  <si>
+    <t>Wheel of Time</t>
+  </si>
+  <si>
+    <t>Delayed Guard</t>
   </si>
 </sst>
 </file>
@@ -1206,15 +1239,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E0050C6-5A96-0D4F-8EE8-DB1A30499FA5}" name="Table13" displayName="Table13" ref="A1:H31" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:H31" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E0050C6-5A96-0D4F-8EE8-DB1A30499FA5}" name="Table13" displayName="Table13" ref="A1:I31" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:I31" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
     <sortCondition ref="C2:C31"/>
     <sortCondition ref="H2:H31"/>
     <sortCondition ref="D2:D31"/>
     <sortCondition ref="E2:E31"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D7BAF323-FB19-DE4E-8241-E8A673166D79}" name="Card"/>
     <tableColumn id="2" xr3:uid="{78259434-0171-D54A-98EB-47FDC48418DC}" name="Type"/>
     <tableColumn id="3" xr3:uid="{6BE0F913-4927-B548-8967-D2D5E241F539}" name="Rarity"/>
@@ -1223,18 +1256,19 @@
     <tableColumn id="6" xr3:uid="{6DC7B496-C382-6046-8D6B-16011788E342}" name="Cost+" dataDxfId="5"/>
     <tableColumn id="7" xr3:uid="{0544E40D-5A08-6543-9402-BF8DCAF50A36}" name="Effect+" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{6AAC3F2A-041E-9340-A123-6AC70156CDE0}" name="Archtype"/>
+    <tableColumn id="9" xr3:uid="{942EDD7E-F5E2-8E41-A6BC-B04682B3D06E}" name="Done"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:H13" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:H13" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:I13" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:I13" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
     <sortCondition ref="C1:C13"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4ED489C4-F350-1D4A-86C7-32EE92042A1C}" name="Card"/>
     <tableColumn id="2" xr3:uid="{AA19D34C-C869-0D44-BE2A-5180F578A4AD}" name="Type"/>
     <tableColumn id="3" xr3:uid="{AFFE9C0B-45EB-924B-9F20-5928238A8A58}" name="Rarity"/>
@@ -1243,6 +1277,7 @@
     <tableColumn id="6" xr3:uid="{73F1147E-E7F4-A14F-A50E-BDFDDFB67163}" name="Cost+"/>
     <tableColumn id="7" xr3:uid="{FF6644A0-523B-644F-B790-49B0344226F1}" name="Effect+" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{C57FAEB9-782E-3445-A11D-AAACD258DFFF}" name="Archtype"/>
+    <tableColumn id="9" xr3:uid="{52C08126-3467-FD41-9D0A-1DECCB55E8F7}" name="Done"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1893,7 +1928,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2115,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2243,6 +2278,9 @@
       <c r="H4" t="s">
         <v>35</v>
       </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -2465,7 +2503,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2491,7 +2529,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2539,6 +2577,9 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -2614,6 +2655,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>258</v>
+      </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -2638,7 +2682,7 @@
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2845,6 +2889,9 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>262</v>
+      </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
@@ -2910,10 +2957,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2925,9 +2972,10 @@
     <col min="6" max="6" width="12.83203125" style="10" customWidth="1"/>
     <col min="7" max="7" width="40.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2952,8 +3000,11 @@
       <c r="H1" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I1" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>227</v>
       </c>
@@ -2978,8 +3029,14 @@
       <c r="H2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>257</v>
+      </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -3002,7 +3059,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>256</v>
+      </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -3024,8 +3084,11 @@
       <c r="H4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3051,7 +3114,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>243</v>
       </c>
@@ -3077,7 +3140,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>268</v>
+      </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -3099,8 +3165,11 @@
       <c r="H7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -3126,9 +3195,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3152,7 +3221,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -3175,9 +3244,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3201,7 +3270,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>263</v>
+      </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -3224,7 +3296,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>244</v>
       </c>
@@ -3250,7 +3322,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>210</v>
       </c>
@@ -3276,9 +3348,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3302,7 +3374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -3460,7 +3532,7 @@
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3485,6 +3557,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>261</v>
+      </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
@@ -3508,6 +3583,9 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>260</v>
+      </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -3531,6 +3609,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>238</v>
+      </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -3607,7 +3688,7 @@
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3659,7 +3740,7 @@
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3684,6 +3765,9 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>267</v>
+      </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
@@ -3716,10 +3800,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3731,9 +3815,10 @@
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="40.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3758,8 +3843,11 @@
       <c r="H1" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I1" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -3782,7 +3870,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -3805,7 +3893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -3828,7 +3916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -3854,7 +3942,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -3880,7 +3968,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>220</v>
       </c>
@@ -3906,7 +3994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>242</v>
       </c>
@@ -3932,7 +4020,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -3955,7 +4043,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -3981,9 +4069,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4007,7 +4095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4033,7 +4121,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
Implement ArcaneBarrage actions and add 4 new cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DBEBCD-6A14-D842-9C52-EF3F3EA24CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D788FCC3-9C85-C64D-9089-860C8BCF0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="277">
   <si>
     <t>Card</t>
   </si>
@@ -694,6 +694,9 @@
     <t>Cosmic Binding</t>
   </si>
   <si>
+    <t>Tempered Fate</t>
+  </si>
+  <si>
     <t>Essence Flux</t>
   </si>
   <si>
@@ -781,9 +784,6 @@
     <t>Precognition</t>
   </si>
   <si>
-    <t>Temper Fate</t>
-  </si>
-  <si>
     <t>Back in Time</t>
   </si>
   <si>
@@ -851,6 +851,30 @@
   </si>
   <si>
     <t>Delayed Guard</t>
+  </si>
+  <si>
+    <t>Do Again</t>
+  </si>
+  <si>
+    <t>Deep Focus</t>
+  </si>
+  <si>
+    <t>Tip of the Tongue</t>
+  </si>
+  <si>
+    <t>Flashbulb</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Encode</t>
+  </si>
+  <si>
+    <t>Convergence</t>
+  </si>
+  <si>
+    <t>Astral Beam</t>
   </si>
 </sst>
 </file>
@@ -1864,7 +1888,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1887,7 +1911,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2150,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2226,7 +2250,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2255,7 +2279,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2283,6 +2307,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>271</v>
+      </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -2306,6 +2333,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>269</v>
+      </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2330,7 +2360,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2356,7 +2386,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2381,6 +2411,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>275</v>
+      </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -2404,6 +2437,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>261</v>
+      </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -2428,7 +2464,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2453,6 +2489,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -2474,10 +2513,13 @@
       <c r="H12" t="s">
         <v>35</v>
       </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2499,6 +2541,9 @@
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2554,6 +2599,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -2576,7 +2624,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>259</v>
       </c>
@@ -2602,7 +2650,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>208</v>
       </c>
@@ -2628,7 +2676,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>214</v>
       </c>
@@ -2654,7 +2702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>258</v>
       </c>
@@ -2680,7 +2728,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>265</v>
       </c>
@@ -2706,7 +2754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -2732,9 +2780,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2758,9 +2806,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2784,9 +2832,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2810,9 +2858,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2835,10 +2883,13 @@
       <c r="H26" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2862,9 +2913,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2888,7 +2939,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>262</v>
       </c>
@@ -2914,9 +2965,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -2959,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3006,7 +3057,7 @@
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3090,7 +3141,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3116,7 +3167,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3222,6 +3273,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>270</v>
+      </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -3298,7 +3352,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3399,10 +3453,13 @@
       <c r="H16" t="s">
         <v>38</v>
       </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3428,7 +3485,7 @@
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3454,7 +3511,7 @@
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3480,7 +3537,7 @@
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3506,7 +3563,7 @@
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3558,7 +3615,7 @@
     </row>
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3610,7 +3667,7 @@
     </row>
     <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3636,7 +3693,7 @@
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3803,7 +3860,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3871,6 +3928,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>216</v>
+      </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -3970,7 +4030,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -3996,7 +4056,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4045,7 +4105,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4097,7 +4157,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Implement abstract Recall power and update starter relic
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D788FCC3-9C85-C64D-9089-860C8BCF0EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF26716-2943-5A4C-93E2-CA01DF567A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -424,9 +424,6 @@
     <t>Unplayable. When you draw this card, gain 1 Intangible and 3 Jade.</t>
   </si>
   <si>
-    <t>Prevent the next time you lose HP. Gain 2 Jade when this effect triggers.</t>
-  </si>
-  <si>
     <t>Prevent the next 3 times you would obtain Jade.</t>
   </si>
   <si>
@@ -436,12 +433,6 @@
     <t>At the end of your turn, you can choose to place 1 card from your hand onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Deal 8 damage 1 time. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage 1 time. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 8 damage. When you draw this card, increase its damage by 4 this combat.</t>
   </si>
   <si>
@@ -646,12 +637,6 @@
     <t>Broken Watch</t>
   </si>
   <si>
-    <t>The first time you consume Jade each combat, gain 1 E.</t>
-  </si>
-  <si>
-    <t>The next three times you consume Jade each combat, gain 1 E.</t>
-  </si>
-  <si>
     <t>Ancient Watch</t>
   </si>
   <si>
@@ -875,6 +860,21 @@
   </si>
   <si>
     <t>Astral Beam</t>
+  </si>
+  <si>
+    <t>Deal 8 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Innate. Whenever you consume Jade, gain 1 Strength and 1 Dexterity.</t>
+  </si>
+  <si>
+    <t>The first time you consume Jade each combat, draw 2 cards.</t>
+  </si>
+  <si>
+    <t>The next 3 times you consume Jade each combat, gain 1 E and draw 2 cards.</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1619,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1631,7 +1631,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1686,7 +1686,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1727,42 +1727,42 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1897,13 +1897,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1952,7 +1952,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1978,18 +1978,18 @@
         <v>62</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>200</v>
+        <v>275</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2113,13 +2113,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>201</v>
+        <v>276</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2174,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,12 +2216,12 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2233,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2291,13 +2291,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2346,13 +2346,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2450,13 +2450,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
         <v>36</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2476,13 +2476,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>37</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2502,13 +2502,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>
@@ -2519,7 +2519,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2531,13 +2531,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2560,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2586,13 +2586,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2612,13 +2612,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2664,21 +2664,24 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
       </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2690,13 +2693,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -2704,7 +2707,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2730,7 +2733,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2739,13 +2742,13 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>39</v>
@@ -2756,7 +2759,7 @@
     </row>
     <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2765,16 +2768,16 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H22" t="s">
         <v>37</v>
@@ -2782,7 +2785,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2791,16 +2794,16 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H23" t="s">
         <v>37</v>
@@ -2808,7 +2811,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2817,16 +2820,16 @@
         <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>41</v>
@@ -2834,7 +2837,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2860,7 +2863,7 @@
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2869,16 +2872,16 @@
         <v>46</v>
       </c>
       <c r="D26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>130</v>
+        <v>272</v>
       </c>
       <c r="F26" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>131</v>
+        <v>273</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>91</v>
@@ -2889,7 +2892,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2915,7 +2918,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2927,13 +2930,13 @@
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>48</v>
@@ -2941,7 +2944,7 @@
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -2950,16 +2953,16 @@
         <v>46</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
@@ -2967,7 +2970,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -2976,13 +2979,13 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>43</v>
@@ -3010,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3052,12 +3055,12 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3086,7 +3089,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3112,7 +3115,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3124,13 +3127,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -3141,7 +3144,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3167,7 +3170,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3190,10 +3193,13 @@
       <c r="H6" t="s">
         <v>38</v>
       </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3222,7 +3228,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3234,13 +3240,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -3248,7 +3254,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3274,7 +3280,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3286,13 +3292,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H10" t="s">
         <v>37</v>
@@ -3300,7 +3306,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3323,10 +3329,13 @@
       <c r="H11" t="s">
         <v>35</v>
       </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3349,10 +3358,13 @@
       <c r="H12" t="s">
         <v>35</v>
       </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3378,7 +3390,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3404,7 +3416,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3416,13 +3428,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
@@ -3430,7 +3442,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3439,13 +3451,13 @@
         <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>111</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>112</v>
@@ -3459,7 +3471,7 @@
     </row>
     <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3485,7 +3497,7 @@
     </row>
     <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3511,7 +3523,7 @@
     </row>
     <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3523,13 +3535,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -3537,7 +3549,7 @@
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3546,13 +3558,13 @@
         <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>73</v>
@@ -3563,7 +3575,7 @@
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3572,16 +3584,16 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H21" t="s">
         <v>37</v>
@@ -3589,7 +3601,7 @@
     </row>
     <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3598,16 +3610,16 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>37</v>
@@ -3615,7 +3627,7 @@
     </row>
     <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3624,16 +3636,16 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>41</v>
@@ -3641,7 +3653,7 @@
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3667,7 +3679,7 @@
     </row>
     <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3679,13 +3691,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
@@ -3693,7 +3705,7 @@
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3719,7 +3731,7 @@
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3728,13 +3740,13 @@
         <v>46</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>80</v>
@@ -3745,7 +3757,7 @@
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3757,13 +3769,13 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H28" t="s">
         <v>36</v>
@@ -3771,7 +3783,7 @@
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3797,7 +3809,7 @@
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3806,13 +3818,13 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>89</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>90</v>
@@ -3823,7 +3835,7 @@
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3832,13 +3844,13 @@
         <v>46</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>84</v>
@@ -3860,7 +3872,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3901,7 +3913,7 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3918,10 +3930,10 @@
         <v>86</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>86</v>
+        <v>274</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -3929,7 +3941,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -3941,16 +3953,19 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>124</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3970,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>35</v>
@@ -3978,7 +3993,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -3990,21 +4005,24 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4016,13 +4034,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>38</v>
@@ -4030,7 +4048,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4056,7 +4074,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4078,6 +4096,9 @@
       </c>
       <c r="H8" t="s">
         <v>36</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4105,7 +4126,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4131,7 +4152,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4157,7 +4178,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4183,7 +4204,7 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Implement abstract X card and add 6 new cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF26716-2943-5A4C-93E2-CA01DF567A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E5892A-651B-3549-B74C-389D597D32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -285,9 +285,6 @@
     <t>Deal 4 damage. Put a random card from your discard pile into your hand.</t>
   </si>
   <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade.</t>
-  </si>
-  <si>
     <t>Double your Jade. Gain E equal to your Jade and draw 3 cards. Exhaust.</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
     <t>Prevent the next time you lose HP. Gain 1 Jade when this effect triggers.</t>
   </si>
   <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 3 Jade.</t>
-  </si>
-  <si>
     <t>Prevent the next 3 times you would obtain Jade.</t>
   </si>
   <si>
@@ -454,12 +448,6 @@
     <t>Deal 10 damage and apply 3 Vulnerable. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 6 damage and draw 2 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 9 damage and draw 3 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 10 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
   </si>
   <si>
@@ -652,9 +640,6 @@
     <t>Deal 6 damage. Gain 1 E and 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 9 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
     <t>Star Surge</t>
   </si>
   <si>
@@ -875,6 +860,21 @@
   </si>
   <si>
     <t>The next 3 times you consume Jade each combat, gain 1 E and draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage and draw 2 cards. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 9 damage and draw 1 card. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 4 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 1 Intangible and 1 Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1619,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1631,7 +1631,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1686,7 +1686,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1727,31 +1727,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>189</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1888,7 +1888,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1897,13 +1897,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1978,18 +1978,18 @@
         <v>62</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2113,13 +2113,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B13" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D13" t="s">
         <v>63</v>
@@ -2174,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,12 +2216,12 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2233,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>201</v>
+        <v>274</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2262,13 +2262,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2291,13 +2291,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2346,13 +2346,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2378,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2412,7 +2412,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2450,13 +2450,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H10" t="s">
         <v>36</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2476,13 +2476,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>37</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2502,13 +2502,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>136</v>
+        <v>273</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>137</v>
+        <v>272</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>
@@ -2519,7 +2519,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2531,13 +2531,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>35</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2560,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2586,21 +2586,24 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
       </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2612,13 +2615,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -2626,7 +2629,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2652,7 +2655,7 @@
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2664,13 +2667,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -2681,7 +2684,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2693,13 +2696,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -2707,7 +2710,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2719,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F20" s="10">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>44</v>
@@ -2733,7 +2736,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2742,13 +2745,13 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>39</v>
@@ -2759,7 +2762,7 @@
     </row>
     <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2768,16 +2771,16 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H22" t="s">
         <v>37</v>
@@ -2785,7 +2788,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2794,16 +2797,16 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H23" t="s">
         <v>37</v>
@@ -2811,7 +2814,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2820,16 +2823,16 @@
         <v>47</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>41</v>
@@ -2837,7 +2840,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2849,13 +2852,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>35</v>
@@ -2863,7 +2866,7 @@
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2875,16 +2878,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -2892,7 +2895,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2904,13 +2907,13 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="2">
         <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
         <v>36</v>
@@ -2918,7 +2921,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2930,13 +2933,13 @@
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>48</v>
@@ -2944,7 +2947,7 @@
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -2953,16 +2956,16 @@
         <v>46</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H29" t="s">
         <v>37</v>
@@ -2970,7 +2973,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -2979,19 +2982,22 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>40</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="4:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3013,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3055,12 +3061,12 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3072,13 +3078,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -3089,7 +3095,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3101,13 +3107,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -3115,7 +3121,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3127,13 +3133,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -3144,7 +3150,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3156,13 +3162,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
@@ -3170,7 +3176,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3182,13 +3188,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="H6" t="s">
         <v>38</v>
@@ -3199,7 +3205,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3211,13 +3217,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -3228,7 +3234,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3240,13 +3246,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -3254,7 +3260,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3266,13 +3272,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" t="s">
         <v>36</v>
@@ -3280,7 +3286,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3292,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
         <v>37</v>
@@ -3306,7 +3312,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3335,7 +3341,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3364,7 +3370,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3376,13 +3382,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" t="s">
         <v>38</v>
@@ -3390,7 +3396,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3402,13 +3408,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
         <v>38</v>
@@ -3416,7 +3422,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3428,21 +3434,24 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H15" t="s">
         <v>38</v>
       </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3451,16 +3460,16 @@
         <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="H16" t="s">
         <v>38</v>
@@ -3469,9 +3478,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3483,21 +3492,21 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3521,9 +3530,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3535,21 +3544,21 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3558,13 +3567,13 @@
         <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>73</v>
@@ -3573,9 +3582,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3584,24 +3593,24 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3610,24 +3619,24 @@
         <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3636,24 +3645,24 @@
         <v>47</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3665,21 +3674,21 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3691,21 +3700,21 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3728,10 +3737,13 @@
       <c r="H26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3740,24 +3752,27 @@
         <v>46</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>125</v>
+        <v>276</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>80</v>
+        <v>275</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3769,21 +3784,21 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3807,9 +3822,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3818,24 +3833,24 @@
         <v>46</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3844,19 +3859,22 @@
         <v>46</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="H31" t="s">
         <v>37</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3913,7 +3931,7 @@
         <v>34</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3927,13 +3945,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H2" t="s">
         <v>35</v>
@@ -3941,7 +3959,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -3953,13 +3971,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -3979,13 +3997,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>35</v>
@@ -3993,7 +4011,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4005,13 +4023,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>38</v>
@@ -4022,7 +4040,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4034,13 +4052,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>38</v>
@@ -4048,7 +4066,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4060,13 +4078,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -4074,7 +4092,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4086,13 +4104,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -4126,7 +4144,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4138,13 +4156,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>35</v>
@@ -4152,7 +4170,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4178,7 +4196,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4190,13 +4208,13 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>36</v>
@@ -4204,7 +4222,7 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4216,13 +4234,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Add 5 new cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E5892A-651B-3549-B74C-389D597D32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF8B778-7B5B-534C-A3A8-0BE024DF72AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="280">
   <si>
     <t>Card</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Whenever you play a cost X card, its effects are increased by 2.</t>
-  </si>
-  <si>
-    <t>Whenever you play a cost X card, its effects are increased by 3.</t>
   </si>
   <si>
     <t>Deal 10 damage. Trigger all Recall effects this turn.</t>
@@ -169,12 +166,6 @@
 Recall</t>
   </si>
   <si>
-    <t>Deal 18X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 24X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
     <t>Recall
 Jade</t>
   </si>
@@ -198,12 +189,6 @@
     <t>Deal 9 damage. Recall: Gain 9 Block.</t>
   </si>
   <si>
-    <t>Gain 8 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Gain 12 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>The first time you play a cost X card each turn, gain 1 E.</t>
   </si>
   <si>
@@ -394,12 +379,6 @@
     <t>Innate. At the end of your turn, Recall your unused E.</t>
   </si>
   <si>
-    <t>Deal 6 damage. Deal 2 additional damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Deal 3 additional damage for each Jade you have.</t>
-  </si>
-  <si>
     <t>Gain 1 E and 1 Jade. Place this card onto the top of your draw pile.</t>
   </si>
   <si>
@@ -502,12 +481,6 @@
     <t>Deal 12 damage. Recall: If this card is in your discard pile, return it to your hand.</t>
   </si>
   <si>
-    <t>Gain 4 Block. Gain 2 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
-    <t>Gain 4 Block. Gain 1 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
     <t>The next cost X card played this turn has its effects increased by 3.</t>
   </si>
   <si>
@@ -875,6 +848,42 @@
   </si>
   <si>
     <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Whenever you play a cost X card, its effects are increased by 1.</t>
+  </si>
+  <si>
+    <t>Willpower</t>
+  </si>
+  <si>
+    <t>Chain Casting</t>
+  </si>
+  <si>
+    <t>Arcane Blessing</t>
+  </si>
+  <si>
+    <t>Deal 20X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 15X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 8 Block. Gain 1 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Deal 2 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Deal 3 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Gain 10 Block. Gain 2 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Gain 10 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 14 Block. Gain 1 Jade.</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1628,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1631,7 +1640,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1671,10 +1680,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1686,7 +1695,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1727,42 +1736,42 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1888,7 +1897,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1897,13 +1906,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1911,7 +1920,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1923,13 +1932,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1966,7 +1975,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -1975,24 +1984,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" t="s">
         <v>58</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2000,10 +2009,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2011,10 +2020,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2022,10 +2031,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2033,10 +2042,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2044,10 +2053,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2055,24 +2064,24 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2083,10 +2092,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2094,10 +2103,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2105,57 +2114,57 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2174,8 +2183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2213,36 +2222,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -2250,28 +2259,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>275</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>117</v>
+        <v>276</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -2279,28 +2288,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -2308,97 +2317,97 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2407,111 +2416,111 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -2519,28 +2528,28 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -2548,54 +2557,54 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -2603,80 +2612,80 @@
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="10">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -2684,210 +2693,210 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F20" s="10">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -2895,106 +2904,106 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F27" s="2">
         <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>42</v>
+        <v>273</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>43</v>
+        <v>272</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -3019,8 +3028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3058,36 +3067,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3095,54 +3104,54 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>153</v>
+        <v>274</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>152</v>
+        <v>277</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -3150,54 +3159,54 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -3205,28 +3214,28 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3234,106 +3243,106 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -3341,28 +3350,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>278</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>52</v>
+        <v>279</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -3370,80 +3379,80 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -3451,28 +3460,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3480,247 +3489,247 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>183</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
@@ -3735,7 +3744,7 @@
         <v>23</v>
       </c>
       <c r="H26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3743,28 +3752,28 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -3772,106 +3781,106 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D29" s="2">
         <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -3890,7 +3899,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3928,111 +3937,120 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>271</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>269</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -4040,210 +4058,216 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>270</v>
+      </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 8 new cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF8B778-7B5B-534C-A3A8-0BE024DF72AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FABC17-1FEF-A346-9569-9E8AA08CE3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>Gain 3 E. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 9 damage. Place this card on top of your draw pile.</t>
-  </si>
-  <si>
     <t>Archtype</t>
   </si>
   <si>
@@ -304,18 +301,12 @@
 Jade</t>
   </si>
   <si>
-    <t>Draw 1 card. Place a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Gain 7 Block. Put a card from your discard pile onto the top of your draw pile.</t>
   </si>
   <si>
     <t>Gain 10 Block. Put a card from your discard pile onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Draw 2 cards. Place a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Put 2 cards from your draw pile onto the top of your draw pile. Exhaust.</t>
   </si>
   <si>
@@ -355,12 +346,6 @@
     <t>Deal 18 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
-    <t>Deal 10 damage to ALL enemies. Deal 5 additional damage for each Jade gained this combat. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage to ALL enemies. Deal 3 additional damage for each Jade gained this combat. Exhaust.</t>
-  </si>
-  <si>
     <t>Unplayable. When you draw this card, gain 1 E.</t>
   </si>
   <si>
@@ -379,12 +364,6 @@
     <t>Innate. At the end of your turn, Recall your unused E.</t>
   </si>
   <si>
-    <t>Gain 1 E and 1 Jade. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Gain 1 E and 1 Jade. Place this card onto the top of your draw pile. Ethereal.</t>
-  </si>
-  <si>
     <t>Draw 2 cards. Gain 1 Jade.</t>
   </si>
   <si>
@@ -433,12 +412,6 @@
     <t>Deal 14 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
   </si>
   <si>
-    <t>Deal 7 damage. Place the next card that you play onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Deal 11 damage. Place the next card that you play onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Deal 10 damage to the enemy for the next X turns. Exhaust.</t>
   </si>
   <si>
@@ -586,9 +559,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Deal 14 damage. Place this card on top of your draw pile.</t>
-  </si>
-  <si>
     <t>Deal 8 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
   </si>
   <si>
@@ -796,9 +766,6 @@
     <t>Delayed Guard</t>
   </si>
   <si>
-    <t>Do Again</t>
-  </si>
-  <si>
     <t>Deep Focus</t>
   </si>
   <si>
@@ -884,6 +851,39 @@
   </si>
   <si>
     <t>Gain 14 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 10 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 13 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Discard the top 3 cards of your draw pile.</t>
+  </si>
+  <si>
+    <t>Goof Off</t>
+  </si>
+  <si>
+    <t>Deal 13 damage. Discard the top 3 cards of your draw pile.</t>
+  </si>
+  <si>
+    <t>Gain 1 E and 1 Jade. Put this card onto the top of your draw pile. Ethereal.</t>
+  </si>
+  <si>
+    <t>Gain 1 E and 1 Jade. Put this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Draw 1 card. Put a card from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Draw 2 cards. Put a card from your hand onto the top of your draw pile.</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1628,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1640,7 +1640,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1695,7 +1695,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1736,31 +1736,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1906,13 +1906,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1932,13 +1932,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1975,7 +1975,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -1984,24 +1984,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2009,10 +2009,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2020,10 +2020,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2031,10 +2031,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2042,10 +2042,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2053,10 +2053,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2064,24 +2064,24 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2092,10 +2092,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2103,10 +2103,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2114,57 +2114,57 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2183,8 +2183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2222,36 +2222,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -2259,28 +2259,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -2288,28 +2288,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -2317,97 +2317,106 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>129</v>
+        <v>271</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>130</v>
+        <v>273</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>276</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>180</v>
+        <v>277</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2416,111 +2425,111 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -2528,28 +2537,28 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -2557,54 +2566,54 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -2612,39 +2621,39 @@
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -2659,33 +2668,33 @@
         <v>26</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -2693,210 +2702,216 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F20" s="10">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>104</v>
+        <v>269</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>103</v>
+        <v>270</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -2904,106 +2919,109 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F27" s="2">
         <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H29" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -3029,7 +3047,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3067,36 +3085,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3104,54 +3122,57 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>274</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>111</v>
+        <v>275</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -3159,54 +3180,57 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>86</v>
+        <v>278</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -3214,28 +3238,28 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3243,91 +3267,91 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -3342,7 +3366,7 @@
         <v>31</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -3350,28 +3374,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -3379,80 +3403,80 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -3460,28 +3484,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3489,247 +3513,250 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>174</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
@@ -3744,7 +3771,7 @@
         <v>23</v>
       </c>
       <c r="H26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3752,28 +3779,28 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -3781,39 +3808,39 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2">
         <v>3</v>
@@ -3828,59 +3855,59 @@
         <v>28</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="H30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="H31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -3937,36 +3964,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3974,28 +4001,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -4003,54 +4030,54 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -4058,80 +4085,80 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -4139,19 +4166,19 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -4160,33 +4187,33 @@
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -4194,13 +4221,13 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -4215,59 +4242,59 @@
         <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F12" s="2">
         <v>2</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor main mod name
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FABC17-1FEF-A346-9569-9E8AA08CE3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B56DE-BE8C-B443-B716-802DA92170BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -454,12 +454,6 @@
     <t>Deal 12 damage. Recall: If this card is in your discard pile, return it to your hand.</t>
   </si>
   <si>
-    <t>The next cost X card played this turn has its effects increased by 3.</t>
-  </si>
-  <si>
-    <t>The next cost X card played this turn has its effects increased by 4.</t>
-  </si>
-  <si>
     <t>Gain 7 Block. When you draw this card, increase its Block by 3 this combat.</t>
   </si>
   <si>
@@ -766,9 +760,6 @@
     <t>Delayed Guard</t>
   </si>
   <si>
-    <t>Deep Focus</t>
-  </si>
-  <si>
     <t>Tip of the Tongue</t>
   </si>
   <si>
@@ -884,6 +875,15 @@
   </si>
   <si>
     <t>Draw 2 cards. Put a card from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Spell Boost</t>
+  </si>
+  <si>
+    <t>Increase the effect of the next cost X card played by 2.</t>
+  </si>
+  <si>
+    <t>Increase the effect of the next cost X card played by 3.</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1628,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1640,7 +1640,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1695,7 +1695,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1736,31 +1736,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1897,7 +1897,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1906,13 +1906,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1987,18 +1987,18 @@
         <v>56</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D2" t="s">
         <v>57</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2122,13 +2122,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
         <v>57</v>
@@ -2183,8 +2183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2225,12 +2225,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2242,13 +2242,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2271,13 +2271,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2346,7 +2346,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2358,13 +2358,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2387,13 +2387,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2482,7 +2482,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2520,13 +2520,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2537,7 +2537,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2633,13 +2633,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2757,7 +2757,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2766,13 +2766,13 @@
         <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>122</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>37</v>
@@ -2783,7 +2783,7 @@
     </row>
     <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2792,16 +2792,16 @@
         <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H22" t="s">
         <v>35</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2818,16 +2818,16 @@
         <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2844,16 +2844,16 @@
         <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>39</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2873,13 +2873,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>33</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2902,13 +2902,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>84</v>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2957,21 +2957,24 @@
         <v>1</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F28" s="10">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -2980,16 +2983,16 @@
         <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H29" t="s">
         <v>35</v>
@@ -3000,7 +3003,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -3009,16 +3012,16 @@
         <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>38</v>
@@ -3046,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3088,12 +3091,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3122,7 +3125,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3134,13 +3137,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -3151,7 +3154,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3163,13 +3166,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -3180,7 +3183,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3192,13 +3195,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -3209,7 +3212,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3238,7 +3241,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3267,7 +3270,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3290,10 +3293,13 @@
       <c r="H8" t="s">
         <v>34</v>
       </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3316,10 +3322,13 @@
       <c r="H9" t="s">
         <v>34</v>
       </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>240</v>
+        <v>277</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3331,21 +3340,24 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>136</v>
+        <v>278</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>137</v>
+        <v>279</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
       </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3374,7 +3386,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3386,13 +3398,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -3403,7 +3415,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3429,7 +3441,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3455,7 +3467,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3473,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -3484,7 +3496,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3493,13 +3505,13 @@
         <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>100</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>101</v>
@@ -3513,7 +3525,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3539,7 +3551,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3565,7 +3577,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3577,13 +3589,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -3594,7 +3606,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3603,13 +3615,13 @@
         <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>67</v>
@@ -3620,7 +3632,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3629,16 +3641,16 @@
         <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -3646,7 +3658,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3655,13 +3667,13 @@
         <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>127</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>128</v>
@@ -3672,7 +3684,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3681,16 +3693,16 @@
         <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>39</v>
@@ -3698,7 +3710,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3724,7 +3736,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3736,13 +3748,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H25" t="s">
         <v>36</v>
@@ -3750,7 +3762,7 @@
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3779,7 +3791,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3788,16 +3800,16 @@
         <v>42</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>84</v>
@@ -3808,7 +3820,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3820,13 +3832,13 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H28" t="s">
         <v>34</v>
@@ -3834,7 +3846,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3860,7 +3872,7 @@
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3869,13 +3881,13 @@
         <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>82</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>83</v>
@@ -3886,7 +3898,7 @@
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3895,13 +3907,13 @@
         <v>42</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>77</v>
@@ -3926,7 +3938,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3967,12 +3979,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -3990,7 +4002,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -4001,7 +4013,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4030,7 +4042,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4056,7 +4068,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4085,7 +4097,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4111,7 +4123,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4137,7 +4149,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4166,7 +4178,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4178,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -4192,7 +4204,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4221,7 +4233,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4247,7 +4259,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4273,7 +4285,7 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Add 5 new power cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B003C0-8A96-4D4B-9C4A-00A66A43699C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A52285A-9014-3244-B667-362E34BC2CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="281">
   <si>
     <t>Card</t>
   </si>
@@ -316,9 +316,6 @@
     <t>Recall any unblocked damage you receive.</t>
   </si>
   <si>
-    <t>Prevent the next 2 times you would obtain Jade.</t>
-  </si>
-  <si>
     <t>Deal 14 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
@@ -352,9 +349,6 @@
     <t>Prevent the next time you lose HP. Gain 1 Jade when this effect triggers.</t>
   </si>
   <si>
-    <t>Prevent the next 3 times you would obtain Jade.</t>
-  </si>
-  <si>
     <t>Whenever you play a card, upgrade the card for the rest of the combat.</t>
   </si>
   <si>
@@ -577,9 +571,6 @@
     <t>Mystic Shift</t>
   </si>
   <si>
-    <t>Inherit Wisdom</t>
-  </si>
-  <si>
     <t>Time Bomb</t>
   </si>
   <si>
@@ -884,6 +875,18 @@
   </si>
   <si>
     <t>Whenever you consume Jade, your next Attack deals 5 additional damage.</t>
+  </si>
+  <si>
+    <t>The next 3 times you consume Jade, gain E.</t>
+  </si>
+  <si>
+    <t>The next 5 times you consume Jade, gain E.</t>
+  </si>
+  <si>
+    <t>Innate. Whenever you play a card, upgrade the card for the rest of the combat.</t>
+  </si>
+  <si>
+    <t>Inheritance</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1631,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1640,7 +1643,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1680,10 +1683,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1695,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1736,31 +1739,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1771,7 +1774,7 @@
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1779,7 +1782,7 @@
       </c>
       <c r="E8" s="9">
         <f>COUNTIF(Attack!D:D, 3) + COUNTIF(Skill!D:D, 3) + COUNTIF(Power!D:D, 3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="9">
         <f>COUNTIF(Attack!D:D, 4) + COUNTIF(Skill!D:D, 4) + COUNTIF(Power!D:D, 4)</f>
@@ -1897,7 +1900,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1906,13 +1909,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1920,7 +1923,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1932,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1987,18 +1990,18 @@
         <v>55</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2072,7 +2075,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2122,13 +2125,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D13" t="s">
         <v>56</v>
@@ -2225,12 +2228,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2242,13 +2245,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -2259,7 +2262,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2271,13 +2274,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -2288,7 +2291,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2300,13 +2303,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -2317,7 +2320,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2329,13 +2332,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -2346,7 +2349,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2358,13 +2361,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -2375,7 +2378,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2404,7 +2407,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2416,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2430,7 +2433,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2456,7 +2459,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2468,13 +2471,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
@@ -2485,7 +2488,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2497,13 +2500,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>35</v>
@@ -2511,7 +2514,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2523,13 +2526,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2540,7 +2543,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2552,13 +2555,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>33</v>
@@ -2569,7 +2572,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2581,13 +2584,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -2595,7 +2598,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2607,13 +2610,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -2624,7 +2627,7 @@
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2636,13 +2639,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
@@ -2650,7 +2653,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2676,7 +2679,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2688,13 +2691,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2714,13 +2717,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -2731,7 +2734,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2766,16 +2769,16 @@
         <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -2783,7 +2786,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2792,16 +2795,16 @@
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H22" t="s">
         <v>35</v>
@@ -2809,7 +2812,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2818,16 +2821,16 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>38</v>
@@ -2835,7 +2838,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2847,13 +2850,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -2864,7 +2867,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2876,13 +2879,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>80</v>
@@ -2893,7 +2896,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2905,13 +2908,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
@@ -2919,7 +2922,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2931,13 +2934,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>43</v>
@@ -2948,7 +2951,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2957,16 +2960,16 @@
         <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -2977,7 +2980,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -2986,16 +2989,16 @@
         <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>37</v>
@@ -3065,12 +3068,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3082,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
@@ -3099,7 +3102,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3111,13 +3114,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -3128,7 +3131,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3140,13 +3143,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -3157,7 +3160,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3169,13 +3172,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -3186,7 +3189,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3215,7 +3218,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3244,7 +3247,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3256,13 +3259,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -3270,7 +3273,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3282,13 +3285,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
@@ -3299,7 +3302,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3311,13 +3314,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -3328,7 +3331,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3357,7 +3360,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3369,13 +3372,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3412,7 +3415,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3424,13 +3427,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -3441,7 +3444,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3450,16 +3453,16 @@
         <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -3470,7 +3473,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3482,13 +3485,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>80</v>
@@ -3496,7 +3499,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3508,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3525,7 +3528,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3551,7 +3554,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3563,13 +3566,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -3580,7 +3583,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3589,13 +3592,13 @@
         <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>66</v>
@@ -3606,7 +3609,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3615,16 +3618,16 @@
         <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -3632,7 +3635,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3641,16 +3644,16 @@
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>35</v>
@@ -3658,7 +3661,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3667,16 +3670,16 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -3684,7 +3687,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3693,16 +3696,16 @@
         <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>38</v>
@@ -3710,7 +3713,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3736,7 +3739,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3748,13 +3751,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H26" t="s">
         <v>36</v>
@@ -3762,7 +3765,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3791,7 +3794,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3800,16 +3803,16 @@
         <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>80</v>
@@ -3820,7 +3823,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3832,13 +3835,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
@@ -3846,7 +3849,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3872,7 +3875,7 @@
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3881,13 +3884,13 @@
         <v>41</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>78</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>79</v>
@@ -3898,7 +3901,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3907,13 +3910,13 @@
         <v>41</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>76</v>
@@ -3938,7 +3941,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3979,12 +3982,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -3996,13 +3999,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -4013,7 +4016,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4025,13 +4028,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -4040,9 +4043,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4054,21 +4057,24 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>90</v>
+        <v>277</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>102</v>
+        <v>278</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4080,13 +4086,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>36</v>
@@ -4097,7 +4103,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4106,24 +4112,27 @@
         <v>42</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>279</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>280</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4135,21 +4144,24 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4161,13 +4173,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -4178,7 +4190,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4190,21 +4202,24 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
       </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4216,13 +4231,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -4233,7 +4248,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4259,7 +4274,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4268,13 +4283,13 @@
         <v>41</v>
       </c>
       <c r="D12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>89</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>89</v>
@@ -4282,10 +4297,13 @@
       <c r="H12" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4297,7 +4315,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Add 6 new cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A52285A-9014-3244-B667-362E34BC2CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE100F6-8BA4-2841-8FA5-1D1718B5AF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -313,9 +313,6 @@
     <t>Recall: Gain 8 Block.</t>
   </si>
   <si>
-    <t>Recall any unblocked damage you receive.</t>
-  </si>
-  <si>
     <t>Deal 14 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
@@ -799,9 +796,6 @@
     <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Draw 1 card. Put a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Draw 2 cards. Put a card from your hand onto the top of your draw pile.</t>
   </si>
   <si>
@@ -887,6 +881,12 @@
   </si>
   <si>
     <t>Inheritance</t>
+  </si>
+  <si>
+    <t>Draw 3 cards. Put a card from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Whenever you receive unblocked damage, Recall the amount of damage received as Block.</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1631,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1643,7 +1643,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1698,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1739,31 +1739,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>149</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1909,13 +1909,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1990,18 +1990,18 @@
         <v>55</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2125,13 +2125,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" t="s">
         <v>56</v>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2228,12 +2228,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2245,13 +2245,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2274,13 +2274,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2303,13 +2303,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2332,13 +2332,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2361,13 +2361,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2419,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2430,10 +2430,13 @@
       <c r="H8" t="s">
         <v>34</v>
       </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2456,10 +2459,13 @@
       <c r="H9" t="s">
         <v>34</v>
       </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2471,13 +2477,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
@@ -2488,7 +2494,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2500,21 +2506,24 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2526,13 +2535,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2543,7 +2552,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2555,13 +2564,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>33</v>
@@ -2572,7 +2581,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2584,13 +2593,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -2598,7 +2607,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2610,13 +2619,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F15" s="10">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -2627,7 +2636,7 @@
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2639,13 +2648,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="F16" s="10">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
@@ -2653,7 +2662,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2679,7 +2688,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2691,13 +2700,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -2705,7 +2714,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2717,13 +2726,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F19" s="10">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -2734,7 +2743,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2760,7 +2769,7 @@
     </row>
     <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2769,16 +2778,16 @@
         <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -2786,7 +2795,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2795,16 +2804,16 @@
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="H22" t="s">
         <v>35</v>
@@ -2812,7 +2821,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2821,16 +2830,16 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>38</v>
@@ -2838,7 +2847,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2850,13 +2859,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -2867,7 +2876,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2879,13 +2888,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="F25" s="10">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>80</v>
@@ -2896,7 +2905,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2908,13 +2917,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
@@ -2922,7 +2931,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2934,13 +2943,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="F27" s="10">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>43</v>
@@ -2951,7 +2960,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2960,16 +2969,16 @@
         <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -2980,7 +2989,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -2989,16 +2998,16 @@
         <v>41</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>37</v>
@@ -3026,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3068,12 +3077,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3085,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
@@ -3102,7 +3111,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3114,13 +3123,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -3131,7 +3140,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3143,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -3160,7 +3169,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3172,13 +3181,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -3189,7 +3198,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3218,7 +3227,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3247,7 +3256,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3259,21 +3268,24 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
       </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3285,13 +3297,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
@@ -3302,7 +3314,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3314,13 +3326,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -3331,7 +3343,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3360,7 +3372,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3372,13 +3384,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -3389,7 +3401,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3415,7 +3427,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3427,13 +3439,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -3444,7 +3456,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3453,16 +3465,16 @@
         <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -3473,7 +3485,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3485,13 +3497,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>80</v>
@@ -3499,7 +3511,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3511,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3528,7 +3540,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3554,7 +3566,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3566,13 +3578,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -3583,7 +3595,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3592,13 +3604,13 @@
         <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>66</v>
@@ -3609,7 +3621,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3618,16 +3630,16 @@
         <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -3635,7 +3647,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3644,16 +3656,16 @@
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>35</v>
@@ -3661,7 +3673,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3670,16 +3682,16 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -3687,7 +3699,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3696,16 +3708,16 @@
         <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>38</v>
@@ -3713,7 +3725,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3739,7 +3751,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3751,13 +3763,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="F26" s="10">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="H26" t="s">
         <v>36</v>
@@ -3765,7 +3777,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3794,7 +3806,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3803,16 +3815,16 @@
         <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>80</v>
@@ -3823,7 +3835,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3835,13 +3847,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
@@ -3849,7 +3861,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3875,7 +3887,7 @@
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3884,13 +3896,13 @@
         <v>41</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>78</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>79</v>
@@ -3901,7 +3913,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3910,13 +3922,13 @@
         <v>41</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>76</v>
@@ -3940,8 +3952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3982,12 +3994,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -3999,13 +4011,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -4016,7 +4028,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4028,13 +4040,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -4045,7 +4057,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4057,13 +4069,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>33</v>
@@ -4074,7 +4086,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4086,13 +4098,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>36</v>
@@ -4103,7 +4115,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4115,13 +4127,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>36</v>
@@ -4132,7 +4144,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4144,13 +4156,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
@@ -4161,7 +4173,7 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4173,13 +4185,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -4190,7 +4202,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4202,13 +4214,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -4219,7 +4231,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4231,13 +4243,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -4248,7 +4260,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4271,10 +4283,13 @@
       <c r="H11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4286,13 +4301,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>89</v>
+        <v>280</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>89</v>
+        <v>280</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>34</v>
@@ -4303,7 +4318,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4315,7 +4330,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4325,6 +4340,9 @@
       </c>
       <c r="H13" t="s">
         <v>35</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add gain and consume jade actions
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE100F6-8BA4-2841-8FA5-1D1718B5AF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06812D8C-9A9B-F749-A6B7-5055959E74B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="280">
   <si>
     <t>Card</t>
   </si>
@@ -156,10 +156,6 @@
 Jade</t>
   </si>
   <si>
-    <t>X-cost
-Recall</t>
-  </si>
-  <si>
     <t>Recall
 Jade</t>
   </si>
@@ -279,12 +275,6 @@
     <t>Deal 9 damage. Recall all your Jade.</t>
   </si>
   <si>
-    <t>Draw X cards. They cost 0 this turn. Exhaust.</t>
-  </si>
-  <si>
-    <t>Draw X+1 cards. They cost 0 this turn. Exhaust.</t>
-  </si>
-  <si>
     <t>Manipulation
 Jade</t>
   </si>
@@ -295,12 +285,6 @@
     <t>Gain 10 Block. Put a card from your discard pile onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Put 2 cards from your draw pile onto the top of your draw pile. Exhaust.</t>
-  </si>
-  <si>
-    <t>Put 3 cards from your draw pile onto the top of your draw pile. Exhaust.</t>
-  </si>
-  <si>
     <t>Draw 3 cards. Gain 1 Jade.</t>
   </si>
   <si>
@@ -424,12 +408,6 @@
     <t>Gain 1 E and draw 1 card at the start of your next X turns.</t>
   </si>
   <si>
-    <t>Gain 1 E. When you draw this card, increase its effect by 1 this combat.</t>
-  </si>
-  <si>
-    <t>Innate. Gain 1 E. When you draw this card, increase its effect by 1 this combat.</t>
-  </si>
-  <si>
     <t>Recall: If any of the enemies intend to attack, gain 24 Block. Otherwise gain 2 Artifact.</t>
   </si>
   <si>
@@ -439,33 +417,12 @@
     <t>Recall: Deal 7 damage twice X times.</t>
   </si>
   <si>
-    <t>Deal 7 damage to a random enemy X times. Apply 1 Vulnerable and 1 Weak to enemies hit 3 or more times.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage to a random enemy X times. Apply 2 Vulnerable and 2 Weak to enemies hit 3 or more times.</t>
-  </si>
-  <si>
-    <t>Can only be played if you have 3 E or more. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Can only be played if you have 3 E or more. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
     <t>If the enemy intends to attack, gain 7X Block. Otherwise, deal 8X damage.</t>
   </si>
   <si>
-    <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 11X damage.</t>
-  </si>
-  <si>
     <t>Recall: If any of the enemies intend to attack, gain 30 Block. Otherwise gain 3 Artifact.</t>
   </si>
   <si>
-    <t>At the end of this turn, retain up to X cards. Recall: They cost 1 less E this turn.</t>
-  </si>
-  <si>
-    <t>At the end of this turn, retain up to X cards. Recall: They cost 2 less E this turn.</t>
-  </si>
-  <si>
     <t>Recall: Gain 1 E.</t>
   </si>
   <si>
@@ -706,9 +663,6 @@
     <t>Flashbulb</t>
   </si>
   <si>
-    <t>Store</t>
-  </si>
-  <si>
     <t>Encode</t>
   </si>
   <si>
@@ -802,18 +756,6 @@
     <t>Spell Boost</t>
   </si>
   <si>
-    <t>Deal 4X damage to ALL enemies. Recall: Draw X cards.</t>
-  </si>
-  <si>
-    <t>Deal 6X damage to ALL enemies. Recall: Draw X cards.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Recall: If the enemy intends to attack, gain 2 Strength.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Recall: If the enemy intends to attack, gain 1 Strength.</t>
-  </si>
-  <si>
     <t>Recurring Nightmare</t>
   </si>
   <si>
@@ -871,12 +813,6 @@
     <t>Whenever you consume Jade, your next Attack deals 5 additional damage.</t>
   </si>
   <si>
-    <t>The next 3 times you consume Jade, gain E.</t>
-  </si>
-  <si>
-    <t>The next 5 times you consume Jade, gain E.</t>
-  </si>
-  <si>
     <t>Innate. Whenever you play a card, upgrade the card for the rest of the combat.</t>
   </si>
   <si>
@@ -887,6 +823,67 @@
   </si>
   <si>
     <t>Whenever you receive unblocked damage, Recall the amount of damage received as Block.</t>
+  </si>
+  <si>
+    <t>Consume a Jade and gain 1 E. When you draw this card, increase E gained from this card by 1 this combat.</t>
+  </si>
+  <si>
+    <t>Innate. Consume a Jade and gain 1 E. When you draw this card, increase E gained from this card by 1 this combat.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage to a random enemy X times. If X is 3 or more, apply 1 Vulnerable and 1 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage to a random enemy X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Require 2 E. Deal 6 damage. If you have Jade, consume Jade to deal double damage.</t>
+  </si>
+  <si>
+    <t>Require 2 E. Deal 9 damage. If you have Jade, consume Jade to deal double damage.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 6 damage to ALL enemies X times.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage. Recall all your Jade.</t>
+  </si>
+  <si>
+    <t>Require: 3 E. Draw X cards. They cost 0 this turn. Exhaust.</t>
+  </si>
+  <si>
+    <t>Require: 3 E. Draw X cards. They cost 0 this turn.</t>
+  </si>
+  <si>
+    <t>Jade
+Manipulation</t>
+  </si>
+  <si>
+    <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 10X damage.</t>
+  </si>
+  <si>
+    <t>Memorize</t>
+  </si>
+  <si>
+    <t>At the end of your turn, retain a card. Recall: It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Gain 9 Block X times. Gain 2 Jade.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Gain 12 Block X times. Gain 2 Jade.</t>
+  </si>
+  <si>
+    <t>Prevent the next 2 times you gain Jade.</t>
+  </si>
+  <si>
+    <t>Prevent the next 3 times you gain Jade.</t>
   </si>
 </sst>
 </file>
@@ -943,7 +940,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -984,6 +981,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1631,7 +1631,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1643,7 +1643,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1698,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1739,31 +1739,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1909,13 +1909,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1935,13 +1935,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1978,7 +1978,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -1987,24 +1987,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2012,10 +2012,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2023,10 +2023,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2034,10 +2034,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2045,10 +2045,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2056,10 +2056,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2067,24 +2067,24 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2095,10 +2095,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2106,10 +2106,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2117,57 +2117,57 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2228,30 +2228,30 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -2262,25 +2262,25 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -2291,25 +2291,25 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -2320,25 +2320,25 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -2349,25 +2349,25 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -2378,25 +2378,25 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
@@ -2407,19 +2407,19 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2436,25 +2436,25 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
@@ -2465,25 +2465,25 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
@@ -2494,25 +2494,25 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>35</v>
@@ -2523,25 +2523,25 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2552,161 +2552,161 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
+        <v>266</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H13" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H13" t="s">
         <v>33</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H14" t="s">
-        <v>36</v>
+      <c r="H14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="10">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
       </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>153</v>
+        <v>99</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F18" s="2">
+        <v>25</v>
+      </c>
+      <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>254</v>
+        <v>26</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -2714,25 +2714,25 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -2743,129 +2743,129 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>77</v>
+        <v>269</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>132</v>
+        <v>273</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>185</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>147</v>
+        <v>264</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -2876,28 +2876,28 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -2905,25 +2905,25 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
@@ -2931,28 +2931,28 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -2960,25 +2960,25 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>134</v>
+        <v>262</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -2989,25 +2989,25 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>37</v>
@@ -3035,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3077,30 +3077,30 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -3111,25 +3111,25 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -3140,25 +3140,25 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -3169,25 +3169,25 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -3198,25 +3198,25 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -3227,25 +3227,25 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
@@ -3256,25 +3256,25 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -3285,25 +3285,25 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
@@ -3314,25 +3314,25 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -3343,13 +3343,13 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -3372,25 +3372,25 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -3401,25 +3401,25 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>274</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>83</v>
+        <v>275</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>84</v>
+        <v>275</v>
       </c>
       <c r="H13" t="s">
         <v>36</v>
@@ -3427,25 +3427,25 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -3456,25 +3456,25 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -3485,51 +3485,51 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
@@ -3540,25 +3540,25 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -3566,25 +3566,25 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -3595,51 +3595,51 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -3647,25 +3647,25 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>35</v>
@@ -3673,25 +3673,25 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -3699,91 +3699,91 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>220</v>
+        <v>182</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>138</v>
+        <v>276</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>139</v>
+        <v>277</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>126</v>
+        <v>260</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H26" t="s">
-        <v>36</v>
+        <v>261</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
@@ -3806,28 +3806,28 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -3835,25 +3835,25 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
@@ -3861,13 +3861,13 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
@@ -3885,27 +3885,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>78</v>
+        <v>270</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>35</v>
@@ -3913,25 +3913,25 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="H32" t="s">
         <v>35</v>
@@ -3952,8 +3952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3994,30 +3994,30 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -4028,25 +4028,25 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -4057,25 +4057,25 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>33</v>
@@ -4086,25 +4086,25 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>36</v>
@@ -4115,25 +4115,25 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>36</v>
@@ -4144,25 +4144,25 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
@@ -4173,25 +4173,25 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -4202,25 +4202,25 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -4231,25 +4231,25 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>33</v>
@@ -4260,13 +4260,13 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
@@ -4289,25 +4289,25 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>34</v>
@@ -4318,19 +4318,19 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Add 5 new cards. All rare cards done
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06812D8C-9A9B-F749-A6B7-5055959E74B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3999016-D7B4-994C-8AB4-8734F473FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -408,9 +408,6 @@
     <t>Gain 1 E and draw 1 card at the start of your next X turns.</t>
   </si>
   <si>
-    <t>Recall: If any of the enemies intend to attack, gain 24 Block. Otherwise gain 2 Artifact.</t>
-  </si>
-  <si>
     <t>Recall: Deal 5 damage twice X times.</t>
   </si>
   <si>
@@ -418,9 +415,6 @@
   </si>
   <si>
     <t>If the enemy intends to attack, gain 7X Block. Otherwise, deal 8X damage.</t>
-  </si>
-  <si>
-    <t>Recall: If any of the enemies intend to attack, gain 30 Block. Otherwise gain 3 Artifact.</t>
   </si>
   <si>
     <t>Recall: Gain 1 E.</t>
@@ -884,6 +878,12 @@
   </si>
   <si>
     <t>Prevent the next 3 times you gain Jade.</t>
+  </si>
+  <si>
+    <t>Recall: If any of the enemies intend to attack, gain 22 Block. Otherwise gain 2 Artifact.</t>
+  </si>
+  <si>
+    <t>Recall: If any of the enemies intend to attack, gain 28 Block. Otherwise gain 3 Artifact.</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1631,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1643,7 +1643,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1698,7 +1698,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1739,31 +1739,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>134</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1900,7 +1900,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1909,13 +1909,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1990,18 +1990,18 @@
         <v>54</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D2" t="s">
         <v>55</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -2125,13 +2125,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D13" t="s">
         <v>55</v>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2228,12 +2228,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2245,13 +2245,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2303,13 +2303,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2332,13 +2332,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -2349,7 +2349,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2361,13 +2361,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2494,7 +2494,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2535,13 +2535,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2564,13 +2564,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2633,7 +2633,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2674,13 +2674,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H17" t="s">
         <v>36</v>
@@ -2688,7 +2688,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2761,7 +2761,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>38</v>
@@ -2769,7 +2769,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2778,16 +2778,16 @@
         <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -2804,16 +2804,16 @@
         <v>41</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>42</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2830,16 +2830,16 @@
         <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>37</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2859,13 +2859,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2888,13 +2888,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>77</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2943,13 +2943,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F27" s="10">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>42</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2969,16 +2969,16 @@
         <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -2998,16 +2998,16 @@
         <v>40</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>37</v>
@@ -3035,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3077,12 +3077,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3111,7 +3111,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3123,13 +3123,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3152,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3181,13 +3181,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3227,7 +3227,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3268,13 +3268,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3326,13 +3326,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3384,13 +3384,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3413,13 +3413,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H13" t="s">
         <v>36</v>
@@ -3427,7 +3427,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3465,13 +3465,13 @@
         <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>87</v>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3523,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3566,7 +3566,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3604,13 +3604,13 @@
         <v>41</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>64</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>65</v>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3630,13 +3630,13 @@
         <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>120</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3656,13 +3656,13 @@
         <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>110</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>111</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3682,16 +3682,16 @@
         <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3708,16 +3708,16 @@
         <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>37</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3748,10 +3748,13 @@
       <c r="H25" t="s">
         <v>33</v>
       </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3763,21 +3766,24 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3806,7 +3812,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3815,16 +3821,16 @@
         <v>40</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>77</v>
@@ -3835,7 +3841,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3847,21 +3853,24 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>121</v>
+        <v>278</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>125</v>
+        <v>279</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
       </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3884,10 +3893,13 @@
       <c r="H30" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3896,24 +3908,27 @@
         <v>40</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3922,13 +3937,13 @@
         <v>40</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>75</v>
@@ -3952,7 +3967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -3994,12 +4009,12 @@
         <v>32</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4011,13 +4026,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -4028,7 +4043,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4057,7 +4072,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4069,13 +4084,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>33</v>
@@ -4086,7 +4101,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4115,7 +4130,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4133,7 +4148,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>36</v>
@@ -4144,7 +4159,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4173,7 +4188,7 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4185,13 +4200,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -4202,7 +4217,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4214,13 +4229,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -4231,7 +4246,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4260,7 +4275,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4289,7 +4304,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4301,13 +4316,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>34</v>
@@ -4318,7 +4333,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4330,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Add 2 attack cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3999016-D7B4-994C-8AB4-8734F473FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC74D628-C5EF-F149-847D-0A52796180EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -744,9 +744,6 @@
     <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Draw 2 cards. Put a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Spell Boost</t>
   </si>
   <si>
@@ -813,9 +810,6 @@
     <t>Inheritance</t>
   </si>
   <si>
-    <t>Draw 3 cards. Put a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Whenever you receive unblocked damage, Recall the amount of damage received as Block.</t>
   </si>
   <si>
@@ -835,12 +829,6 @@
   </si>
   <si>
     <t>Deal 10 damage to a random enemy X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Require 2 E. Deal 6 damage. If you have Jade, consume Jade to deal double damage.</t>
-  </si>
-  <si>
-    <t>Require 2 E. Deal 9 damage. If you have Jade, consume Jade to deal double damage.</t>
   </si>
   <si>
     <t>Recall: Deal 6 damage to ALL enemies X times.</t>
@@ -884,6 +872,18 @@
   </si>
   <si>
     <t>Recall: If any of the enemies intend to attack, gain 28 Block. Otherwise gain 3 Artifact.</t>
+  </si>
+  <si>
+    <t>Require 2 E. Deal 5 damage. If you have Jade, consume Jade to deal 5 damage to ALL enemies.</t>
+  </si>
+  <si>
+    <t>Require 2 E. Deal 7 damage. If you have Jade, consume Jade to deal 7 damage to ALL enemies.</t>
+  </si>
+  <si>
+    <t>Scry 3. Draw 1 card.</t>
+  </si>
+  <si>
+    <t>Scry 2. Draw 1 card.</t>
   </si>
 </sst>
 </file>
@@ -1770,11 +1770,11 @@
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2550,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>196</v>
       </c>
@@ -2564,16 +2564,19 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2630,6 +2633,9 @@
       <c r="H15" t="s">
         <v>36</v>
       </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -2761,7 +2767,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>38</v>
@@ -2787,7 +2793,7 @@
         <v>131</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H21" t="s">
         <v>35</v>
@@ -2807,13 +2813,13 @@
         <v>131</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>131</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>42</v>
@@ -2833,13 +2839,13 @@
         <v>131</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>131</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>37</v>
@@ -2972,13 +2978,13 @@
         <v>131</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>131</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H28" t="s">
         <v>35</v>
@@ -3035,8 +3041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3152,13 +3158,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H4" t="s">
         <v>33</v>
@@ -3167,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -3178,16 +3184,16 @@
         <v>39</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>233</v>
+        <v>279</v>
       </c>
       <c r="F5" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -3256,7 +3262,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3268,13 +3274,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -3314,7 +3320,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3326,13 +3332,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -3390,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -3401,7 +3407,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3413,13 +3419,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H13" t="s">
         <v>36</v>
@@ -3523,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3647,7 +3653,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3673,7 +3679,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3685,13 +3691,13 @@
         <v>131</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>131</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H23" t="s">
         <v>35</v>
@@ -3711,13 +3717,13 @@
         <v>131</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>131</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>37</v>
@@ -3766,16 +3772,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3853,13 +3859,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
@@ -3911,13 +3917,13 @@
         <v>131</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>131</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>35</v>
@@ -4026,13 +4032,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -4084,13 +4090,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>33</v>
@@ -4148,7 +4154,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>36</v>
@@ -4159,7 +4165,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4200,13 +4206,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
@@ -4229,13 +4235,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -4316,13 +4322,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>34</v>
@@ -4333,7 +4339,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Add 7 cards. All Attack cards done
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC74D628-C5EF-F149-847D-0A52796180EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED3BCFC-3AFF-BE45-BD82-3F96A2E822F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="281">
   <si>
     <t>Card</t>
   </si>
@@ -114,12 +114,6 @@
   </si>
   <si>
     <t>Whenever you play a cost X card, its effects are increased by 2.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Trigger all Recall effects this turn.</t>
-  </si>
-  <si>
-    <t>Deal 14 damage. Trigger all Recall effects this turn.</t>
   </si>
   <si>
     <t>Gain 2 E. Gain 1 Jade.</t>
@@ -272,9 +266,6 @@
     <t>Your next Attack deals 9X additional damage.</t>
   </si>
   <si>
-    <t>Deal 9 damage. Recall all your Jade.</t>
-  </si>
-  <si>
     <t>Manipulation
 Jade</t>
   </si>
@@ -297,12 +288,6 @@
     <t>Recall: Gain 8 Block.</t>
   </si>
   <si>
-    <t>Deal 14 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
-  </si>
-  <si>
-    <t>Deal 18 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
-  </si>
-  <si>
     <t>Unplayable. When you draw this card, gain 1 E.</t>
   </si>
   <si>
@@ -387,12 +372,6 @@
     <t>Recall: Deal 16 damage to ALL enemies.</t>
   </si>
   <si>
-    <t>Deal 15 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
-    <t>Deal 20 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
     <t>Deal 6 damage. Recall: Deal 6 damage.</t>
   </si>
   <si>
@@ -456,12 +435,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Deal 8 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
-  </si>
-  <si>
-    <t>Deal 11 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
-  </si>
-  <si>
     <t>Broken Watch</t>
   </si>
   <si>
@@ -823,18 +796,6 @@
   </si>
   <si>
     <t>Require 3 E. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Deal 7 damage to a random enemy X times. If X is 3 or more, apply 1 Vulnerable and 1 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage to a random enemy X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Recall: Deal 6 damage to ALL enemies X times.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage. Recall all your Jade.</t>
   </si>
   <si>
     <t>Require: 3 E. Draw X cards. They cost 0 this turn. Exhaust.</t>
@@ -856,12 +817,6 @@
     <t>At the end of your turn, retain a card. Recall: It costs 0 this turn.</t>
   </si>
   <si>
-    <t>Require: 2 E. Gain 9 Block X times. Gain 2 Jade.</t>
-  </si>
-  <si>
-    <t>Require: 2 E. Gain 12 Block X times. Gain 2 Jade.</t>
-  </si>
-  <si>
     <t>Prevent the next 2 times you gain Jade.</t>
   </si>
   <si>
@@ -884,6 +839,54 @@
   </si>
   <si>
     <t>Scry 2. Draw 1 card.</t>
+  </si>
+  <si>
+    <t>Deal 9 damage. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Deal 13 damage. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Recall all your Jade.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. Recall all your Jade.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 18 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 5 damage to ALL enemies X times. If X is 3 or more, apply 1 Vulnerable and 1 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 10 damage to a random enemy X times.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 13 damage to a random enemy X times.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
+  </si>
+  <si>
+    <t>Deal 16 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Gain 8 Block and 1 Jade. Gain 9 Block X times.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Gain 10 Block and 1 Jade. Gain 10 Block X times.</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1634,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1643,7 +1646,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1683,10 +1686,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1698,7 +1701,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1739,31 +1742,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>136</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1900,7 +1903,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1909,13 +1912,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1923,7 +1926,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1935,13 +1938,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1978,7 +1981,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -1987,24 +1990,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2012,10 +2015,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2023,10 +2026,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2034,10 +2037,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2045,10 +2048,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
-      </c>
-      <c r="D6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2056,10 +2059,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -2067,24 +2070,24 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2095,10 +2098,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2106,10 +2109,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2117,57 +2120,57 @@
         <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2186,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2225,36 +2228,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -2262,28 +2265,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -2291,28 +2294,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -2320,28 +2323,28 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -2349,28 +2352,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -2378,28 +2381,28 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -2407,19 +2410,19 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2428,7 +2431,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -2436,28 +2439,28 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -2465,28 +2468,28 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>271</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>115</v>
+        <v>272</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -2494,28 +2497,28 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -2523,28 +2526,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -2552,28 +2555,28 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -2581,28 +2584,28 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -2610,28 +2613,28 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -2639,28 +2642,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -2668,80 +2671,86 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>137</v>
+        <v>267</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>138</v>
+        <v>268</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>25</v>
+        <v>265</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -2749,132 +2758,144 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>76</v>
+        <v>269</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="I22" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -2882,28 +2903,28 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -2911,54 +2932,57 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>84</v>
+        <v>277</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="H26" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F27" s="10">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -2966,28 +2990,28 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -2995,28 +3019,28 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -3041,8 +3065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3080,36 +3104,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3117,28 +3141,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -3146,28 +3170,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -3175,28 +3199,28 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -3204,28 +3228,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -3233,28 +3257,28 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3262,28 +3286,28 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -3291,28 +3315,28 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -3320,28 +3344,28 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -3349,28 +3373,28 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -3378,28 +3402,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -3407,54 +3431,54 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="H13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -3462,28 +3486,28 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -3491,54 +3515,54 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -3546,54 +3570,54 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -3601,158 +3625,158 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="H23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3760,28 +3784,28 @@
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3789,13 +3813,13 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
@@ -3810,7 +3834,7 @@
         <v>23</v>
       </c>
       <c r="H27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -3818,28 +3842,28 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -3847,28 +3871,28 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="H29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -3876,28 +3900,28 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F30" s="10">
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -3905,28 +3929,28 @@
     </row>
     <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -3934,28 +3958,28 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -4012,36 +4036,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -4049,28 +4073,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -4078,28 +4102,28 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -4107,28 +4131,28 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -4136,28 +4160,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -4165,28 +4189,28 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -4194,28 +4218,28 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -4223,28 +4247,28 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -4252,28 +4276,28 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -4281,28 +4305,28 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -4310,28 +4334,28 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -4339,19 +4363,19 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4360,7 +4384,7 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Add 8 cards. All Skill cards done
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED3BCFC-3AFF-BE45-BD82-3F96A2E822F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B883E45-9C84-F344-85A7-A7820D57529A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -642,9 +642,6 @@
     <t>Deal 8 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 10 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
-  </si>
-  <si>
     <t>The first time you consume Jade each combat, draw 2 cards.</t>
   </si>
   <si>
@@ -814,9 +811,6 @@
     <t>Memorize</t>
   </si>
   <si>
-    <t>At the end of your turn, retain a card. Recall: It costs 0 this turn.</t>
-  </si>
-  <si>
     <t>Prevent the next 2 times you gain Jade.</t>
   </si>
   <si>
@@ -883,10 +877,16 @@
     <t>Deal 16 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
-    <t>Require: 2 E. Gain 8 Block and 1 Jade. Gain 9 Block X times.</t>
-  </si>
-  <si>
     <t>Require: 2 E. Gain 10 Block and 1 Jade. Gain 10 Block X times.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Gain 8 Block and 1 Jade. Gain 8 Block X times.</t>
+  </si>
+  <si>
+    <t>Retain a card. Recall: It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
 </sst>
 </file>
@@ -2004,7 +2004,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -2134,7 +2134,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
@@ -2189,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -2306,13 +2306,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2335,13 +2335,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2364,13 +2364,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2480,13 +2480,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2538,13 +2538,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -2567,13 +2567,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H13" t="s">
         <v>31</v>
@@ -2683,13 +2683,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
@@ -2712,13 +2712,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2770,13 +2770,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2805,7 +2805,7 @@
         <v>124</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -2828,13 +2828,13 @@
         <v>124</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>124</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>40</v>
@@ -2857,13 +2857,13 @@
         <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -2886,13 +2886,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -2915,13 +2915,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="F25" s="10">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>74</v>
@@ -2944,13 +2944,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -3002,13 +3002,13 @@
         <v>124</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3031,13 +3031,13 @@
         <v>124</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>35</v>
@@ -3065,8 +3065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3153,13 +3153,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -3182,13 +3182,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3211,13 +3211,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3286,7 +3286,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3298,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3356,13 +3356,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="F10" s="10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3414,13 +3414,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3429,9 +3429,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3443,16 +3443,19 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3538,6 +3541,9 @@
       <c r="H16" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -3553,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3593,6 +3599,9 @@
       <c r="H18" t="s">
         <v>32</v>
       </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -3648,6 +3657,9 @@
       <c r="H20" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -3674,10 +3686,13 @@
       <c r="H21" t="s">
         <v>33</v>
       </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3700,10 +3715,13 @@
       <c r="H22" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3715,16 +3733,19 @@
         <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3741,16 +3762,19 @@
         <v>124</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3796,16 +3820,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F26" s="10">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3854,13 +3878,13 @@
         <v>125</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>125</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>74</v>
@@ -3883,13 +3907,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -3941,13 +3965,13 @@
         <v>124</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -4044,7 +4068,7 @@
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4056,13 +4080,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4102,7 +4126,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4114,13 +4138,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4178,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4189,7 +4213,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4230,13 +4254,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4259,13 +4283,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4346,13 +4370,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4363,7 +4387,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4375,7 +4399,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Create art for starter relic
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B883E45-9C84-F344-85A7-A7820D57529A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F64A732-E0BA-114F-8ED0-95361158F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -642,12 +642,6 @@
     <t>Deal 8 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
   <si>
-    <t>The first time you consume Jade each combat, draw 2 cards.</t>
-  </si>
-  <si>
-    <t>The next 3 times you consume Jade each combat, gain 1 E and draw 2 cards.</t>
-  </si>
-  <si>
     <t>Deal 12 damage and draw 2 cards. Gain 1 Jade.</t>
   </si>
   <si>
@@ -887,6 +881,12 @@
   </si>
   <si>
     <t>Deal 6 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>The first time you consume Jade each combat, gain E.</t>
+  </si>
+  <si>
+    <t>The first 3 times you consume Jade each combat, gain E.</t>
   </si>
 </sst>
 </file>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2396E-0670-B44C-B534-C216CC78A82B}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2004,7 +2004,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>199</v>
+        <v>279</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -2134,7 +2134,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -2306,13 +2306,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2335,13 +2335,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2364,13 +2364,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2480,13 +2480,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2538,13 +2538,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -2567,13 +2567,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H13" t="s">
         <v>31</v>
@@ -2683,13 +2683,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
@@ -2712,13 +2712,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2770,13 +2770,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2805,7 +2805,7 @@
         <v>124</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -2828,13 +2828,13 @@
         <v>124</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>124</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>40</v>
@@ -2857,13 +2857,13 @@
         <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -2886,13 +2886,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -2915,7 +2915,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
@@ -2944,13 +2944,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -3002,13 +3002,13 @@
         <v>124</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3031,13 +3031,13 @@
         <v>124</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>35</v>
@@ -3065,7 +3065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3153,13 +3153,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -3182,13 +3182,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3211,13 +3211,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3286,7 +3286,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3298,13 +3298,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3356,13 +3356,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3414,13 +3414,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3443,13 +3443,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -3559,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3721,7 +3721,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3733,13 +3733,13 @@
         <v>124</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
@@ -3762,13 +3762,13 @@
         <v>124</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
@@ -3820,16 +3820,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3878,13 +3878,13 @@
         <v>125</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>125</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>74</v>
@@ -3907,13 +3907,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -3965,13 +3965,13 @@
         <v>124</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>124</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4080,13 +4080,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4126,7 +4126,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4138,13 +4138,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4202,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4213,7 +4213,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4254,13 +4254,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4283,13 +4283,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4370,13 +4370,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4399,7 +4399,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Add 3 new relics
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F64A732-E0BA-114F-8ED0-95361158F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B47D89B-FA37-7841-AED8-2BA9EC5085F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="283">
   <si>
     <t>Card</t>
   </si>
@@ -173,9 +173,6 @@
     <t>Deal 9 damage. Recall: Gain 9 Block.</t>
   </si>
   <si>
-    <t>The first time you play a cost X card each turn, gain 1 E.</t>
-  </si>
-  <si>
     <t>Relic</t>
   </si>
   <si>
@@ -185,21 +182,12 @@
     <t>Shop</t>
   </si>
   <si>
-    <t>Remove 1 Jade at the end of your turn.</t>
-  </si>
-  <si>
     <t>Starting</t>
   </si>
   <si>
     <t>The first card you play each combat costs 0.</t>
   </si>
   <si>
-    <t>Whenever you play a X cost card, you can choose the amount of Energy to use.</t>
-  </si>
-  <si>
-    <t>The first cost X card you play each combat has its effect increased by 4.</t>
-  </si>
-  <si>
     <t>Exclusive</t>
   </si>
   <si>
@@ -212,18 +200,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>At the end of your turn, gain 2 Block for each Jade that you have.</t>
-  </si>
-  <si>
     <t>Gain 1 E and draw 1 card at the start of your next X turns. Exhaust.</t>
   </si>
   <si>
-    <t>At the start of your turn, gain 4 Block if you trigger a Recall effect.</t>
-  </si>
-  <si>
-    <t>Whenever you have unused Energy at the end of your turn, upgrade a random card in your hand for the rest of the combat.</t>
-  </si>
-  <si>
     <t>At the start of your turn, gain 2 Strength and 1 Jade.</t>
   </si>
   <si>
@@ -240,12 +219,6 @@
   </si>
   <si>
     <t>At the start of your third turn, remove all your debuffs.</t>
-  </si>
-  <si>
-    <t>Whenever your shuffle your draw pile, you can choose a card to place in your discard pile.</t>
-  </si>
-  <si>
-    <t>At the start of each combat, you can choose up to 3 cards from your draw pile to place in your discard pile.</t>
   </si>
   <si>
     <t>Deal 6 damage. Put a card from your discard pile into your hand.</t>
@@ -887,6 +860,39 @@
   </si>
   <si>
     <t>The first 3 times you consume Jade each combat, gain E.</t>
+  </si>
+  <si>
+    <t>Whenever you spend E on a cost X card, a random card in your hand costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Remove a Jade at the end of your turn.</t>
+  </si>
+  <si>
+    <t>At the start of the battle, you can choose to place up to 4 cards into your discard pile.</t>
+  </si>
+  <si>
+    <t>The first cost X card you play each combat has its effect increased by 3.</t>
+  </si>
+  <si>
+    <t>Whenever you play 4 cards that cost 0, draw 1 card.</t>
+  </si>
+  <si>
+    <t>Grimoire</t>
+  </si>
+  <si>
+    <t>Winder</t>
+  </si>
+  <si>
+    <t>The first time you trigger a Recall effect each turn, gain E.</t>
+  </si>
+  <si>
+    <t>Whenever you trigger a Recall effect, deal 2 damage to a random enemy.</t>
+  </si>
+  <si>
+    <t>Whenever you consume Jade, gain 5 Block.</t>
+  </si>
+  <si>
+    <t>Old Wine</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1640,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1646,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1686,10 +1692,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1701,7 +1707,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1742,31 +1748,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1903,7 +1909,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1912,13 +1918,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1926,7 +1932,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1938,13 +1944,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1964,10 +1970,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2396E-0670-B44C-B534-C216CC78A82B}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1981,7 +1987,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -1990,24 +1996,27 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2015,21 +2024,21 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>58</v>
+        <v>280</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>276</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2037,10 +2046,10 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>66</v>
+        <v>274</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2048,10 +2057,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>275</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2059,35 +2068,41 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>281</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>277</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2101,7 +2116,7 @@
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -2109,76 +2124,80 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>271</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>278</v>
+      </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>279</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>282</v>
+      </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>43</v>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="3"/>
-    </row>
-    <row r="62" spans="3:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="61" spans="3:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2231,12 +2250,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2248,13 +2267,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -2265,7 +2284,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2277,13 +2296,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -2294,7 +2313,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2306,13 +2325,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -2323,7 +2342,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2335,13 +2354,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2352,7 +2371,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2364,13 +2383,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2381,7 +2400,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2393,13 +2412,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
@@ -2410,7 +2429,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2422,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2439,7 +2458,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2468,7 +2487,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2480,13 +2499,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2497,7 +2516,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2509,13 +2528,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>33</v>
@@ -2526,7 +2545,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2538,13 +2557,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -2555,7 +2574,7 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2567,13 +2586,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H13" t="s">
         <v>31</v>
@@ -2584,7 +2603,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2596,13 +2615,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>31</v>
@@ -2613,7 +2632,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2625,13 +2644,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -2642,7 +2661,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2654,13 +2673,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -2671,7 +2690,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2683,13 +2702,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
@@ -2700,7 +2719,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2712,13 +2731,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2729,7 +2748,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2741,13 +2760,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -2758,7 +2777,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2770,13 +2789,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2787,7 +2806,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2796,16 +2815,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -2816,7 +2835,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -2825,16 +2844,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>40</v>
@@ -2845,7 +2864,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2854,16 +2873,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -2874,7 +2893,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2886,13 +2905,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -2903,7 +2922,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2915,16 +2934,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -2932,7 +2951,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2944,13 +2963,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -2961,7 +2980,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2973,13 +2992,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>40</v>
@@ -2990,7 +3009,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -2999,16 +3018,16 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3019,7 +3038,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3028,16 +3047,16 @@
         <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>35</v>
@@ -3107,12 +3126,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3124,13 +3143,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -3141,7 +3160,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3153,13 +3172,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -3170,7 +3189,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3182,13 +3201,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3199,7 +3218,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3211,13 +3230,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3228,7 +3247,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3240,13 +3259,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -3257,7 +3276,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3269,13 +3288,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -3286,7 +3305,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3298,13 +3317,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3315,7 +3334,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3327,13 +3346,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H9" t="s">
         <v>32</v>
@@ -3344,7 +3363,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3356,13 +3375,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3373,7 +3392,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3402,7 +3421,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3414,13 +3433,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3431,7 +3450,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3443,13 +3462,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -3460,7 +3479,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3472,13 +3491,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="H14" t="s">
         <v>34</v>
@@ -3489,7 +3508,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3498,16 +3517,16 @@
         <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -3518,7 +3537,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3530,16 +3549,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3547,7 +3566,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3559,13 +3578,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -3576,7 +3595,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3588,13 +3607,13 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -3605,7 +3624,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3617,13 +3636,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -3634,7 +3653,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3643,16 +3662,16 @@
         <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>40</v>
@@ -3663,7 +3682,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3672,16 +3691,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -3692,7 +3711,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3701,16 +3720,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3721,7 +3740,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3730,16 +3749,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
@@ -3750,7 +3769,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3759,16 +3778,16 @@
         <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
@@ -3779,7 +3798,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3791,13 +3810,13 @@
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
         <v>31</v>
@@ -3808,7 +3827,7 @@
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3820,16 +3839,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3837,7 +3856,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3866,7 +3885,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3875,19 +3894,19 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -3895,7 +3914,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3907,13 +3926,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -3924,7 +3943,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3953,7 +3972,7 @@
     </row>
     <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3962,16 +3981,16 @@
         <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -3982,7 +4001,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -3991,16 +4010,16 @@
         <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="H32" t="s">
         <v>33</v>
@@ -4063,12 +4082,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4080,13 +4099,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4097,7 +4116,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4109,13 +4128,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -4126,7 +4145,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4138,13 +4157,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4155,7 +4174,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4167,13 +4186,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>34</v>
@@ -4184,7 +4203,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4196,13 +4215,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4213,7 +4232,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4225,13 +4244,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -4242,7 +4261,7 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4254,13 +4273,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4271,7 +4290,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4283,13 +4302,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4300,7 +4319,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4312,13 +4331,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>31</v>
@@ -4329,7 +4348,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4358,7 +4377,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4370,13 +4389,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4387,7 +4406,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4399,7 +4418,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Update Recall power with priority based on order played
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B47D89B-FA37-7841-AED8-2BA9EC5085F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF112B7-23D0-DB48-ADE4-34BE4377B227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -883,9 +883,6 @@
     <t>Winder</t>
   </si>
   <si>
-    <t>The first time you trigger a Recall effect each turn, gain E.</t>
-  </si>
-  <si>
     <t>Whenever you trigger a Recall effect, deal 2 damage to a random enemy.</t>
   </si>
   <si>
@@ -893,6 +890,9 @@
   </si>
   <si>
     <t>Old Wine</t>
+  </si>
+  <si>
+    <t>Once per turn, trigger the first Recall effect twice.</t>
   </si>
 </sst>
 </file>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2024,7 +2024,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
@@ -2068,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -2166,7 +2166,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D14" t="s">
         <v>49</v>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Add 8 relics. All relics done
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF112B7-23D0-DB48-ADE4-34BE4377B227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E5558-BF14-2F4A-806D-337481E7235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="291">
   <si>
     <t>Card</t>
   </si>
@@ -194,9 +194,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>At the end of your turn, if you have 3 or more cards in your hand, Recall: Draw 2 cards.</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
   </si>
   <si>
     <t>Draw 1 card. Recall: Gain 1 E.</t>
-  </si>
-  <si>
-    <t>At the start of your third turn, remove all your debuffs.</t>
   </si>
   <si>
     <t>Deal 6 damage. Put a card from your discard pile into your hand.</t>
@@ -856,21 +850,9 @@
     <t>Deal 6 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
   <si>
-    <t>The first time you consume Jade each combat, gain E.</t>
-  </si>
-  <si>
-    <t>The first 3 times you consume Jade each combat, gain E.</t>
-  </si>
-  <si>
     <t>Whenever you spend E on a cost X card, a random card in your hand costs 0 this turn.</t>
   </si>
   <si>
-    <t>Remove a Jade at the end of your turn.</t>
-  </si>
-  <si>
-    <t>At the start of the battle, you can choose to place up to 4 cards into your discard pile.</t>
-  </si>
-  <si>
     <t>The first cost X card you play each combat has its effect increased by 3.</t>
   </si>
   <si>
@@ -893,6 +875,48 @@
   </si>
   <si>
     <t>Once per turn, trigger the first Recall effect twice.</t>
+  </si>
+  <si>
+    <t>Magical Herb</t>
+  </si>
+  <si>
+    <t>At the start of your first three turns, Recall: Gain E and draw 1 card.</t>
+  </si>
+  <si>
+    <t>At the start of each combat, Recall: Gain E and draw 1 card.</t>
+  </si>
+  <si>
+    <t>Broom</t>
+  </si>
+  <si>
+    <t>Scroll</t>
+  </si>
+  <si>
+    <t>Magnifying Glass</t>
+  </si>
+  <si>
+    <t>Cat's Tail</t>
+  </si>
+  <si>
+    <t>Feather Quill</t>
+  </si>
+  <si>
+    <t>Ruby Amulet</t>
+  </si>
+  <si>
+    <t>At the start of the battle, you can choose to place up to 5 cards into your discard pile.</t>
+  </si>
+  <si>
+    <t>Consume a Jade at the end of your turn.</t>
+  </si>
+  <si>
+    <t>The first time you receive unblocked Attack damage each combat, deal damage to ALL enemies equal to damage received.</t>
+  </si>
+  <si>
+    <t>Whenever you draw an Unplayable card, draw 1 card.</t>
+  </si>
+  <si>
+    <t>Refresher</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1652,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1640,7 +1664,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1652,7 +1676,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1692,10 +1716,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1707,7 +1731,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1748,31 +1772,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>116</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1909,7 +1933,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1918,13 +1942,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -1932,7 +1956,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1944,13 +1968,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1973,7 +1997,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1999,18 +2023,18 @@
         <v>48</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="D2" t="s">
         <v>49</v>
@@ -2020,63 +2044,93 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>280</v>
+      </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>282</v>
+      </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>281</v>
+      </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
       </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>285</v>
+      </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
       </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -2085,7 +2139,7 @@
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -2093,13 +2147,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
@@ -2109,36 +2163,48 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>290</v>
+      </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>283</v>
+      </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>288</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>271</v>
+      <c r="C12" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
@@ -2148,25 +2214,31 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>277</v>
+      </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="D13" t="s">
         <v>49</v>
       </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D14" t="s">
         <v>49</v>
@@ -2177,13 +2249,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
         <v>49</v>
@@ -2250,12 +2322,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2267,13 +2339,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -2284,7 +2356,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2296,13 +2368,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -2313,7 +2385,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2325,13 +2397,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -2342,7 +2414,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2354,13 +2426,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2371,7 +2443,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2383,13 +2455,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2400,7 +2472,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2412,13 +2484,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
@@ -2429,7 +2501,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2441,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2458,7 +2530,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2487,7 +2559,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2499,13 +2571,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2516,7 +2588,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2528,13 +2600,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>33</v>
@@ -2545,7 +2617,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2557,13 +2629,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -2574,7 +2646,7 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2586,13 +2658,13 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H13" t="s">
         <v>31</v>
@@ -2603,7 +2675,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2615,13 +2687,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>31</v>
@@ -2632,7 +2704,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2644,13 +2716,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -2661,7 +2733,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2673,13 +2745,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -2690,7 +2762,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2702,13 +2774,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H17" t="s">
         <v>34</v>
@@ -2719,7 +2791,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2731,13 +2803,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2748,7 +2820,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2760,13 +2832,13 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -2777,7 +2849,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2789,13 +2861,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2806,7 +2878,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -2815,16 +2887,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -2835,7 +2907,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -2844,16 +2916,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>40</v>
@@ -2864,7 +2936,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -2873,16 +2945,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -2893,7 +2965,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -2905,13 +2977,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -2922,7 +2994,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -2934,16 +3006,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -2951,7 +3023,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -2963,13 +3035,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F26" s="2">
         <v>2</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -2980,7 +3052,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2992,13 +3064,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>40</v>
@@ -3009,7 +3081,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3018,16 +3090,16 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3038,7 +3110,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3047,16 +3119,16 @@
         <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>35</v>
@@ -3126,12 +3198,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3143,13 +3215,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -3160,7 +3232,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3172,13 +3244,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -3189,7 +3261,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3201,13 +3273,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3218,7 +3290,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3230,13 +3302,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3247,7 +3319,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3259,13 +3331,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -3276,7 +3348,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3288,13 +3360,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -3305,7 +3377,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3317,13 +3389,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3334,7 +3406,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3346,13 +3418,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H9" t="s">
         <v>32</v>
@@ -3363,7 +3435,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3375,13 +3447,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3392,7 +3464,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3421,7 +3493,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3433,13 +3505,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3450,7 +3522,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3462,13 +3534,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -3479,7 +3551,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3491,13 +3563,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
         <v>34</v>
@@ -3508,7 +3580,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3517,16 +3589,16 @@
         <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -3537,7 +3609,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3549,16 +3621,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3566,7 +3638,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3578,13 +3650,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -3595,7 +3667,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3607,13 +3679,13 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -3624,7 +3696,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3636,13 +3708,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -3653,7 +3725,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3662,16 +3734,16 @@
         <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>40</v>
@@ -3682,7 +3754,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3691,16 +3763,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -3711,7 +3783,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3720,16 +3792,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3740,7 +3812,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3749,16 +3821,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
@@ -3769,7 +3841,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3778,16 +3850,16 @@
         <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
@@ -3798,7 +3870,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3810,13 +3882,13 @@
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H25" t="s">
         <v>31</v>
@@ -3827,7 +3899,7 @@
     </row>
     <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3839,16 +3911,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3856,7 +3928,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -3885,7 +3957,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -3894,19 +3966,19 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -3914,7 +3986,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3926,13 +3998,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -3943,7 +4015,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -3972,7 +4044,7 @@
     </row>
     <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -3981,16 +4053,16 @@
         <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -4001,7 +4073,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4010,16 +4082,16 @@
         <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H32" t="s">
         <v>33</v>
@@ -4041,7 +4113,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4082,12 +4154,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4099,13 +4171,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4116,7 +4188,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4128,13 +4200,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -4145,7 +4217,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4157,13 +4229,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4174,7 +4246,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4186,13 +4258,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>34</v>
@@ -4203,7 +4275,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4215,13 +4287,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4232,7 +4304,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4244,13 +4316,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -4261,7 +4333,7 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4273,13 +4345,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4290,7 +4362,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4302,13 +4374,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4319,7 +4391,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4331,13 +4403,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>31</v>
@@ -4348,7 +4420,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4377,7 +4449,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4389,13 +4461,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4406,7 +4478,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4418,7 +4490,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F13">
         <v>1</v>

</xml_diff>

<commit_message>
Add beta card art
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E5558-BF14-2F4A-806D-337481E7235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFBB2E-F305-FD40-A5E2-0C14FA0451C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -1996,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2396E-0670-B44C-B534-C216CC78A82B}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2280,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change rewinder and precognition effect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08EF1BB-6203-9742-9421-D2E03AE4D78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F0488-16B9-BF4E-B309-0A6F75E7C8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="296">
   <si>
     <t>Card</t>
   </si>
@@ -658,18 +658,9 @@
     <t>Spell Boost</t>
   </si>
   <si>
-    <t>Recurring Nightmare</t>
-  </si>
-  <si>
     <t>Recurring Dream</t>
   </si>
   <si>
-    <t>The enemy loses 10 HP at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
-    <t>The enemy loses 13 HP at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
     <t>Gain 4 Block. Gain 1 additional Block for each Jade that you have.</t>
   </si>
   <si>
@@ -700,12 +691,6 @@
     <t>Adept Spellcaster</t>
   </si>
   <si>
-    <t>Increase the effect of the next cost X card played this turn by 2.</t>
-  </si>
-  <si>
-    <t>Increase the effect of the next cost X card played this turn by 3.</t>
-  </si>
-  <si>
     <t>Whenever you spend at least 3 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
   </si>
   <si>
@@ -724,12 +709,6 @@
     <t>Whenever you receive unblocked damage, Recall the amount of damage received as Block.</t>
   </si>
   <si>
-    <t>Consume a Jade and gain 1 E. When you draw this card, increase E gained from this card by 1 this combat.</t>
-  </si>
-  <si>
-    <t>Innate. Consume a Jade and gain 1 E. When you draw this card, increase E gained from this card by 1 this combat.</t>
-  </si>
-  <si>
     <t>Require 3 E. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
   </si>
   <si>
@@ -742,10 +721,6 @@
     <t>Require: 3 E. Draw X cards. They cost 0 this turn.</t>
   </si>
   <si>
-    <t>Jade
-Manipulation</t>
-  </si>
-  <si>
     <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 10X damage.</t>
   </si>
   <si>
@@ -806,12 +781,6 @@
     <t>Deal 16 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
-    <t>Require: 2 E. Gain 10 Block and 1 Jade. Gain 10 Block X times.</t>
-  </si>
-  <si>
-    <t>Require: 2 E. Gain 8 Block and 1 Jade. Gain 8 Block X times.</t>
-  </si>
-  <si>
     <t>Retain a card. Recall: It costs 0 this turn.</t>
   </si>
   <si>
@@ -939,6 +908,30 @@
   </si>
   <si>
     <t>Ethereal. Gain 2 E and draw 2 cards. At the end of your turn, gain an extra action. Exhaust.</t>
+  </si>
+  <si>
+    <t>Increase the effect of the next cost X card played by 2.</t>
+  </si>
+  <si>
+    <t>Increase the effect of the next cost X card played by 3.</t>
+  </si>
+  <si>
+    <t>Repeat your next Recall effect 3 times. Gain 2 Jade.</t>
+  </si>
+  <si>
+    <t>Nightmare</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Consume Jade X-1 times. Exhaust.</t>
+  </si>
+  <si>
+    <t>Require: E. Consume Jade X times. Exhaust.</t>
+  </si>
+  <si>
+    <t>The enemy loses 10 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>The enemy loses 13 HP at the start of your next X turns.</t>
   </si>
 </sst>
 </file>
@@ -2105,7 +2098,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
@@ -2116,13 +2109,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -2133,13 +2126,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -2150,13 +2143,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
@@ -2167,13 +2160,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2184,13 +2177,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -2218,13 +2211,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
@@ -2235,13 +2228,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
@@ -2252,13 +2245,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
@@ -2275,7 +2268,7 @@
         <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -2286,13 +2279,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -2303,13 +2296,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
@@ -2320,13 +2313,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
@@ -2351,7 +2344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -2497,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2642,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2758,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="H14" t="s">
         <v>31</v>
@@ -2845,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>61</v>
@@ -2874,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2903,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -2932,13 +2925,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2961,13 +2954,13 @@
         <v>109</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>109</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>40</v>
@@ -2996,7 +2989,7 @@
         <v>109</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H22" t="s">
         <v>33</v>
@@ -3019,13 +3012,13 @@
         <v>109</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -3077,7 +3070,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
@@ -3094,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3106,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -3164,13 +3157,13 @@
         <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3227,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3344,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3373,13 +3366,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3448,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3460,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3518,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>218</v>
+        <v>288</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>219</v>
+        <v>289</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3582,7 +3575,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3593,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3605,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -3721,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3854,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3883,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>291</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3895,13 +3888,13 @@
         <v>109</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>206</v>
+        <v>294</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>207</v>
+        <v>295</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
@@ -3924,13 +3917,13 @@
         <v>109</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>253</v>
+        <v>293</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
@@ -3968,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -3982,16 +3975,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>226</v>
+        <v>290</v>
       </c>
       <c r="F26" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>227</v>
+        <v>290</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>232</v>
+        <v>36</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -4069,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -4127,13 +4120,13 @@
         <v>109</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>109</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -4242,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4300,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4364,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4375,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4416,13 +4409,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4445,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4532,13 +4525,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4549,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4588,8 +4581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4635,7 +4628,7 @@
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4647,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
@@ -4661,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4673,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4696,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4720,13 +4713,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Tweak card numbers and fix ArrowOfTime
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F0488-16B9-BF4E-B309-0A6F75E7C8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE5A2E-35ED-F74B-983B-7522AEE3E5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="296">
   <si>
     <t>Card</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Recall your Block. Gain 8 Block X times.</t>
   </si>
   <si>
-    <t>Recall your Block. Gain 10 Block X times.</t>
-  </si>
-  <si>
     <t>Draw 1 card. Recall: Gain 1 E.</t>
   </si>
   <si>
@@ -706,15 +703,6 @@
     <t>Inheritance</t>
   </si>
   <si>
-    <t>Whenever you receive unblocked damage, Recall the amount of damage received as Block.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
     <t>Require: 3 E. Draw X cards. They cost 0 this turn. Exhaust.</t>
   </si>
   <si>
@@ -932,6 +920,18 @@
   </si>
   <si>
     <t>The enemy loses 13 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>Recall your Block. Gain 12 Block X times.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 10 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 14 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Whenever you lose HP, Recall the amount of HP lost as Block.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>106</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,31 +1836,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>110</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="G8" s="9">
         <f>COUNTIF(Attack!D:D, "X") + COUNTIF(Skill!D:D, "X") + COUNTIF(Power!D:D, "X") + 1</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="9">
         <f>COUNTIF(Attack!D:D, "-") + COUNTIF(Skill!D:D, "-") + COUNTIF(Power!D:D, "-")</f>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2087,18 +2087,18 @@
         <v>47</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2177,13 +2177,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2386,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2432,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>194</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2548,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>33</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>31</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H14" t="s">
         <v>31</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2780,13 +2780,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,16 +2838,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2925,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>40</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H22" t="s">
         <v>33</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="F24" s="10">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,16 +3070,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3124,17 +3124,17 @@
       <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="2">
-        <v>1</v>
+      <c r="D27" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F27" s="10">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>40</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>222</v>
+        <v>293</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>35</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3366,13 +3366,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3395,13 +3395,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3482,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" t="s">
         <v>32</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3569,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
         <v>34</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,16 +3653,16 @@
         <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3685,16 +3685,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>53</v>
+        <v>292</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>40</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3856,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,16 +3914,16 @@
         <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3946,13 +3946,13 @@
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H25" t="s">
         <v>31</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,13 +3975,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>36</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,19 +4030,19 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,16 +4146,16 @@
         <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H32" t="s">
         <v>33</v>
@@ -4176,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4218,12 +4218,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>34</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4351,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4409,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4467,13 +4467,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>31</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4511,9 +4511,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4525,13 +4525,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4623,12 +4623,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4713,13 +4713,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Rebalance and tweak some numbers
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE5A2E-35ED-F74B-983B-7522AEE3E5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB1C3F9-4EA6-5949-A11F-B61000C01E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -238,9 +238,6 @@
     <t>Draw 3 cards. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Trigger all Recall effects this turn.</t>
-  </si>
-  <si>
     <t>Recall: Gain 5 Block.</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>Innate. At the end of your turn, Recall your unused E.</t>
   </si>
   <si>
-    <t>Draw 2 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Whenever you play 4 cards in a single turn, gain 1 E, 1 Jade and draw 1 card.</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
     <t>Whenever you play a card, upgrade the card for the rest of the combat.</t>
   </si>
   <si>
-    <t>At the end of your turn, you can choose to place 1 card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Deal 8 damage. When you draw this card, increase its damage by 4 this combat.</t>
   </si>
   <si>
@@ -403,535 +394,544 @@
     <t>Twilight Assault</t>
   </si>
   <si>
+    <t>Star Surge</t>
+  </si>
+  <si>
+    <t>Memento</t>
+  </si>
+  <si>
+    <t>Parallel Universe</t>
+  </si>
+  <si>
+    <t>Wormhole</t>
+  </si>
+  <si>
+    <t>Time Dilation</t>
+  </si>
+  <si>
+    <t>Temporal Paradox</t>
+  </si>
+  <si>
+    <t>Ring Singularity</t>
+  </si>
+  <si>
+    <t>Cosmic Binding</t>
+  </si>
+  <si>
+    <t>Tempered Fate</t>
+  </si>
+  <si>
+    <t>Essence Flux</t>
+  </si>
+  <si>
+    <t>Mystic Shot</t>
+  </si>
+  <si>
+    <t>Arcane Barrage</t>
+  </si>
+  <si>
+    <t>Mystic Shift</t>
+  </si>
+  <si>
+    <t>Time Bomb</t>
+  </si>
+  <si>
+    <t>Time Warp</t>
+  </si>
+  <si>
+    <t>Mystic Blast</t>
+  </si>
+  <si>
+    <t>Borrowed Time</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Surge</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>Malefice</t>
+  </si>
+  <si>
+    <t>Glimpse</t>
+  </si>
+  <si>
+    <t>Boomerang Blade</t>
+  </si>
+  <si>
+    <t>Fortune's End</t>
+  </si>
+  <si>
+    <t>Fate's Edict</t>
+  </si>
+  <si>
+    <t>False Promise</t>
+  </si>
+  <si>
+    <t>Arcane Bolt</t>
+  </si>
+  <si>
+    <t>Mystic Flare</t>
+  </si>
+  <si>
+    <t>Deja Vu</t>
+  </si>
+  <si>
+    <t>Rewinder</t>
+  </si>
+  <si>
+    <t>Split Second</t>
+  </si>
+  <si>
+    <t>Time Sink</t>
+  </si>
+  <si>
+    <t>Continuum Split</t>
+  </si>
+  <si>
+    <t>Tides of Time</t>
+  </si>
+  <si>
+    <t>Distort Reality</t>
+  </si>
+  <si>
+    <t>Precognition</t>
+  </si>
+  <si>
+    <t>Back in Time</t>
+  </si>
+  <si>
+    <t>Singularity</t>
+  </si>
+  <si>
+    <t>Event Horizon</t>
+  </si>
+  <si>
+    <t>Predestination</t>
+  </si>
+  <si>
+    <t>Butterfly Effect</t>
+  </si>
+  <si>
+    <t>Arrow of Time</t>
+  </si>
+  <si>
+    <t>Mana Ball</t>
+  </si>
+  <si>
+    <t>Mana Shield</t>
+  </si>
+  <si>
+    <t>Causality</t>
+  </si>
+  <si>
+    <t>Eternal Form</t>
+  </si>
+  <si>
+    <t>Mystic Barrier</t>
+  </si>
+  <si>
+    <t>Lucid Dream</t>
+  </si>
+  <si>
+    <t>Flashback</t>
+  </si>
+  <si>
+    <t>Flash Forward</t>
+  </si>
+  <si>
+    <t>Big Bang</t>
+  </si>
+  <si>
+    <t>Astral Banishment</t>
+  </si>
+  <si>
+    <t>Dark Matter</t>
+  </si>
+  <si>
+    <t>Accelerate</t>
+  </si>
+  <si>
+    <t>Wheel of Time</t>
+  </si>
+  <si>
+    <t>Delayed Guard</t>
+  </si>
+  <si>
+    <t>Tip of the Tongue</t>
+  </si>
+  <si>
+    <t>Flashbulb</t>
+  </si>
+  <si>
+    <t>Encode</t>
+  </si>
+  <si>
+    <t>Convergence</t>
+  </si>
+  <si>
+    <t>Astral Beam</t>
+  </si>
+  <si>
+    <t>Deal 8 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage and draw 2 cards. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 9 damage and draw 1 card. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Whenever you play a cost X card, its effects are increased by 1.</t>
+  </si>
+  <si>
+    <t>Willpower</t>
+  </si>
+  <si>
+    <t>Arcane Blessing</t>
+  </si>
+  <si>
+    <t>Deal 20X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 15X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Deal 2 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Deal 3 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Gain 14 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 10 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 13 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Goof Off</t>
+  </si>
+  <si>
+    <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Spell Boost</t>
+  </si>
+  <si>
+    <t>Recurring Dream</t>
+  </si>
+  <si>
+    <t>Gain 4 Block. Gain 1 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. Gain 2 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Gain 18 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>Gain 6 Block. Recall: Draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Gain 9 Block. Recall: Draw 2 cards.</t>
+  </si>
+  <si>
+    <t>Apply 1 Weak to ALL enemies at the end of your turn if you have triggered a Recall effect this turn.</t>
+  </si>
+  <si>
+    <t>Apply 2 Weak to ALL enemies at the end of your turn if you have triggered a Recall effect this turn.</t>
+  </si>
+  <si>
+    <t>Adept Spellcaster</t>
+  </si>
+  <si>
+    <t>Whenever you spend at least 3 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
+  </si>
+  <si>
+    <t>Whenever you consume Jade, your next Attack deals 3 additional damage.</t>
+  </si>
+  <si>
+    <t>Whenever you consume Jade, your next Attack deals 5 additional damage.</t>
+  </si>
+  <si>
+    <t>Innate. Whenever you play a card, upgrade the card for the rest of the combat.</t>
+  </si>
+  <si>
+    <t>Inheritance</t>
+  </si>
+  <si>
+    <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 10X damage.</t>
+  </si>
+  <si>
+    <t>Memorize</t>
+  </si>
+  <si>
+    <t>Prevent the next 2 times you gain Jade.</t>
+  </si>
+  <si>
+    <t>Prevent the next 3 times you gain Jade.</t>
+  </si>
+  <si>
+    <t>Recall: If any of the enemies intend to attack, gain 22 Block. Otherwise gain 2 Artifact.</t>
+  </si>
+  <si>
+    <t>Recall: If any of the enemies intend to attack, gain 28 Block. Otherwise gain 3 Artifact.</t>
+  </si>
+  <si>
+    <t>Scry 3. Draw 1 card.</t>
+  </si>
+  <si>
+    <t>Deal 9 damage. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Deal 13 damage. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Recall all your Jade.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. Recall all your Jade.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 18 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 5 damage to ALL enemies X times. If X is 3 or more, apply 1 Vulnerable and 1 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
+  </si>
+  <si>
+    <t>Deal 16 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
+  </si>
+  <si>
+    <t>Retain a card. Recall: It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Whenever you spend E on a cost X card, a random card in your hand costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>The first cost X card you play each combat has its effect increased by 3.</t>
+  </si>
+  <si>
+    <t>Whenever you play 4 cards that cost 0, draw 1 card.</t>
+  </si>
+  <si>
+    <t>Grimoire</t>
+  </si>
+  <si>
+    <t>Winder</t>
+  </si>
+  <si>
+    <t>Whenever you trigger a Recall effect, deal 2 damage to a random enemy.</t>
+  </si>
+  <si>
+    <t>Whenever you consume Jade, gain 5 Block.</t>
+  </si>
+  <si>
+    <t>Old Wine</t>
+  </si>
+  <si>
+    <t>Once per turn, trigger the first Recall effect twice.</t>
+  </si>
+  <si>
+    <t>Magical Herb</t>
+  </si>
+  <si>
+    <t>Broom</t>
+  </si>
+  <si>
+    <t>Scroll</t>
+  </si>
+  <si>
+    <t>Magnifying Glass</t>
+  </si>
+  <si>
+    <t>Cat's Tail</t>
+  </si>
+  <si>
+    <t>Feather Quill</t>
+  </si>
+  <si>
+    <t>Ruby Amulet</t>
+  </si>
+  <si>
+    <t>At the start of the battle, you can choose to place up to 5 cards into your discard pile.</t>
+  </si>
+  <si>
+    <t>Consume a Jade at the end of your turn.</t>
+  </si>
+  <si>
+    <t>The first time you receive unblocked Attack damage each combat, deal damage to ALL enemies equal to damage received.</t>
+  </si>
+  <si>
+    <t>Whenever you draw an Unplayable card, draw 1 card.</t>
+  </si>
+  <si>
+    <t>Refresher</t>
+  </si>
+  <si>
+    <t>Whenever you shuffle your draw pile, you can choose to place a card from your draw pile into your discard pile.</t>
+  </si>
+  <si>
+    <t>Whenever you shuffle your draw pile, you can choose to place up to 3 cards from your draw pile into your discard pile.</t>
+  </si>
+  <si>
+    <t>The first time you consume Jade each combat, gain 1 Strength and 1 Dexterity.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Discard the top 3 cards of your draw pile and draw a card.</t>
+  </si>
+  <si>
+    <t>Deal 13 damage. Discard the top 3 cards of your draw pile and draw a card.</t>
+  </si>
+  <si>
+    <t>Magic Chant - Spring</t>
+  </si>
+  <si>
+    <t>Deal 6 damage. Recall: Add a Magic Chant - Summer to your hand.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Recall: Add a Magic Chant - Summer+ to your hand.</t>
+  </si>
+  <si>
+    <t>Magic Chant - Summer</t>
+  </si>
+  <si>
+    <t>Magic Chant - Fall</t>
+  </si>
+  <si>
+    <t>Magic Chant - Winter</t>
+  </si>
+  <si>
+    <t>Gain 10 Block. Recall: Add a Magic Chant - Fall to your hand. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 13 Block. Recall: Add a Magic Chant - Fall+ to your hand. Exhaust.</t>
+  </si>
+  <si>
+    <t>At the start of your turn, gain E and draw 1 card. Recall: Add a Magic Chant - Winter to your hand.</t>
+  </si>
+  <si>
+    <t>Ethereal. Gain E and draw 1 card. At the end of your turn, gain an extra action. Exhaust.</t>
+  </si>
+  <si>
+    <t>Ethereal. Gain 2 E and draw 2 cards. At the end of your turn, gain an extra action. Exhaust.</t>
+  </si>
+  <si>
+    <t>Increase the effect of the next cost X card played by 2.</t>
+  </si>
+  <si>
+    <t>Increase the effect of the next cost X card played by 3.</t>
+  </si>
+  <si>
+    <t>Nightmare</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Consume Jade X-1 times. Exhaust.</t>
+  </si>
+  <si>
+    <t>Require: E. Consume Jade X times. Exhaust.</t>
+  </si>
+  <si>
+    <t>Recall your Block. Gain 12 Block X times.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 10 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 14 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Whenever you lose HP, Recall the amount of HP lost as Block.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage to ALL enemies. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage to ALL enemies. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 9 damage to a random enemy X times.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 12 damage to a random enemy X times.</t>
+  </si>
+  <si>
+    <t>Scry 5. Draw 1 card.</t>
+  </si>
+  <si>
+    <t>Draw 4 cards. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>The enemy loses 12 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>The enemy loses 16 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>Repeat your next Recall effect 3 times. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade. Ethereal.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 1 Intangible and 1 Jade. Ethereal.</t>
+  </si>
+  <si>
+    <t>At the start of your turn, draw 1 card and put a card from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
     <t>Deal 6 damage. Gain 1 E and 1 Jade.</t>
   </si>
   <si>
-    <t>Star Surge</t>
-  </si>
-  <si>
-    <t>Memento</t>
-  </si>
-  <si>
-    <t>Parallel Universe</t>
-  </si>
-  <si>
-    <t>Wormhole</t>
-  </si>
-  <si>
-    <t>Time Dilation</t>
-  </si>
-  <si>
-    <t>Temporal Paradox</t>
-  </si>
-  <si>
-    <t>Ring Singularity</t>
-  </si>
-  <si>
-    <t>Cosmic Binding</t>
-  </si>
-  <si>
-    <t>Tempered Fate</t>
-  </si>
-  <si>
-    <t>Essence Flux</t>
-  </si>
-  <si>
-    <t>Mystic Shot</t>
-  </si>
-  <si>
-    <t>Arcane Barrage</t>
-  </si>
-  <si>
-    <t>Mystic Shift</t>
-  </si>
-  <si>
-    <t>Time Bomb</t>
-  </si>
-  <si>
-    <t>Time Warp</t>
-  </si>
-  <si>
-    <t>Mystic Blast</t>
-  </si>
-  <si>
-    <t>Borrowed Time</t>
-  </si>
-  <si>
-    <t>Flux</t>
-  </si>
-  <si>
-    <t>Surge</t>
-  </si>
-  <si>
-    <t>Black Hole</t>
-  </si>
-  <si>
-    <t>Malefice</t>
-  </si>
-  <si>
-    <t>Glimpse</t>
-  </si>
-  <si>
-    <t>Boomerang Blade</t>
-  </si>
-  <si>
-    <t>Fortune's End</t>
-  </si>
-  <si>
-    <t>Fate's Edict</t>
-  </si>
-  <si>
-    <t>False Promise</t>
-  </si>
-  <si>
-    <t>Arcane Bolt</t>
-  </si>
-  <si>
-    <t>Mystic Flare</t>
-  </si>
-  <si>
-    <t>Deja Vu</t>
-  </si>
-  <si>
-    <t>Rewinder</t>
-  </si>
-  <si>
-    <t>Split Second</t>
-  </si>
-  <si>
-    <t>Time Sink</t>
-  </si>
-  <si>
-    <t>Continuum Split</t>
-  </si>
-  <si>
-    <t>Tides of Time</t>
-  </si>
-  <si>
-    <t>Distort Reality</t>
-  </si>
-  <si>
-    <t>Precognition</t>
-  </si>
-  <si>
-    <t>Back in Time</t>
-  </si>
-  <si>
-    <t>Singularity</t>
-  </si>
-  <si>
-    <t>Event Horizon</t>
-  </si>
-  <si>
-    <t>Predestination</t>
-  </si>
-  <si>
-    <t>Butterfly Effect</t>
-  </si>
-  <si>
-    <t>Arrow of Time</t>
-  </si>
-  <si>
-    <t>Mana Ball</t>
-  </si>
-  <si>
-    <t>Mana Shield</t>
-  </si>
-  <si>
-    <t>Causality</t>
-  </si>
-  <si>
-    <t>Eternal Form</t>
-  </si>
-  <si>
-    <t>Mystic Barrier</t>
-  </si>
-  <si>
-    <t>Lucid Dream</t>
-  </si>
-  <si>
-    <t>Flashback</t>
-  </si>
-  <si>
-    <t>Flash Forward</t>
-  </si>
-  <si>
-    <t>Big Bang</t>
-  </si>
-  <si>
-    <t>Astral Banishment</t>
-  </si>
-  <si>
-    <t>Dark Matter</t>
-  </si>
-  <si>
-    <t>Accelerate</t>
-  </si>
-  <si>
-    <t>Wheel of Time</t>
-  </si>
-  <si>
-    <t>Delayed Guard</t>
-  </si>
-  <si>
-    <t>Tip of the Tongue</t>
-  </si>
-  <si>
-    <t>Flashbulb</t>
-  </si>
-  <si>
-    <t>Encode</t>
-  </si>
-  <si>
-    <t>Convergence</t>
-  </si>
-  <si>
-    <t>Astral Beam</t>
-  </si>
-  <si>
-    <t>Deal 8 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage and draw 2 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 9 damage and draw 1 card. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 4 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 1 Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Whenever you play a cost X card, its effects are increased by 1.</t>
-  </si>
-  <si>
-    <t>Willpower</t>
-  </si>
-  <si>
-    <t>Arcane Blessing</t>
-  </si>
-  <si>
-    <t>Deal 20X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 15X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Deal 2 additional damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Deal 3 additional damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Gain 14 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Gain 2 Jade. Deal 10 damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Gain 2 Jade. Deal 13 damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Goof Off</t>
-  </si>
-  <si>
-    <t>Gain 1 E and 1 Jade. Put this card onto the top of your draw pile. Ethereal.</t>
-  </si>
-  <si>
-    <t>Gain 1 E and 1 Jade. Put this card onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Spell Boost</t>
-  </si>
-  <si>
-    <t>Recurring Dream</t>
-  </si>
-  <si>
-    <t>Gain 4 Block. Gain 1 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
-    <t>Gain 5 Block. Gain 2 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
-    <t>Gain 18 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Trigger all Recall effects this turn. Exhaust.</t>
-  </si>
-  <si>
-    <t>Teleport</t>
-  </si>
-  <si>
-    <t>Gain 6 Block. Recall: Draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Gain 9 Block. Recall: Draw 2 cards.</t>
-  </si>
-  <si>
-    <t>Apply 1 Weak to ALL enemies at the end of your turn if you have triggered a Recall effect this turn.</t>
-  </si>
-  <si>
-    <t>Apply 2 Weak to ALL enemies at the end of your turn if you have triggered a Recall effect this turn.</t>
-  </si>
-  <si>
-    <t>Adept Spellcaster</t>
-  </si>
-  <si>
-    <t>Whenever you spend at least 3 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
-  </si>
-  <si>
-    <t>Whenever you consume Jade, your next Attack deals 3 additional damage.</t>
-  </si>
-  <si>
-    <t>Whenever you consume Jade, your next Attack deals 5 additional damage.</t>
-  </si>
-  <si>
-    <t>Innate. Whenever you play a card, upgrade the card for the rest of the combat.</t>
-  </si>
-  <si>
-    <t>Inheritance</t>
-  </si>
-  <si>
-    <t>Require: 3 E. Draw X cards. They cost 0 this turn. Exhaust.</t>
-  </si>
-  <si>
-    <t>Require: 3 E. Draw X cards. They cost 0 this turn.</t>
-  </si>
-  <si>
-    <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 10X damage.</t>
-  </si>
-  <si>
-    <t>Memorize</t>
-  </si>
-  <si>
-    <t>Prevent the next 2 times you gain Jade.</t>
-  </si>
-  <si>
-    <t>Prevent the next 3 times you gain Jade.</t>
-  </si>
-  <si>
-    <t>Recall: If any of the enemies intend to attack, gain 22 Block. Otherwise gain 2 Artifact.</t>
-  </si>
-  <si>
-    <t>Recall: If any of the enemies intend to attack, gain 28 Block. Otherwise gain 3 Artifact.</t>
-  </si>
-  <si>
-    <t>Scry 3. Draw 1 card.</t>
-  </si>
-  <si>
-    <t>Scry 2. Draw 1 card.</t>
-  </si>
-  <si>
-    <t>Deal 9 damage. Trigger all Recall effects this turn.</t>
-  </si>
-  <si>
-    <t>Deal 13 damage. Trigger all Recall effects this turn.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Recall all your Jade.</t>
-  </si>
-  <si>
-    <t>Deal 11 damage. Recall all your Jade.</t>
-  </si>
-  <si>
-    <t>Deal 14 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
-    <t>Deal 18 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
-    <t>Deal 5 damage to ALL enemies X times. If X is 3 or more, apply 1 Vulnerable and 1 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Recall: Deal 10 damage to a random enemy X times.</t>
-  </si>
-  <si>
-    <t>Recall: Deal 13 damage to a random enemy X times.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
-  </si>
-  <si>
-    <t>Deal 16 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
-  </si>
-  <si>
-    <t>Retain a card. Recall: It costs 0 this turn.</t>
-  </si>
-  <si>
-    <t>Deal 6 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Whenever you spend E on a cost X card, a random card in your hand costs 0 this turn.</t>
-  </si>
-  <si>
-    <t>The first cost X card you play each combat has its effect increased by 3.</t>
-  </si>
-  <si>
-    <t>Whenever you play 4 cards that cost 0, draw 1 card.</t>
-  </si>
-  <si>
-    <t>Grimoire</t>
-  </si>
-  <si>
-    <t>Winder</t>
-  </si>
-  <si>
-    <t>Whenever you trigger a Recall effect, deal 2 damage to a random enemy.</t>
-  </si>
-  <si>
-    <t>Whenever you consume Jade, gain 5 Block.</t>
-  </si>
-  <si>
-    <t>Old Wine</t>
-  </si>
-  <si>
-    <t>Once per turn, trigger the first Recall effect twice.</t>
-  </si>
-  <si>
-    <t>Magical Herb</t>
-  </si>
-  <si>
-    <t>Broom</t>
-  </si>
-  <si>
-    <t>Scroll</t>
-  </si>
-  <si>
-    <t>Magnifying Glass</t>
-  </si>
-  <si>
-    <t>Cat's Tail</t>
-  </si>
-  <si>
-    <t>Feather Quill</t>
-  </si>
-  <si>
-    <t>Ruby Amulet</t>
-  </si>
-  <si>
-    <t>At the start of the battle, you can choose to place up to 5 cards into your discard pile.</t>
-  </si>
-  <si>
-    <t>Consume a Jade at the end of your turn.</t>
-  </si>
-  <si>
-    <t>The first time you receive unblocked Attack damage each combat, deal damage to ALL enemies equal to damage received.</t>
-  </si>
-  <si>
-    <t>Whenever you draw an Unplayable card, draw 1 card.</t>
-  </si>
-  <si>
-    <t>Refresher</t>
-  </si>
-  <si>
-    <t>Whenever you shuffle your draw pile, you can choose to place a card from your draw pile into your discard pile.</t>
-  </si>
-  <si>
-    <t>Whenever you shuffle your draw pile, you can choose to place up to 3 cards from your draw pile into your discard pile.</t>
-  </si>
-  <si>
-    <t>The first time you consume Jade each combat, gain 1 Strength and 1 Dexterity.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Discard the top 3 cards of your draw pile and draw a card.</t>
-  </si>
-  <si>
-    <t>Deal 13 damage. Discard the top 3 cards of your draw pile and draw a card.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Gain 1 Jade. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage. Gain 1 Jade. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
-  </si>
-  <si>
-    <t>Magic Chant - Spring</t>
-  </si>
-  <si>
-    <t>Deal 6 damage. Recall: Add a Magic Chant - Summer to your hand.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Recall: Add a Magic Chant - Summer+ to your hand.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage to ALL enemies. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 16 damage to ALL enemies. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Magic Chant - Summer</t>
-  </si>
-  <si>
-    <t>Magic Chant - Fall</t>
-  </si>
-  <si>
-    <t>Magic Chant - Winter</t>
-  </si>
-  <si>
-    <t>Gain 10 Block. Recall: Add a Magic Chant - Fall to your hand. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 13 Block. Recall: Add a Magic Chant - Fall+ to your hand. Exhaust.</t>
-  </si>
-  <si>
-    <t>At the start of your turn, gain E and draw 1 card. Recall: Add a Magic Chant - Winter to your hand.</t>
-  </si>
-  <si>
-    <t>Ethereal. Gain E and draw 1 card. At the end of your turn, gain an extra action. Exhaust.</t>
-  </si>
-  <si>
-    <t>Ethereal. Gain 2 E and draw 2 cards. At the end of your turn, gain an extra action. Exhaust.</t>
-  </si>
-  <si>
-    <t>Increase the effect of the next cost X card played by 2.</t>
-  </si>
-  <si>
-    <t>Increase the effect of the next cost X card played by 3.</t>
-  </si>
-  <si>
-    <t>Repeat your next Recall effect 3 times. Gain 2 Jade.</t>
-  </si>
-  <si>
-    <t>Nightmare</t>
-  </si>
-  <si>
-    <t>Require: 2 E. Consume Jade X-1 times. Exhaust.</t>
-  </si>
-  <si>
-    <t>Require: E. Consume Jade X times. Exhaust.</t>
-  </si>
-  <si>
-    <t>The enemy loses 10 HP at the start of your next X turns.</t>
-  </si>
-  <si>
-    <t>The enemy loses 13 HP at the start of your next X turns.</t>
-  </si>
-  <si>
-    <t>Recall your Block. Gain 12 Block X times.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 10 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 14 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Whenever you lose HP, Recall the amount of HP lost as Block.</t>
+    <t>Deal 9 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. Gain 1 E and 1 Jade. Place this card onto the top of your drawpile. Ethereal.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. Gain 1 E and 1 Jade. Place this card onto the top of your drawpile.</t>
+  </si>
+  <si>
+    <t>Discard your draw pile. Trigger all Recall effects this turn. Exhaust.</t>
+  </si>
+  <si>
+    <t>Discard your draw pile. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Require: 3 E. Shuffle ALL your cards into your draw pile. Draw X cards. They cost 0 this turn.</t>
+  </si>
+  <si>
+    <t>Require: 3 E. Shuffle ALL your cards into your draw pile. Draw X+1 cards. They cost 0 this turn.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,42 +1836,42 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>109</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -2087,18 +2087,18 @@
         <v>47</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="D2" t="s">
         <v>48</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D4" t="s">
         <v>49</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2177,13 +2177,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="D14" t="s">
         <v>48</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2386,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>184</v>
+        <v>288</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>119</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2432,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>200</v>
+        <v>273</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>33</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>31</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2780,13 +2780,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>60</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="H18" t="s">
         <v>32</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2925,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>237</v>
+        <v>278</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>238</v>
+        <v>279</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>40</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="H22" t="s">
         <v>33</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>35</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F24" s="10">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,13 +3070,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>60</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3125,16 @@
         <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>40</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>35</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>281</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>198</v>
+        <v>290</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>199</v>
+        <v>291</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3363,16 +3363,16 @@
         <v>37</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="F5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3482,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
         <v>32</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3569,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F12" s="10">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
         <v>34</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,16 +3653,16 @@
         <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3685,13 +3685,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>60</v>
@@ -3700,9 +3700,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>207</v>
+        <v>292</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>64</v>
+        <v>293</v>
       </c>
       <c r="H17" t="s">
         <v>32</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>40</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3856,16 @@
         <v>39</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>39</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="H23" t="s">
         <v>33</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,16 +3914,16 @@
         <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>35</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,13 +3975,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>36</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,16 +4030,16 @@
         <v>38</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>186</v>
+        <v>285</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>185</v>
+        <v>286</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>60</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="H29" t="s">
         <v>32</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4106,9 +4106,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>38</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>219</v>
+        <v>294</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>33</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,13 +4146,13 @@
         <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>59</v>
@@ -4176,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4218,12 +4218,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>77</v>
+        <v>287</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>77</v>
+        <v>287</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>34</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4351,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>34</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4409,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4467,13 +4467,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>31</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4525,13 +4525,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4623,12 +4623,12 @@
         <v>30</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4713,13 +4713,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Buff Jade cards number
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB1C3F9-4EA6-5949-A11F-B61000C01E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4229934-6F69-CE44-90CF-0EF5EBEC1F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Power" sheetId="7" r:id="rId6"/>
     <sheet name="Colorless" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,9 +105,6 @@
     <t>Deal 8 damage. Recall: Deal 8 damage.</t>
   </si>
   <si>
-    <t>Deal 8X damage. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 12X damage. Gain 1 Jade.</t>
   </si>
   <si>
@@ -213,12 +210,6 @@
     <t>Deal 4 damage. Put a random card from your discard pile into your hand.</t>
   </si>
   <si>
-    <t>Double your Jade. Gain E equal to your Jade and draw 3 cards. Exhaust.</t>
-  </si>
-  <si>
-    <t>Double your Jade. Gain E equal to your Jade and draw 5 cards. Exhaust.</t>
-  </si>
-  <si>
     <t>Your next Attack deals 6X additional damage.</t>
   </si>
   <si>
@@ -238,12 +229,6 @@
     <t>Draw 3 cards. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Recall: Gain 5 Block.</t>
-  </si>
-  <si>
-    <t>Recall: Gain 8 Block.</t>
-  </si>
-  <si>
     <t>Unplayable. When you draw this card, gain 1 E.</t>
   </si>
   <si>
@@ -337,9 +322,6 @@
     <t>Recall: Deal 7 damage twice X times.</t>
   </si>
   <si>
-    <t>If the enemy intends to attack, gain 7X Block. Otherwise, deal 8X damage.</t>
-  </si>
-  <si>
     <t>Recall: Gain 1 E.</t>
   </si>
   <si>
@@ -580,12 +562,6 @@
     <t>Deal 8 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 12 damage and draw 2 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 9 damage and draw 1 card. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Whenever you play a cost X card, its effects are increased by 1.</t>
   </si>
   <si>
@@ -595,21 +571,6 @@
     <t>Arcane Blessing</t>
   </si>
   <si>
-    <t>Deal 20X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 15X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Deal 2 additional damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Deal 3 additional damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Gain 14 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Gain 2 Jade. Deal 10 damage for each Jade you have.</t>
   </si>
   <si>
@@ -628,15 +589,6 @@
     <t>Recurring Dream</t>
   </si>
   <si>
-    <t>Gain 4 Block. Gain 1 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
-    <t>Gain 5 Block. Gain 2 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
-    <t>Gain 18 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Teleport</t>
   </si>
   <si>
@@ -670,9 +622,6 @@
     <t>Inheritance</t>
   </si>
   <si>
-    <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 10X damage.</t>
-  </si>
-  <si>
     <t>Memorize</t>
   </si>
   <si>
@@ -709,12 +658,6 @@
     <t>Deal 18 damage. Recall: Gain 2 E.</t>
   </si>
   <si>
-    <t>Deal 5 damage to ALL enemies X times. If X is 3 or more, apply 1 Vulnerable and 1 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 12 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
@@ -853,9 +796,6 @@
     <t>Require: E. Consume Jade X times. Exhaust.</t>
   </si>
   <si>
-    <t>Recall your Block. Gain 12 Block X times.</t>
-  </si>
-  <si>
     <t>Require 3 E. Deal 10 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
   </si>
   <si>
@@ -868,12 +808,6 @@
     <t>Deal 11 damage. Place this card onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Deal 10 damage to ALL enemies. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 14 damage to ALL enemies. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 7 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
   </si>
   <si>
@@ -901,21 +835,9 @@
     <t>Repeat your next Recall effect 3 times. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade. Ethereal.</t>
-  </si>
-  <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 1 Jade. Ethereal.</t>
-  </si>
-  <si>
     <t>At the start of your turn, draw 1 card and put a card from your hand onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Deal 6 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 9 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
     <t>Gain 5 Block. Gain 1 E and 1 Jade. Place this card onto the top of your drawpile. Ethereal.</t>
   </si>
   <si>
@@ -932,6 +854,84 @@
   </si>
   <si>
     <t>Require: 3 E. Shuffle ALL your cards into your draw pile. Draw X+1 cards. They cost 0 this turn.</t>
+  </si>
+  <si>
+    <t>If the enemy intends to attack, gain 7X Block. Otherwise, deal 7X damage.</t>
+  </si>
+  <si>
+    <t>If the enemy intends to attack, gain 10X Block. Otherwise, deal 10X damage.</t>
+  </si>
+  <si>
+    <t>Deal 9X damage. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Recall your Block. Gain 11 Block X times.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 1 Intangible and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Deal 5 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Deal 3 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Deal 15 damage and draw 2 cards. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage and draw 1 card. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage to ALL enemies. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 16 damage to ALL enemies. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 5 damage to ALL enemies X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 3 Vulnerable and 3 Weak to ALL enemies and gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 18X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 24X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 7 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 4 Block. Gain 2 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Gain 6 Block. Gain 3 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Recall: Gain 6 Block.</t>
+  </si>
+  <si>
+    <t>Recall: Gain 9 Block.</t>
+  </si>
+  <si>
+    <t>Gain 12 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 16 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn. Exhaust.</t>
+  </si>
+  <si>
+    <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,42 +1836,42 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>109</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1913,7 +1913,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,21 +2006,21 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2075,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -2084,24 +2084,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2109,16 +2109,16 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -2126,16 +2126,16 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2143,16 +2143,16 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2194,16 +2194,16 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -2211,16 +2211,16 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2228,16 +2228,16 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -2245,16 +2245,16 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -2262,16 +2262,16 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -2279,16 +2279,16 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -2296,16 +2296,16 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -2313,16 +2313,16 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -2383,36 +2383,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -2420,28 +2420,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -2449,28 +2449,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>185</v>
+        <v>277</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -2478,28 +2478,28 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -2507,28 +2507,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -2536,28 +2536,28 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -2565,19 +2565,19 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2586,7 +2586,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -2594,28 +2594,28 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -2623,28 +2623,28 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -2652,28 +2652,28 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -2681,28 +2681,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>179</v>
+        <v>279</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>178</v>
+        <v>278</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -2710,28 +2710,28 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -2739,28 +2739,28 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -2768,28 +2768,28 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -2797,28 +2797,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -2826,28 +2826,28 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -2855,28 +2855,28 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -2884,28 +2884,28 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -2913,28 +2913,28 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -2942,28 +2942,28 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>1</v>
@@ -2971,28 +2971,28 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>97</v>
+        <v>270</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>208</v>
+        <v>271</v>
       </c>
       <c r="H22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -3000,28 +3000,28 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>221</v>
+        <v>282</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -3029,28 +3029,28 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F24" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -3058,28 +3058,28 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3087,28 +3087,28 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="H26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3116,28 +3116,28 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -3145,28 +3145,28 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="H28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -3174,28 +3174,28 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>184</v>
+        <v>284</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>183</v>
+        <v>285</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3259,36 +3259,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3296,28 +3296,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -3325,28 +3325,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>194</v>
+        <v>288</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>195</v>
+        <v>289</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -3354,28 +3354,28 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -3383,28 +3383,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -3412,28 +3412,28 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>290</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>65</v>
+        <v>291</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3441,28 +3441,28 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -3470,28 +3470,28 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -3499,28 +3499,28 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -3528,28 +3528,28 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -3557,28 +3557,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>187</v>
+        <v>292</v>
       </c>
       <c r="F12" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>196</v>
+        <v>293</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -3586,28 +3586,28 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -3615,28 +3615,28 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -3644,28 +3644,28 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -3673,28 +3673,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3702,28 +3702,28 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -3731,28 +3731,28 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -3760,28 +3760,28 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -3789,28 +3789,28 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -3818,28 +3818,28 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -3847,28 +3847,28 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -3876,28 +3876,28 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="H23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -3905,57 +3905,57 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>294</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>57</v>
+        <v>295</v>
       </c>
       <c r="H25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3963,28 +3963,28 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3992,28 +3992,28 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -4021,28 +4021,28 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4050,28 +4050,28 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="H29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -4079,28 +4079,28 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="10">
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -4108,28 +4108,28 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -4137,28 +4137,28 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -4176,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4215,36 +4215,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -4252,28 +4252,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -4281,28 +4281,28 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -4310,28 +4310,28 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -4339,28 +4339,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -4368,28 +4368,28 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -4397,28 +4397,28 @@
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -4426,28 +4426,28 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -4455,28 +4455,28 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -4484,28 +4484,28 @@
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -4513,28 +4513,28 @@
     </row>
     <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -4542,28 +4542,28 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -4620,106 +4620,106 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change Goggles relic effect and tweak numbers on some cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4229934-6F69-CE44-90CF-0EF5EBEC1F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF24A8B-F1C1-B342-A20A-D587B40452A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>Starting</t>
   </si>
   <si>
-    <t>The first card you play each combat costs 0.</t>
-  </si>
-  <si>
     <t>Exclusive</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>Innate. Whenever you play 4 cards in a single turn, gain 1 E, 1 Jade and draw 1 card.</t>
   </si>
   <si>
-    <t>Prevent the next time you lose HP. Gain 1 Jade when this effect triggers.</t>
-  </si>
-  <si>
     <t>Whenever you play a card, upgrade the card for the rest of the combat.</t>
   </si>
   <si>
@@ -307,12 +301,6 @@
     <t>Gain 7 Block. When you draw this card, increase its Block by 3 this combat.</t>
   </si>
   <si>
-    <t>Gain 8 Block. Recall: Gain 8 Block.</t>
-  </si>
-  <si>
-    <t>Gain 12 Block. Recall: Gain 12 Block.</t>
-  </si>
-  <si>
     <t>Gain 1 E and draw 1 card at the start of your next X turns.</t>
   </si>
   <si>
@@ -598,12 +586,6 @@
     <t>Gain 9 Block. Recall: Draw 2 cards.</t>
   </si>
   <si>
-    <t>Apply 1 Weak to ALL enemies at the end of your turn if you have triggered a Recall effect this turn.</t>
-  </si>
-  <si>
-    <t>Apply 2 Weak to ALL enemies at the end of your turn if you have triggered a Recall effect this turn.</t>
-  </si>
-  <si>
     <t>Adept Spellcaster</t>
   </si>
   <si>
@@ -802,9 +784,6 @@
     <t>Require 3 E. Deal 14 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
   </si>
   <si>
-    <t>Whenever you lose HP, Recall the amount of HP lost as Block.</t>
-  </si>
-  <si>
     <t>Deal 11 damage. Place this card onto the top of your draw pile.</t>
   </si>
   <si>
@@ -931,7 +910,28 @@
     <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn. Exhaust.</t>
   </si>
   <si>
-    <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn.</t>
+    <t>Repeat your next Recall effect 2 times. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Whenever you receive unblocked Attack damage, Recall the amount of damage received as Block.</t>
+  </si>
+  <si>
+    <t>The next time you would lose HP, reduce it to 1. Gain 1 Jade when this effect triggers.</t>
+  </si>
+  <si>
+    <t>The first time you trigger a Recall effect each turn, apply 1 Weak to ALL enemies.</t>
+  </si>
+  <si>
+    <t>The first time you trigger a Recall effect each turn, apply 2 Weak to ALL enemies.</t>
+  </si>
+  <si>
+    <t>Gain E equals to the cost of the first card you play each combat.</t>
+  </si>
+  <si>
+    <t>Gain 10 Block. Recall: Gain 10 Block.</t>
+  </si>
+  <si>
+    <t>Gain 14 Block. Recall: Gain 14 Block.</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1377,8 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:I13" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:I13" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
-    <sortCondition ref="C1:C13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I13">
+    <sortCondition ref="C2:C13"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4ED489C4-F350-1D4A-86C7-32EE92042A1C}" name="Card"/>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,31 +1836,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2061,7 +2061,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2084,24 +2084,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2109,16 +2109,16 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -2126,16 +2126,16 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2143,16 +2143,16 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2194,16 +2194,16 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -2211,16 +2211,16 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2228,16 +2228,16 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -2245,16 +2245,16 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -2262,16 +2262,16 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -2279,16 +2279,16 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -2296,16 +2296,16 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -2313,16 +2313,16 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -2344,7 +2344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2386,12 +2386,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2432,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2548,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>30</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2780,13 +2780,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2925,13 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F20" s="10">
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>35</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,16 +3070,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3125,16 @@
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3366,13 +3366,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3395,13 +3395,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3482,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,16 +3653,16 @@
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3685,16 +3685,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3743,13 +3743,13 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>87</v>
+        <v>294</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>88</v>
+        <v>295</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3856,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,16 +3914,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>34</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3943,16 +3943,16 @@
         <v>37</v>
       </c>
       <c r="D25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3972,16 +3972,16 @@
         <v>37</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,19 +4030,19 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,16 +4146,16 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="H32" t="s">
         <v>32</v>
@@ -4176,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4218,12 +4218,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>290</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>68</v>
+        <v>290</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4351,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="2">
+        <v>291</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>65</v>
+        <v>292</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4395,9 +4395,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4406,27 +4406,27 @@
         <v>38</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,16 +4438,16 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9">
+        <v>289</v>
+      </c>
+      <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
+        <v>289</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4464,27 +4464,27 @@
         <v>37</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
+        <v>63</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4493,27 +4493,27 @@
         <v>37</v>
       </c>
       <c r="D11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
+        <v>66</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4522,19 +4522,19 @@
         <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4623,12 +4623,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4713,13 +4713,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add Repeat keyword, balance change and change predestination effect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF24A8B-F1C1-B342-A20A-D587B40452A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BD0891-884E-6143-94C8-4EAB08754D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -189,9 +189,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Gain 1 E and draw 1 card at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
     <t>Gain 1 Blur. Recall: Deal damage to ALL enemies equal to your Block.</t>
   </si>
   <si>
@@ -253,12 +250,6 @@
     <t>Deal 8 damage. When you draw this card, increase its damage by 4 this combat.</t>
   </si>
   <si>
-    <t>Gain 5 Block. When you draw this card, increase its Block by 2 this combat.</t>
-  </si>
-  <si>
-    <t>Deal 6 damage. When you draw this card, increase its damage by 3 this combat.</t>
-  </si>
-  <si>
     <t>Deal 4 damage. Increase this card's cost by 1 and double its damage this combat.</t>
   </si>
   <si>
@@ -301,7 +292,7 @@
     <t>Gain 7 Block. When you draw this card, increase its Block by 3 this combat.</t>
   </si>
   <si>
-    <t>Gain 1 E and draw 1 card at the start of your next X turns.</t>
+    <t>Gain 12 Block. Recall: Gain 12 Block.</t>
   </si>
   <si>
     <t>Recall: Deal 5 damage twice X times.</t>
@@ -568,9 +559,6 @@
     <t>Goof Off</t>
   </si>
   <si>
-    <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Spell Boost</t>
   </si>
   <si>
@@ -619,27 +607,12 @@
     <t>Recall: If any of the enemies intend to attack, gain 28 Block. Otherwise gain 3 Artifact.</t>
   </si>
   <si>
-    <t>Scry 3. Draw 1 card.</t>
-  </si>
-  <si>
     <t>Deal 9 damage. Trigger all Recall effects this turn.</t>
   </si>
   <si>
     <t>Deal 13 damage. Trigger all Recall effects this turn.</t>
   </si>
   <si>
-    <t>Deal 8 damage. Recall all your Jade.</t>
-  </si>
-  <si>
-    <t>Deal 11 damage. Recall all your Jade.</t>
-  </si>
-  <si>
-    <t>Deal 14 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
-    <t>Deal 18 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
     <t>Deal 12 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
   </si>
   <si>
@@ -772,21 +745,6 @@
     <t>Nightmare</t>
   </si>
   <si>
-    <t>Require: 2 E. Consume Jade X-1 times. Exhaust.</t>
-  </si>
-  <si>
-    <t>Require: E. Consume Jade X times. Exhaust.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 10 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 14 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Deal 11 damage. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Deal 7 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
   </si>
   <si>
@@ -799,9 +757,6 @@
     <t>Recall: Deal 12 damage to a random enemy X times.</t>
   </si>
   <si>
-    <t>Scry 5. Draw 1 card.</t>
-  </si>
-  <si>
     <t>Draw 4 cards. Gain 1 Jade.</t>
   </si>
   <si>
@@ -928,10 +883,55 @@
     <t>Gain E equals to the cost of the first card you play each combat.</t>
   </si>
   <si>
-    <t>Gain 10 Block. Recall: Gain 10 Block.</t>
-  </si>
-  <si>
-    <t>Gain 14 Block. Recall: Gain 14 Block.</t>
+    <t>Deal 12 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 16 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. When you draw this card, increase its damage by 6 this combat.</t>
+  </si>
+  <si>
+    <t>Gain 7 Block. When you draw this card, increase its Block by 5 this combat.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Scry 3. Draw 1 card. Exhaust.</t>
+  </si>
+  <si>
+    <t>Scry 5. Draw 1 card. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 9 Block. Recall: Gain 9 Block.</t>
+  </si>
+  <si>
+    <t>Gain 2 E and draw 1 card at the start of your next X turns. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 2 E and draw 1 card at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage. Repeat your next Recall effect.</t>
+  </si>
+  <si>
+    <t>Deal 18 damage. Repeat your next Recall effect.</t>
+  </si>
+  <si>
+    <t>Deal 15 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 20 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Add X random cards into your hand. They cost 0 this turn. Gain 2 Jade.</t>
+  </si>
+  <si>
+    <t>Require: 2 E. Add X random upgraded cards into your hand. They cost 0 this turn. Gain 2 Jade.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,42 +1836,42 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>96</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2087,18 +2087,18 @@
         <v>45</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D4" t="s">
         <v>47</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -2177,13 +2177,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -2194,13 +2194,13 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2386,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2432,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>174</v>
+        <v>280</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2548,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>196</v>
+        <v>292</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>197</v>
+        <v>293</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>30</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2780,13 +2780,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>68</v>
+        <v>281</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2922,19 +2922,19 @@
         <v>38</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>194</v>
+        <v>290</v>
       </c>
       <c r="F20" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>195</v>
+        <v>291</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,16 +3070,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3125,16 @@
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>245</v>
+        <v>284</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3363,16 +3363,16 @@
         <v>36</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>191</v>
+        <v>285</v>
       </c>
       <c r="F5" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>251</v>
+        <v>286</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3395,13 +3395,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3482,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>84</v>
+        <v>282</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,16 +3653,16 @@
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3685,16 +3685,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3740,16 +3740,16 @@
         <v>38</v>
       </c>
       <c r="D18" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>295</v>
+        <v>82</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>288</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>85</v>
+        <v>289</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3856,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>32</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3903,9 +3903,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,19 +3914,19 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>243</v>
+        <v>295</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3946,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,13 +3975,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,19 +4030,19 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,16 +4146,16 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="H32" t="s">
         <v>32</v>
@@ -4218,12 +4218,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4351,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4409,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4467,13 +4467,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4496,13 +4496,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>30</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4623,12 +4623,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4713,13 +4713,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change precognition and predestination effect, and googles relic effect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BD0891-884E-6143-94C8-4EAB08754D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6F4297-13C2-7F41-905A-A3BDE64CFEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change precognition and recurring dream effect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6F4297-13C2-7F41-905A-A3BDE64CFEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0826D3D-AFAA-9D40-B50C-082D02B3455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Power" sheetId="7" r:id="rId6"/>
     <sheet name="Colorless" sheetId="10" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -280,12 +280,6 @@
     <t>Deal 18 damage. It costs 0 if you have used at least 2 E on a X cost card this turn.</t>
   </si>
   <si>
-    <t>Gain 10 Block at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 13 Block at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
     <t>Deal 6 damage. Recall: Deal 6 damage.</t>
   </si>
   <si>
@@ -784,12 +778,6 @@
     <t>Discard your draw pile. Trigger all Recall effects this turn.</t>
   </si>
   <si>
-    <t>Require: 3 E. Shuffle ALL your cards into your draw pile. Draw X cards. They cost 0 this turn.</t>
-  </si>
-  <si>
-    <t>Require: 3 E. Shuffle ALL your cards into your draw pile. Draw X+1 cards. They cost 0 this turn.</t>
-  </si>
-  <si>
     <t>If the enemy intends to attack, gain 7X Block. Otherwise, deal 7X damage.</t>
   </si>
   <si>
@@ -928,10 +916,22 @@
     <t>Deal 20 damage. Recall: Gain 2 E.</t>
   </si>
   <si>
-    <t>Require: 2 E. Add X random cards into your hand. They cost 0 this turn. Gain 2 Jade.</t>
-  </si>
-  <si>
-    <t>Require: 2 E. Add X random upgraded cards into your hand. They cost 0 this turn. Gain 2 Jade.</t>
+    <t>Shuffle X random cost X cards into your draw pile. They are free to play once. Exhaust.</t>
+  </si>
+  <si>
+    <t>Shuffle X random upgraded cost X cards into your draw pile. They are free to play once. Exhaust.</t>
+  </si>
+  <si>
+    <t>Shuffle ALL your cards into your draw pile. Draw X cards. They are free to play once.</t>
+  </si>
+  <si>
+    <t>Shuffle ALL your cards into your draw pile. Draw X cards. They are free to play once. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 10 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 14 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,31 +1836,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -2087,18 +2087,18 @@
         <v>45</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
         <v>47</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -2177,13 +2177,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -2194,13 +2194,13 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -2386,12 +2386,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2815,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2925,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,13 +3070,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>55</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3125,16 @@
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3366,13 +3366,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,13 +3653,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>60</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,19 +3856,19 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
+        <v>294</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>79</v>
+        <v>295</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,16 +3914,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3946,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,13 +3975,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,16 +4030,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>55</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>246</v>
+        <v>293</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,13 +4146,13 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>54</v>
@@ -4218,12 +4218,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4409,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4623,12 +4623,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4713,13 +4713,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Swap precognition and predestination effect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0826D3D-AFAA-9D40-B50C-082D02B3455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D657CA55-0969-0C40-A495-9FC41D902BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -922,16 +922,16 @@
     <t>Shuffle X random upgraded cost X cards into your draw pile. They are free to play once. Exhaust.</t>
   </si>
   <si>
-    <t>Shuffle ALL your cards into your draw pile. Draw X cards. They are free to play once.</t>
-  </si>
-  <si>
-    <t>Shuffle ALL your cards into your draw pile. Draw X cards. They are free to play once. Exhaust.</t>
-  </si>
-  <si>
     <t>Gain 10 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
   </si>
   <si>
     <t>Gain 14 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Draw X cards. They are free to play once. Exhaust.</t>
+  </si>
+  <si>
+    <t>Draw X cards. They are free to play once.</t>
   </si>
 </sst>
 </file>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3859,13 +3859,13 @@
         <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>90</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3903,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3917,13 +3917,13 @@
         <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>90</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -4120,13 +4120,13 @@
         <v>90</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>90</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Remove all recall power priority
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70607CEF-C600-3A4C-8B47-1EA8C06BB012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EAF110-13B4-7945-B538-3040C039F4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -715,15 +715,6 @@
     <t>Gain 13 Block. Recall: Add a Magic Chant - Fall+ to your hand. Exhaust.</t>
   </si>
   <si>
-    <t>At the start of your turn, gain E and draw 1 card. Recall: Add a Magic Chant - Winter to your hand.</t>
-  </si>
-  <si>
-    <t>Ethereal. Gain E and draw 1 card. At the end of your turn, gain an extra action. Exhaust.</t>
-  </si>
-  <si>
-    <t>Ethereal. Gain 2 E and draw 2 cards. At the end of your turn, gain an extra action. Exhaust.</t>
-  </si>
-  <si>
     <t>Increase the effect of the next cost X card played by 2.</t>
   </si>
   <si>
@@ -784,15 +775,6 @@
     <t>Recall your Block. Gain 11 Block X times.</t>
   </si>
   <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 2 Jade.</t>
-  </si>
-  <si>
-    <t>Unplayable. When you draw this card, gain 1 Intangible and 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. Deal 5 additional damage for each Jade you have.</t>
-  </si>
-  <si>
     <t>Deal 8 damage. Deal 3 additional damage for each Jade you have.</t>
   </si>
   <si>
@@ -829,9 +811,6 @@
     <t>Gain 4 Block. Gain 2 additional Block for each Jade that you have.</t>
   </si>
   <si>
-    <t>Gain 6 Block. Gain 3 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
     <t>Recall: Gain 6 Block.</t>
   </si>
   <si>
@@ -922,16 +901,37 @@
     <t>Gain 14 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
   </si>
   <si>
-    <t>Draw X cards. They are free to play once. Exhaust.</t>
-  </si>
-  <si>
-    <t>Draw X cards. They are free to play once.</t>
-  </si>
-  <si>
     <t>Recall: Gain 1 E and draw 1 card.</t>
   </si>
   <si>
     <t>Draw 1 card. Recall: Gain 1 E and draw 1 card.</t>
+  </si>
+  <si>
+    <t>Ethereal. Unplayable. When you draw this card, gain 1 Intangible and 2 Jade.</t>
+  </si>
+  <si>
+    <t>Ethereal. Unplayable. When you draw this card, gain 1 Intangible and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Draw X cards. They cost 0 this turn. Exhaust.</t>
+  </si>
+  <si>
+    <t>Draw X cards. They cost 0 this turn.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. Gain 3 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Deal 4 additional damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter to your hand.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter+ to your hand.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, gain an extra action. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1912,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DEF958-860E-CA46-81B7-63BF564B50D2}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,7 +2009,7 @@
         <v>88</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>88</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2200,7 +2200,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>248</v>
+        <v>292</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2815,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2925,13 +2925,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2954,13 +2954,13 @@
         <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2983,13 +2983,13 @@
         <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3012,13 +3012,13 @@
         <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3157,13 +3157,13 @@
         <v>88</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3186,13 +3186,13 @@
         <v>88</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3366,13 +3366,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3569,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3633,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3772,7 +3772,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
@@ -3807,7 +3807,7 @@
         <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3830,13 +3830,13 @@
         <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3859,13 +3859,13 @@
         <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3888,13 +3888,13 @@
         <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3903,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -3917,13 +3917,13 @@
         <v>88</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3946,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3975,13 +3975,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -4033,13 +4033,13 @@
         <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>246</v>
+        <v>287</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>89</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>54</v>
@@ -4120,13 +4120,13 @@
         <v>88</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4581,8 +4581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4689,13 +4689,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>293</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>223</v>
+        <v>294</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -4710,16 +4710,16 @@
         <v>37</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>224</v>
+        <v>295</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>225</v>
+        <v>295</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Fix jade to consume E after E gain from Recall
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EAF110-13B4-7945-B538-3040C039F4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D50654D-C249-C54B-ADD0-D268EE946BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -739,12 +739,6 @@
     <t>Draw 4 cards. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>The enemy loses 12 HP at the start of your next X turns.</t>
-  </si>
-  <si>
-    <t>The enemy loses 16 HP at the start of your next X turns.</t>
-  </si>
-  <si>
     <t>Repeat your next Recall effect 3 times. Gain 1 Jade.</t>
   </si>
   <si>
@@ -895,10 +889,10 @@
     <t>Shuffle X random upgraded cost X cards into your draw pile. They are free to play once. Exhaust.</t>
   </si>
   <si>
-    <t>Gain 10 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 14 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
+    <t>Gain 11 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 15 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
   </si>
   <si>
     <t>Recall: Gain 1 E and draw 1 card.</t>
@@ -932,6 +926,12 @@
   </si>
   <si>
     <t>At the end of your turn, gain an extra action. Exhaust.</t>
+  </si>
+  <si>
+    <t>The enemy loses 13 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>The enemy loses 18 HP at the start of your next X turns.</t>
   </si>
 </sst>
 </file>
@@ -2009,7 +2009,7 @@
         <v>88</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>88</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2200,7 +2200,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2815,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2925,13 +2925,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2983,13 +2983,13 @@
         <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3012,13 +3012,13 @@
         <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3157,13 +3157,13 @@
         <v>88</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3186,13 +3186,13 @@
         <v>88</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3366,13 +3366,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3569,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3633,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3772,7 +3772,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
@@ -3807,7 +3807,7 @@
         <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3830,13 +3830,13 @@
         <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3859,13 +3859,13 @@
         <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3888,13 +3888,13 @@
         <v>88</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>231</v>
+        <v>294</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>232</v>
+        <v>295</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3917,13 +3917,13 @@
         <v>88</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3946,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3975,13 +3975,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -4033,13 +4033,13 @@
         <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>89</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>54</v>
@@ -4120,13 +4120,13 @@
         <v>88</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4581,7 +4581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4689,13 +4689,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -4713,13 +4713,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Nerf Mana cards, fix Encode and ButterflyEffect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D50654D-C249-C54B-ADD0-D268EE946BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB258F1B-37A0-5340-8CAD-482BB160AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -244,9 +244,6 @@
     <t>Whenever you play a card, upgrade the card for the rest of the combat.</t>
   </si>
   <si>
-    <t>Deal 8 damage. When you draw this card, increase its damage by 4 this combat.</t>
-  </si>
-  <si>
     <t>Deal 4 damage. Increase this card's cost by 1 and double its damage this combat.</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>Deal 6 damage. Recall: Deal 6 damage.</t>
   </si>
   <si>
-    <t>Gain 7 Block. When you draw this card, increase its Block by 3 this combat.</t>
-  </si>
-  <si>
     <t>Gain 12 Block. Recall: Gain 12 Block.</t>
   </si>
   <si>
@@ -601,12 +595,6 @@
     <t>Deal 13 damage. Trigger all Recall effects this turn.</t>
   </si>
   <si>
-    <t>Deal 12 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
-  </si>
-  <si>
-    <t>Deal 16 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
-  </si>
-  <si>
     <t>Retain a card. Recall: It costs 0 this turn.</t>
   </si>
   <si>
@@ -844,12 +832,6 @@
     <t>Deal 16 damage. Place this card onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Deal 8 damage. When you draw this card, increase its damage by 6 this combat.</t>
-  </si>
-  <si>
-    <t>Gain 7 Block. When you draw this card, increase its Block by 5 this combat.</t>
-  </si>
-  <si>
     <t>Require 3 E. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
   </si>
   <si>
@@ -871,12 +853,6 @@
     <t>Gain 2 E and draw 1 card at the start of your next X turns.</t>
   </si>
   <si>
-    <t>Deal 14 damage. Repeat your next Recall effect.</t>
-  </si>
-  <si>
-    <t>Deal 18 damage. Repeat your next Recall effect.</t>
-  </si>
-  <si>
     <t>Deal 15 damage. Recall: Gain 2 E.</t>
   </si>
   <si>
@@ -925,13 +901,37 @@
     <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter+ to your hand.</t>
   </si>
   <si>
-    <t>At the end of your turn, gain an extra action. Exhaust.</t>
-  </si>
-  <si>
     <t>The enemy loses 13 HP at the start of your next X turns.</t>
   </si>
   <si>
     <t>The enemy loses 18 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. When you draw this card, increase its Block by 3 this combat.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. When you draw this card, increase its Block by 5 this combat.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage. When you draw this card, increase its damage by 4 this combat.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage. When you draw this card, increase its damage by 6 this combat.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
+  </si>
+  <si>
+    <t>Deal 13 damage. Recall: Deal damage to ALL enemies based on unblocked damage dealt.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage. Repeat your next Recall effect.</t>
+  </si>
+  <si>
+    <t>Deal 16 damage. Repeat your next Recall effect.</t>
+  </si>
+  <si>
+    <t>Repeat ALL your Recall effects. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,31 +1836,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2087,18 +2087,18 @@
         <v>45</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
         <v>47</v>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -2160,13 +2160,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -2177,13 +2177,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -2194,13 +2194,13 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2211,13 +2211,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2279,13 +2279,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -2296,13 +2296,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2386,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2432,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>30</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2780,13 +2780,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>66</v>
+        <v>289</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>185</v>
+        <v>291</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>186</v>
+        <v>292</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2925,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,13 +3070,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>54</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3125,16 @@
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3285,7 +3285,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3366,13 +3366,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3482,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>287</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,13 +3653,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>59</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3856,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,16 +3914,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3946,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,13 +3975,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,16 +4030,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>54</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4062,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,13 +4146,13 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>53</v>
@@ -4218,12 +4218,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4409,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4581,8 +4581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4623,12 +4623,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4640,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4666,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4689,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4710,16 +4710,16 @@
         <v>37</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Nerf jade card numbers
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB258F1B-37A0-5340-8CAD-482BB160AA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4055D08-B3A9-2441-9490-41687BC3F829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="295">
   <si>
     <t>Card</t>
   </si>
@@ -250,18 +250,6 @@
     <t>Deal 6 damage. Increase this card's cost by 1 and double its damage this combat.</t>
   </si>
   <si>
-    <t>Deal 8 damage and apply 2 Vulnerable. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage and apply 3 Vulnerable. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 10 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
-  </si>
-  <si>
-    <t>Deal 14 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
-  </si>
-  <si>
     <t>Recall: If the enemy intends to attack, apply 3 Weak. Otherwise apply 3 Vulnerable.</t>
   </si>
   <si>
@@ -424,9 +412,6 @@
     <t>Deja Vu</t>
   </si>
   <si>
-    <t>Rewinder</t>
-  </si>
-  <si>
     <t>Split Second</t>
   </si>
   <si>
@@ -532,12 +517,6 @@
     <t>Arcane Blessing</t>
   </si>
   <si>
-    <t>Gain 2 Jade. Deal 10 damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Gain 2 Jade. Deal 13 damage for each Jade you have.</t>
-  </si>
-  <si>
     <t>Goof Off</t>
   </si>
   <si>
@@ -727,18 +706,9 @@
     <t>Draw 4 cards. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Repeat your next Recall effect 3 times. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>At the start of your turn, draw 1 card and put a card from your hand onto the top of your draw pile.</t>
   </si>
   <si>
-    <t>Gain 5 Block. Gain 1 E and 1 Jade. Place this card onto the top of your drawpile. Ethereal.</t>
-  </si>
-  <si>
-    <t>Gain 5 Block. Gain 1 E and 1 Jade. Place this card onto the top of your drawpile.</t>
-  </si>
-  <si>
     <t>Discard your draw pile. Trigger all Recall effects this turn. Exhaust.</t>
   </si>
   <si>
@@ -760,57 +730,24 @@
     <t>Deal 8 damage. Deal 3 additional damage for each Jade you have.</t>
   </si>
   <si>
-    <t>Deal 15 damage and draw 2 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage and draw 1 card. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 12 damage to ALL enemies. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 16 damage to ALL enemies. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 5 damage to ALL enemies X times. If X is 3 or more, apply 2 Vulnerable and 2 Weak to ALL enemies and gain 1 Jade.</t>
   </si>
   <si>
     <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 3 Vulnerable and 3 Weak to ALL enemies and gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 18X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Deal 24X damage. Gain X Jade. Exhaust.</t>
-  </si>
-  <si>
     <t>Deal 7 damage. Gain 1 E and 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 11 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
-    <t>Gain 4 Block. Gain 2 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
     <t>Recall: Gain 6 Block.</t>
   </si>
   <si>
     <t>Recall: Gain 9 Block.</t>
   </si>
   <si>
-    <t>Gain 12 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Gain 16 Block. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn. Exhaust.</t>
   </si>
   <si>
-    <t>Repeat your next Recall effect 2 times. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Whenever you receive unblocked Attack damage, Recall the amount of damage received as Block.</t>
   </si>
   <si>
@@ -838,12 +775,6 @@
     <t>Require 3 E. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
   </si>
   <si>
-    <t>Scry 3. Draw 1 card. Exhaust.</t>
-  </si>
-  <si>
-    <t>Scry 5. Draw 1 card. Exhaust.</t>
-  </si>
-  <si>
     <t>Gain 9 Block. Recall: Gain 9 Block.</t>
   </si>
   <si>
@@ -889,9 +820,6 @@
     <t>Draw X cards. They cost 0 this turn.</t>
   </si>
   <si>
-    <t>Gain 5 Block. Gain 3 additional Block for each Jade that you have.</t>
-  </si>
-  <si>
     <t>Deal 10 damage. Deal 4 additional damage for each Jade you have.</t>
   </si>
   <si>
@@ -932,6 +860,75 @@
   </si>
   <si>
     <t>Repeat ALL your Recall effects. Exhaust.</t>
+  </si>
+  <si>
+    <t>Repeat your next Recall effect twice. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 5 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage and apply 1 Vulnerable. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage and apply 2 Vulnerable. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage and draw 1 card. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 13 damage and draw 2 cards. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 15 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage to ALL enemies. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage to ALL enemies. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 9 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 11 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Deal 15X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 20X damage. Gain X Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Draw 2 cards. Put a card from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Draw 3 cards. Put a card from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Gain 6 Block. Gain 2 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Gain 8 Block. Gain 3 additional Block for each Jade that you have.</t>
+  </si>
+  <si>
+    <t>Gain 4 Block. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 6 Block. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 11 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 14 Block. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Rewind</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1725,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1737,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1777,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1792,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,42 +1833,42 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>88</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9">
         <f>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1997,7 +1994,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2003,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2020,7 +2017,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2029,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2087,18 +2084,18 @@
         <v>45</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -2109,13 +2106,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -2126,13 +2123,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
         <v>47</v>
@@ -2143,13 +2140,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -2160,13 +2157,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -2177,13 +2174,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -2194,13 +2191,13 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2211,13 +2208,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -2228,13 +2225,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -2245,13 +2242,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -2262,13 +2259,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2279,13 +2276,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -2296,13 +2293,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -2313,13 +2310,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -2345,7 +2342,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2383,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2400,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2420,7 +2417,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2429,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>274</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>275</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -2449,7 +2446,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2458,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2478,7 +2475,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2487,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2507,7 +2504,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2516,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2565,7 +2562,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2591,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2623,7 +2620,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2632,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2652,7 +2649,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2661,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -2681,7 +2678,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2690,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>239</v>
+        <v>276</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2710,7 +2707,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2719,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>279</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>71</v>
+        <v>278</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>30</v>
@@ -2739,7 +2736,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2748,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2768,7 +2765,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2797,7 +2794,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2806,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2826,7 +2823,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2835,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2855,7 +2852,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2864,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -2884,7 +2881,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2893,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2913,7 +2910,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2922,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2942,7 +2939,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2948,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2971,7 +2968,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2977,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3000,7 +2997,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3006,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3029,7 +3026,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3038,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>162</v>
+        <v>282</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>163</v>
+        <v>283</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3058,7 +3055,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,13 +3067,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>54</v>
@@ -3087,7 +3084,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3096,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3116,7 +3113,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3122,16 @@
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -3145,7 +3142,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3151,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3174,7 +3171,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3180,16 @@
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3220,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3259,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3285,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3294,9 +3291,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3305,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3325,7 +3322,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3334,16 +3331,16 @@
         <v>36</v>
       </c>
       <c r="D4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3352,9 +3349,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3363,16 +3360,16 @@
         <v>36</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="F5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3383,7 +3380,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3412,7 +3409,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3421,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3441,7 +3438,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3450,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -3470,7 +3467,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3479,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
@@ -3499,7 +3496,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3508,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3528,7 +3525,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3557,7 +3554,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3569,13 +3566,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>252</v>
+        <v>293</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3586,7 +3583,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3595,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -3615,7 +3612,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3624,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3644,7 +3641,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,13 +3650,13 @@
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>59</v>
@@ -3673,7 +3670,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3702,7 +3699,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3711,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3731,7 +3728,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3760,7 +3757,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3769,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -3789,7 +3786,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3795,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3818,7 +3815,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3824,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3847,7 +3844,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3853,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3876,7 +3873,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3882,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3914,16 +3911,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3934,7 +3931,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3946,13 +3943,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3963,7 +3960,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>294</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3972,16 +3969,16 @@
         <v>37</v>
       </c>
       <c r="D26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>227</v>
+        <v>272</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -3992,7 +3989,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4021,7 +4018,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4030,16 +4027,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>54</v>
@@ -4050,7 +4047,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,13 +4059,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
@@ -4079,7 +4076,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4108,7 +4105,7 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4114,16 @@
         <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4137,7 +4134,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,13 +4143,13 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>53</v>
@@ -4177,7 +4174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4218,12 +4215,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4232,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4252,7 +4249,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4261,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4281,7 +4278,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4290,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -4310,7 +4307,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4319,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4339,7 +4336,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4357,7 +4354,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -4368,7 +4365,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4377,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4397,7 +4394,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4406,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4426,7 +4423,7 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4435,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4455,7 +4452,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4484,7 +4481,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4513,7 +4510,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4542,7 +4539,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4581,7 +4578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -4623,12 +4620,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4640,13 +4637,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4654,7 +4651,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4666,18 +4663,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4689,19 +4686,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4713,13 +4710,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add card art and nerf some numbers
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4055D08-B3A9-2441-9490-41687BC3F829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E83A52-44AB-394A-82F1-33C19CFE97B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -201,12 +201,6 @@
     <t>Deal 4 damage. Put a random card from your discard pile into your hand.</t>
   </si>
   <si>
-    <t>Your next Attack deals 6X additional damage.</t>
-  </si>
-  <si>
-    <t>Your next Attack deals 9X additional damage.</t>
-  </si>
-  <si>
     <t>Manipulation
 Jade</t>
   </si>
@@ -538,9 +532,6 @@
     <t>Adept Spellcaster</t>
   </si>
   <si>
-    <t>Whenever you spend at least 3 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
-  </si>
-  <si>
     <t>Whenever you consume Jade, your next Attack deals 3 additional damage.</t>
   </si>
   <si>
@@ -739,12 +730,6 @@
     <t>Deal 7 damage. Gain 1 E and 1 Jade.</t>
   </si>
   <si>
-    <t>Recall: Gain 6 Block.</t>
-  </si>
-  <si>
-    <t>Recall: Gain 9 Block.</t>
-  </si>
-  <si>
     <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn. Exhaust.</t>
   </si>
   <si>
@@ -829,12 +814,6 @@
     <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter+ to your hand.</t>
   </si>
   <si>
-    <t>The enemy loses 13 HP at the start of your next X turns.</t>
-  </si>
-  <si>
-    <t>The enemy loses 18 HP at the start of your next X turns.</t>
-  </si>
-  <si>
     <t>Gain 5 Block. When you draw this card, increase its Block by 3 this combat.</t>
   </si>
   <si>
@@ -904,12 +883,6 @@
     <t>Deal 20X damage. Gain X Jade. Exhaust.</t>
   </si>
   <si>
-    <t>Draw 2 cards. Put a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Draw 3 cards. Put a card from your hand onto the top of your draw pile.</t>
-  </si>
-  <si>
     <t>Gain 6 Block. Gain 2 additional Block for each Jade that you have.</t>
   </si>
   <si>
@@ -929,6 +902,33 @@
   </si>
   <si>
     <t>Rewind</t>
+  </si>
+  <si>
+    <t>Draw 4 cards. Put 3 cards from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Draw 5 cards. Put 3 cards from your hand onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Recall: Gain 5 Block.</t>
+  </si>
+  <si>
+    <t>Recall: Gain 8 Block.</t>
+  </si>
+  <si>
+    <t>Your next Attack deals 5X additional damage.</t>
+  </si>
+  <si>
+    <t>Your next Attack deals 8X additional damage.</t>
+  </si>
+  <si>
+    <t>The enemy loses 12 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>The enemy loses 16 HP at the start of your next X turns.</t>
+  </si>
+  <si>
+    <t>Whenever you spend at least 2 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1725,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1737,7 +1737,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1777,10 +1777,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1792,7 +1792,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1833,31 +1833,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1994,7 +1994,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2003,13 +2003,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2029,13 +2029,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2084,18 +2084,18 @@
         <v>45</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -2106,13 +2106,13 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -2123,13 +2123,13 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
         <v>47</v>
@@ -2140,13 +2140,13 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -2157,13 +2157,13 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -2174,13 +2174,13 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D7" t="s">
         <v>46</v>
@@ -2191,13 +2191,13 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2208,13 +2208,13 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -2225,13 +2225,13 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -2242,13 +2242,13 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
@@ -2276,13 +2276,13 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D13" t="s">
         <v>46</v>
@@ -2293,13 +2293,13 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -2310,13 +2310,13 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D15" t="s">
         <v>46</v>
@@ -2342,7 +2342,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2383,12 +2383,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2400,13 +2400,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2429,13 +2429,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2458,13 +2458,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2487,13 +2487,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2516,13 +2516,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2533,7 +2533,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2632,13 +2632,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2661,13 +2661,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>32</v>
@@ -2678,7 +2678,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2690,13 +2690,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2719,13 +2719,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>30</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2748,13 +2748,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2777,13 +2777,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2806,13 +2806,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2835,13 +2835,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2864,13 +2864,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H18" t="s">
         <v>31</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2893,13 +2893,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2922,13 +2922,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2939,7 +2939,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2948,16 +2948,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2977,16 +2977,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3006,16 +3006,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3026,7 +3026,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3038,13 +3038,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3067,16 +3067,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3096,13 +3096,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3122,16 +3122,16 @@
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3151,16 +3151,16 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3180,16 +3180,16 @@
         <v>37</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3217,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3259,12 +3259,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3276,13 +3276,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3293,7 +3293,7 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3305,13 +3305,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3322,7 +3322,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3334,13 +3334,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3392,13 +3392,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3421,13 +3421,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>231</v>
+        <v>288</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>232</v>
+        <v>289</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3438,7 +3438,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3450,13 +3450,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3479,13 +3479,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
         <v>31</v>
@@ -3496,7 +3496,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3508,13 +3508,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3554,7 +3554,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3566,13 +3566,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3583,7 +3583,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3595,13 +3595,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H13" t="s">
         <v>33</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3624,13 +3624,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3650,16 +3650,16 @@
         <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H15" t="s">
         <v>33</v>
@@ -3670,7 +3670,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3682,16 +3682,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3699,7 +3699,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3711,13 +3711,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3769,13 +3769,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3795,16 +3795,16 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3815,7 +3815,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3824,16 +3824,16 @@
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3853,16 +3853,16 @@
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3873,7 +3873,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3882,16 +3882,16 @@
         <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>261</v>
+        <v>292</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3911,16 +3911,16 @@
         <v>38</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3931,7 +3931,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3943,13 +3943,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3960,7 +3960,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3972,13 +3972,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -3989,7 +3989,7 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4027,19 +4027,19 @@
         <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4059,13 +4059,13 @@
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H29" t="s">
         <v>31</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4114,16 +4114,16 @@
         <v>37</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4143,16 +4143,16 @@
         <v>37</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>52</v>
+        <v>290</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>53</v>
+        <v>291</v>
       </c>
       <c r="H32" t="s">
         <v>32</v>
@@ -4173,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4215,12 +4215,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4232,13 +4232,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4261,13 +4261,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4290,13 +4290,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4319,13 +4319,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4336,7 +4336,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4348,13 +4348,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>33</v>
@@ -4365,7 +4365,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4377,13 +4377,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4406,13 +4406,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>164</v>
+        <v>294</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>164</v>
+        <v>294</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4435,13 +4435,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4464,13 +4464,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4493,13 +4493,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>30</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4539,7 +4539,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4551,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -4579,7 +4579,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4620,12 +4620,12 @@
         <v>29</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4637,13 +4637,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4663,18 +4663,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4686,19 +4686,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4710,13 +4710,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change Goof Off effect
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E83A52-44AB-394A-82F1-33C19CFE97B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13AFAF7-5689-5745-81EF-A984965EC1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -643,12 +643,6 @@
     <t>The first time you consume Jade each combat, gain 1 Strength and 1 Dexterity.</t>
   </si>
   <si>
-    <t>Deal 10 damage. Discard the top 3 cards of your draw pile and draw a card.</t>
-  </si>
-  <si>
-    <t>Deal 13 damage. Discard the top 3 cards of your draw pile and draw a card.</t>
-  </si>
-  <si>
     <t>Magic Chant - Spring</t>
   </si>
   <si>
@@ -929,6 +923,12 @@
   </si>
   <si>
     <t>Whenever you spend at least 2 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. Draw 3 cards and discard them.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage. Draw 3 cards and discard them.</t>
   </si>
 </sst>
 </file>
@@ -2006,7 +2006,7 @@
         <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>80</v>
@@ -2029,13 +2029,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2197,7 +2197,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D8" t="s">
         <v>47</v>
@@ -2341,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2400,13 +2400,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -2429,13 +2429,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -2458,13 +2458,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -2487,13 +2487,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>199</v>
+        <v>293</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>200</v>
+        <v>294</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -2516,13 +2516,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -2632,13 +2632,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -2690,13 +2690,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -2719,13 +2719,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>30</v>
@@ -2748,13 +2748,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H14" t="s">
         <v>30</v>
@@ -2806,13 +2806,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H16" t="s">
         <v>33</v>
@@ -2835,13 +2835,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>33</v>
@@ -2893,13 +2893,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H19" t="s">
         <v>31</v>
@@ -2922,13 +2922,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -2951,13 +2951,13 @@
         <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>80</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>39</v>
@@ -2980,13 +2980,13 @@
         <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H22" t="s">
         <v>32</v>
@@ -3009,13 +3009,13 @@
         <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
@@ -3038,13 +3038,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>30</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3096,13 +3096,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
@@ -3154,13 +3154,13 @@
         <v>80</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H28" t="s">
         <v>32</v>
@@ -3183,13 +3183,13 @@
         <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>34</v>
@@ -3282,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -3305,13 +3305,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -3334,13 +3334,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
@@ -3363,13 +3363,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H5" t="s">
         <v>33</v>
@@ -3421,13 +3421,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -3508,13 +3508,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H10" t="s">
         <v>32</v>
@@ -3566,13 +3566,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
@@ -3624,13 +3624,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H14" t="s">
         <v>33</v>
@@ -3711,13 +3711,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H17" t="s">
         <v>31</v>
@@ -3769,7 +3769,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
@@ -3804,7 +3804,7 @@
         <v>80</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>39</v>
@@ -3827,13 +3827,13 @@
         <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H21" t="s">
         <v>32</v>
@@ -3856,13 +3856,13 @@
         <v>80</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
@@ -3873,7 +3873,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,13 +3885,13 @@
         <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H23" t="s">
         <v>32</v>
@@ -3914,13 +3914,13 @@
         <v>80</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>32</v>
@@ -3943,13 +3943,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
@@ -3960,7 +3960,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3972,13 +3972,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>35</v>
@@ -4030,13 +4030,13 @@
         <v>81</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>81</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>52</v>
@@ -4117,13 +4117,13 @@
         <v>80</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>32</v>
@@ -4146,13 +4146,13 @@
         <v>80</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>80</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H32" t="s">
         <v>32</v>
@@ -4173,7 +4173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -4261,13 +4261,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
@@ -4319,13 +4319,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>33</v>
@@ -4377,13 +4377,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -4406,13 +4406,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -4435,13 +4435,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4637,13 +4637,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -4651,7 +4651,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4663,18 +4663,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4686,19 +4686,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -4710,13 +4710,13 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Balance change to some cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189A4894-321B-624B-88DC-44CB93437D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45F108F-9F12-9145-8BCE-65AA9D703D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="297">
   <si>
     <t>Card</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Deal 12X damage. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Play the last card that you played.</t>
   </si>
   <si>
     <t>Whenever you play a cost X card, its effects are increased by 2.</t>
@@ -250,12 +247,6 @@
     <t>Recall: If the enemy intends to attack, apply 2 Weak. Otherwise apply 2 Vulnerable.</t>
   </si>
   <si>
-    <t>Deal 14 damage. It costs 0 if you have used at least 2 E on a X cost card this turn.</t>
-  </si>
-  <si>
-    <t>Deal 18 damage. It costs 0 if you have used at least 2 E on a X cost card this turn.</t>
-  </si>
-  <si>
     <t>Deal 6 damage. Recall: Deal 6 damage.</t>
   </si>
   <si>
@@ -661,12 +652,6 @@
     <t>Magic Chant - Winter</t>
   </si>
   <si>
-    <t>Gain 10 Block. Recall: Add a Magic Chant - Fall to your hand. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 13 Block. Recall: Add a Magic Chant - Fall+ to your hand. Exhaust.</t>
-  </si>
-  <si>
     <t>Increase the effect of the next cost X card played by 2.</t>
   </si>
   <si>
@@ -763,18 +748,9 @@
     <t>Gain 2 E and draw 1 card at the start of your next X turns.</t>
   </si>
   <si>
-    <t>Deal 15 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
-    <t>Deal 20 damage. Recall: Gain 2 E.</t>
-  </si>
-  <si>
     <t>Shuffle X random cost X cards into your draw pile. They are free to play once. Exhaust.</t>
   </si>
   <si>
-    <t>Shuffle X random upgraded cost X cards into your draw pile. They are free to play once. Exhaust.</t>
-  </si>
-  <si>
     <t>Gain 11 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
   </si>
   <si>
@@ -802,12 +778,6 @@
     <t>Deal 10 damage. Deal 4 additional damage for each Jade you have.</t>
   </si>
   <si>
-    <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter to your hand.</t>
-  </si>
-  <si>
-    <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter+ to your hand.</t>
-  </si>
-  <si>
     <t>Gain 5 Block. When you draw this card, increase its Block by 3 this combat.</t>
   </si>
   <si>
@@ -832,9 +802,6 @@
     <t>Deal 16 damage. Repeat your next Recall effect.</t>
   </si>
   <si>
-    <t>Repeat ALL your Recall effects. Exhaust.</t>
-  </si>
-  <si>
     <t>Repeat your next Recall effect twice. Gain 1 Jade.</t>
   </si>
   <si>
@@ -847,12 +814,6 @@
     <t>Deal 10 damage and apply 2 Vulnerable. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 11 damage and draw 1 card. Gain 1 Jade.</t>
-  </si>
-  <si>
-    <t>Deal 13 damage and draw 2 cards. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 15 damage. If you have Jade, gain 1 Jade to deal double damage.</t>
   </si>
   <si>
@@ -929,6 +890,51 @@
   </si>
   <si>
     <t>Deal 14 damage. Draw 3 cards and discard them.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage and draw 1 card. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage and draw 2 cards. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 18 damage. Recall: Gain 2 E.</t>
+  </si>
+  <si>
+    <t>Deal 12 damage. It costs 0 if you have spent E on a X cost card this turn.</t>
+  </si>
+  <si>
+    <t>Deal 16 damage. It costs 0 if you have spent E on a X cost card this turn.</t>
+  </si>
+  <si>
+    <t>Play the last card that you played this turn.</t>
+  </si>
+  <si>
+    <t>Shuffle X random cost X cards into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, repeat your next Recall effect. Recall: Shuffle a Magic Chant - Winter into your draw pile.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain an extra action at the end of your turn.</t>
+  </si>
+  <si>
+    <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter into your draw pile.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, deal 6 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, deal 8 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer+ into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 8 Block. Recall: Shuffle a Magic Chant - Fall into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 10 Block. Recall: Shuffle a Magic Chant - Fall+ into your draw pile. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1040,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="45">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1249,19 +1258,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A0365BF5-8AEF-1541-8A73-1FAFC18B3000}" name="Table5" displayName="Table5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A0365BF5-8AEF-1541-8A73-1FAFC18B3000}" name="Table5" displayName="Table5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{34504B4D-C4C2-9A41-B374-E8AAE8CE5F50}" name="Type Distribution" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{A000506B-CF71-5E40-9E19-3283EB9AB6A5}" name="Attack" dataDxfId="40">
+    <tableColumn id="1" xr3:uid="{34504B4D-C4C2-9A41-B374-E8AAE8CE5F50}" name="Type Distribution" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{A000506B-CF71-5E40-9E19-3283EB9AB6A5}" name="Attack" dataDxfId="41">
       <calculatedColumnFormula>COUNTIF(Attack!B:B, "Attack")+2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E4910042-1C4F-7241-AF97-15EAE0ED3526}" name="Skill" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{E4910042-1C4F-7241-AF97-15EAE0ED3526}" name="Skill" dataDxfId="40">
       <calculatedColumnFormula>COUNTIF(Skill!B:B, "Skill")+2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{ACD01204-B8A4-A94E-9713-ED0AAFE7864A}" name="Power" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{ACD01204-B8A4-A94E-9713-ED0AAFE7864A}" name="Power" dataDxfId="39">
       <calculatedColumnFormula>COUNTIF(Power!B:B, "Power")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C4A535F2-9151-CD4A-B7A5-B26959DE0891}" name="Total" dataDxfId="37">
+    <tableColumn id="5" xr3:uid="{C4A535F2-9151-CD4A-B7A5-B26959DE0891}" name="Total" dataDxfId="38">
       <calculatedColumnFormula>SUM(Table5[[#This Row],[Attack]:[Power]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1270,20 +1279,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FBC4ED66-205A-2B4B-8038-24BE55587C8B}" name="Table6" displayName="Table6" ref="A4:F5" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FBC4ED66-205A-2B4B-8038-24BE55587C8B}" name="Table6" displayName="Table6" ref="A4:F5" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{723025F6-8AC8-A54C-B8BF-62EFE06A88F3}" name="Rarity Distribution" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{5873556F-3E30-8C41-A882-5F91FF21B2CD}" name="Starter" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{97A168A8-6B9F-D544-81CC-2F6894EAA3BD}" name="Common" dataDxfId="32">
+    <tableColumn id="1" xr3:uid="{723025F6-8AC8-A54C-B8BF-62EFE06A88F3}" name="Rarity Distribution" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{5873556F-3E30-8C41-A882-5F91FF21B2CD}" name="Starter" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{97A168A8-6B9F-D544-81CC-2F6894EAA3BD}" name="Common" dataDxfId="33">
       <calculatedColumnFormula>COUNTIF(Attack!C:C, "1 - Common") + COUNTIF(Skill!C:C, "1 - Common")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{CC9EE848-AEB4-F64C-885E-A1555CBCEB7E}" name="Uncommon" dataDxfId="31">
+    <tableColumn id="4" xr3:uid="{CC9EE848-AEB4-F64C-885E-A1555CBCEB7E}" name="Uncommon" dataDxfId="32">
       <calculatedColumnFormula>COUNTIF(Attack!C:C, "2 - Uncommon") + COUNTIF(Skill!C:C, "2 - Uncommon") + COUNTIF(Power!C:C, "2 - Uncommon")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2125D09F-2585-0A4E-BC5B-5316265C0FEE}" name="Rare" dataDxfId="30">
+    <tableColumn id="5" xr3:uid="{2125D09F-2585-0A4E-BC5B-5316265C0FEE}" name="Rare" dataDxfId="31">
       <calculatedColumnFormula>COUNTIF(Attack!C:C, "3 - Rare") + COUNTIF(Skill!C:C, "3 - Rare") + COUNTIF(Power!C:C, "3 - Rare")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F99C6110-6813-294F-8E6C-4A873016DDF9}" name="Total" dataDxfId="29">
+    <tableColumn id="6" xr3:uid="{F99C6110-6813-294F-8E6C-4A873016DDF9}" name="Total" dataDxfId="30">
       <calculatedColumnFormula>SUM(Table6[[#This Row],[Starter]:[Rare]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1292,31 +1301,31 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{61E7CF1C-5F0E-754C-AAD2-411AA0D4C832}" name="Table7" displayName="Table7" ref="A7:I8" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{61E7CF1C-5F0E-754C-AAD2-411AA0D4C832}" name="Table7" displayName="Table7" ref="A7:I8" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{40AE5186-ED5B-7A43-B70B-C74345C2BF59}" name="Energy Distribution" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{6311906F-96D9-1444-8E4B-387C2346C3E9}" name="0" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{40AE5186-ED5B-7A43-B70B-C74345C2BF59}" name="Energy Distribution" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{6311906F-96D9-1444-8E4B-387C2346C3E9}" name="0" dataDxfId="26">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 0) + COUNTIF(Skill!D:D, 0) + COUNTIF(Power!D:D, 0) + 1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{70A46805-952A-8341-9D29-48388A36F6AD}" name="1" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{70A46805-952A-8341-9D29-48388A36F6AD}" name="1" dataDxfId="25">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7C55F4FE-B98F-7048-B862-BD96E32386C7}" name="2" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{7C55F4FE-B98F-7048-B862-BD96E32386C7}" name="2" dataDxfId="24">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DAABB23E-D56D-004E-A811-01E3D4E05C18}" name="3" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{DAABB23E-D56D-004E-A811-01E3D4E05C18}" name="3" dataDxfId="23">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 3) + COUNTIF(Skill!D:D, 3) + COUNTIF(Power!D:D, 3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{48BE9FBD-CD55-934B-AE03-FEE3B5119F04}" name="4+" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{48BE9FBD-CD55-934B-AE03-FEE3B5119F04}" name="4+" dataDxfId="22">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, 4) + COUNTIF(Skill!D:D, 4) + COUNTIF(Power!D:D, 4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{4BD6AD74-51C2-9C4D-8E88-D51309874FDA}" name="X" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{4BD6AD74-51C2-9C4D-8E88-D51309874FDA}" name="X" dataDxfId="21">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, "X") + COUNTIF(Skill!D:D, "X") + COUNTIF(Power!D:D, "X") + 1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{623CD9FD-C1D3-F744-9B45-1427C108460C}" name="-" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{623CD9FD-C1D3-F744-9B45-1427C108460C}" name="-" dataDxfId="20">
       <calculatedColumnFormula>COUNTIF(Attack!D:D, "-") + COUNTIF(Skill!D:D, "-") + COUNTIF(Power!D:D, "-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9780DADF-B233-7D42-BDCD-4E234335988C}" name="Total" dataDxfId="18">
+    <tableColumn id="9" xr3:uid="{9780DADF-B233-7D42-BDCD-4E234335988C}" name="Total" dataDxfId="19">
       <calculatedColumnFormula>SUM(Table7[[#This Row],[0]:[-]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1325,7 +1334,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7C756C6-3086-B84D-8124-5C5A39DD6F88}" name="Table1" displayName="Table1" ref="A1:I29" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7C756C6-3086-B84D-8124-5C5A39DD6F88}" name="Table1" displayName="Table1" ref="A1:I29" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:I29" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I29">
     <sortCondition ref="C2:C29"/>
@@ -1336,10 +1345,10 @@
     <tableColumn id="1" xr3:uid="{1F29B09D-D19E-FA48-9E7F-BAC34439E0F8}" name="Card"/>
     <tableColumn id="2" xr3:uid="{3322A061-A8AA-9A47-91E6-099290785AE1}" name="Type"/>
     <tableColumn id="3" xr3:uid="{11B78D21-A734-1B49-955F-3EFE17677D89}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{C9BCFEFD-AE44-1148-97DD-210162048243}" name="Cost" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{2B64A65A-AD66-494F-9CFA-EF4A4DC964EF}" name="Effect" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{DF6D6DB9-A817-3340-9D8F-068D1C0EE55F}" name="Cost+" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{B016A6E3-657B-0E41-93E9-11821589C0D1}" name="Effect+" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C9BCFEFD-AE44-1148-97DD-210162048243}" name="Cost" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{2B64A65A-AD66-494F-9CFA-EF4A4DC964EF}" name="Effect" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{DF6D6DB9-A817-3340-9D8F-068D1C0EE55F}" name="Cost+" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{B016A6E3-657B-0E41-93E9-11821589C0D1}" name="Effect+" dataDxfId="14"/>
     <tableColumn id="8" xr3:uid="{414D4855-A6B0-5141-92D1-574196120D8E}" name="Archtype"/>
     <tableColumn id="9" xr3:uid="{439B6A21-C7EA-2946-A0F2-B9310052717D}" name="Done"/>
   </tableColumns>
@@ -1348,7 +1357,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E0050C6-5A96-0D4F-8EE8-DB1A30499FA5}" name="Table13" displayName="Table13" ref="A1:I32" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E0050C6-5A96-0D4F-8EE8-DB1A30499FA5}" name="Table13" displayName="Table13" ref="A1:I32" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:I32" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I32">
     <sortCondition ref="C2:C32"/>
@@ -1360,10 +1369,10 @@
     <tableColumn id="1" xr3:uid="{D7BAF323-FB19-DE4E-8241-E8A673166D79}" name="Card"/>
     <tableColumn id="2" xr3:uid="{78259434-0171-D54A-98EB-47FDC48418DC}" name="Type"/>
     <tableColumn id="3" xr3:uid="{6BE0F913-4927-B548-8967-D2D5E241F539}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{4D4696EF-29FA-4648-A3F9-21E237630332}" name="Cost" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{17B7585E-F4A9-8A4E-A271-B6ADA1156BC1}" name="Effect" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{6DC7B496-C382-6046-8D6B-16011788E342}" name="Cost+" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{0544E40D-5A08-6543-9402-BF8DCAF50A36}" name="Effect+" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4D4696EF-29FA-4648-A3F9-21E237630332}" name="Cost" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{17B7585E-F4A9-8A4E-A271-B6ADA1156BC1}" name="Effect" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{6DC7B496-C382-6046-8D6B-16011788E342}" name="Cost+" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{0544E40D-5A08-6543-9402-BF8DCAF50A36}" name="Effect+" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{6AAC3F2A-041E-9340-A123-6AC70156CDE0}" name="Archtype"/>
     <tableColumn id="9" xr3:uid="{942EDD7E-F5E2-8E41-A6BC-B04682B3D06E}" name="Done"/>
   </tableColumns>
@@ -1372,7 +1381,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:I13" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4027ED0F-53C8-8941-A6D5-3595337C2E86}" name="Table134" displayName="Table134" ref="A1:I13" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:I13" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I13">
     <sortCondition ref="C2:C13"/>
@@ -1381,10 +1390,10 @@
     <tableColumn id="1" xr3:uid="{4ED489C4-F350-1D4A-86C7-32EE92042A1C}" name="Card"/>
     <tableColumn id="2" xr3:uid="{AA19D34C-C869-0D44-BE2A-5180F578A4AD}" name="Type"/>
     <tableColumn id="3" xr3:uid="{AFFE9C0B-45EB-924B-9F20-5928238A8A58}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{C1331125-4439-BB41-88D7-CE7B6D51C545}" name="Cost" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{9CE4A36D-0360-6E40-8CBA-FD0E723CC355}" name="Effect" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{C1331125-4439-BB41-88D7-CE7B6D51C545}" name="Cost" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{9CE4A36D-0360-6E40-8CBA-FD0E723CC355}" name="Effect" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{73F1147E-E7F4-A14F-A50E-BDFDDFB67163}" name="Cost+"/>
-    <tableColumn id="7" xr3:uid="{FF6644A0-523B-644F-B790-49B0344226F1}" name="Effect+" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{FF6644A0-523B-644F-B790-49B0344226F1}" name="Effect+" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{C57FAEB9-782E-3445-A11D-AAACD258DFFF}" name="Archtype"/>
     <tableColumn id="9" xr3:uid="{52C08126-3467-FD41-9D0A-1DECCB55E8F7}" name="Done"/>
   </tableColumns>
@@ -1393,7 +1402,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8D4DCD90-8849-BC4E-A780-7EF8A14AE3A0}" name="Table1345" displayName="Table1345" ref="A1:I5" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8D4DCD90-8849-BC4E-A780-7EF8A14AE3A0}" name="Table1345" displayName="Table1345" ref="A1:I5" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:I5" xr:uid="{B86BDAAF-D301-3349-A4C2-63D90E545615}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H5">
     <sortCondition ref="C1:C5"/>
@@ -1402,10 +1411,10 @@
     <tableColumn id="1" xr3:uid="{F392586C-A665-864E-8026-A6F53A3969F1}" name="Card"/>
     <tableColumn id="2" xr3:uid="{B51CD295-89C1-104A-962F-AD1E4F68DF86}" name="Type"/>
     <tableColumn id="3" xr3:uid="{37E6D650-B23D-6A40-B02E-90A20F9D2691}" name="Rarity"/>
-    <tableColumn id="4" xr3:uid="{A1DBCF33-51FA-9649-BFB9-3D2518B80229}" name="Cost" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{AEA37D5C-0344-6941-8456-C3B687F58AF2}" name="Effect" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F7C6D4FE-ABB0-5B45-9A6E-F5507258C202}" name="Cost+"/>
-    <tableColumn id="7" xr3:uid="{D67A734E-BEC8-E54A-810D-E8F4724DA1B3}" name="Effect+" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{A1DBCF33-51FA-9649-BFB9-3D2518B80229}" name="Cost" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{AEA37D5C-0344-6941-8456-C3B687F58AF2}" name="Effect" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F7C6D4FE-ABB0-5B45-9A6E-F5507258C202}" name="Cost+" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{D67A734E-BEC8-E54A-810D-E8F4724DA1B3}" name="Effect+" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{63355E4D-239A-0146-8A40-2DD33EE2AAFD}" name="Archtype"/>
     <tableColumn id="9" xr3:uid="{A359FB33-E6A7-E147-9926-FA66877A5753}" name="Done"/>
   </tableColumns>
@@ -1725,7 +1734,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1737,7 +1746,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1777,10 +1786,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1792,7 +1801,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1833,31 +1842,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="I7" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1994,7 +2003,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2003,13 +2012,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2017,7 +2026,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2029,13 +2038,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2058,7 +2067,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2072,7 +2081,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -2081,24 +2090,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2106,16 +2115,16 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -2123,16 +2132,16 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2140,16 +2149,16 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -2157,16 +2166,16 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2174,16 +2183,16 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2191,16 +2200,16 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -2208,16 +2217,16 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2225,16 +2234,16 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -2242,16 +2251,16 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -2259,16 +2268,16 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -2276,16 +2285,16 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -2293,16 +2302,16 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -2310,16 +2319,16 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -2341,8 +2350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2380,36 +2389,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -2417,28 +2426,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -2446,28 +2455,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -2475,28 +2484,28 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -2504,28 +2513,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -2533,28 +2542,28 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -2562,19 +2571,19 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2583,7 +2592,7 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -2591,28 +2600,28 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -2620,28 +2629,28 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>239</v>
+        <v>284</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>240</v>
+        <v>285</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -2649,28 +2658,28 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>286</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
+        <v>287</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -2678,28 +2687,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -2707,28 +2716,28 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -2736,28 +2745,28 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -2765,28 +2774,28 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -2794,28 +2803,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -2823,28 +2832,28 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -2852,28 +2861,28 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -2881,28 +2890,28 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -2910,28 +2919,28 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="2">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -2939,28 +2948,28 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I21" s="1" t="b">
         <v>1</v>
@@ -2968,28 +2977,28 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -2997,28 +3006,28 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -3026,28 +3035,28 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -3055,28 +3064,28 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3084,28 +3093,28 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3113,28 +3122,28 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -3142,28 +3151,28 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -3171,28 +3180,28 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -3218,7 +3227,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3256,36 +3265,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -3293,28 +3302,28 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -3322,28 +3331,28 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -3351,28 +3360,28 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -3380,28 +3389,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -3409,28 +3418,28 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3438,28 +3447,28 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -3467,28 +3476,28 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -3496,28 +3505,28 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -3525,28 +3534,28 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -3554,28 +3563,28 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -3583,28 +3592,28 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -3612,28 +3621,28 @@
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -3641,28 +3650,28 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -3670,28 +3679,28 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3699,28 +3708,28 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -3728,28 +3737,28 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="10">
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -3757,28 +3766,28 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2">
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -3786,28 +3795,28 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -3815,28 +3824,28 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -3844,28 +3853,28 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -3873,28 +3882,28 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -3902,28 +3911,28 @@
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -3931,28 +3940,28 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3960,28 +3969,28 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -3989,28 +3998,28 @@
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>22</v>
+        <v>288</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>22</v>
+        <v>288</v>
       </c>
       <c r="H27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -4018,28 +4027,28 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4047,28 +4056,28 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -4076,57 +4085,57 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2">
         <v>3</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F30" s="10">
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>241</v>
+        <v>289</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -4134,28 +4143,28 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="H32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -4173,8 +4182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4212,36 +4221,36 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -4249,28 +4258,28 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
@@ -4278,28 +4287,28 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -4307,28 +4316,28 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -4336,28 +4345,28 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -4365,28 +4374,28 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -4394,28 +4403,28 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2">
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -4423,28 +4432,28 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -4452,28 +4461,28 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -4481,28 +4490,28 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -4510,28 +4519,28 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -4539,28 +4548,28 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2">
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -4578,8 +4587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4617,106 +4626,106 @@
         <v>5</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
+        <v>293</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>201</v>
+        <v>294</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+        <v>295</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>206</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
+        <v>292</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>291</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Rework magic chant cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45F108F-9F12-9145-8BCE-65AA9D703D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B1F9E9-1985-E141-BA3A-2E1FAD37779E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -916,25 +916,25 @@
     <t>Shuffle X random cost X cards into your draw pile. Exhaust.</t>
   </si>
   <si>
-    <t>At the end of your turn, repeat your next Recall effect. Recall: Shuffle a Magic Chant - Winter into your draw pile.</t>
-  </si>
-  <si>
-    <t>Unplayable. When you draw this card, gain an extra action at the end of your turn.</t>
-  </si>
-  <si>
-    <t>At the end of your turn, repeat your next Recall effect. Recall: Add a Magic Chant - Winter into your draw pile.</t>
-  </si>
-  <si>
     <t>Unplayable. When you draw this card, deal 6 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer into your draw pile. Exhaust.</t>
   </si>
   <si>
-    <t>Unplayable. When you draw this card, deal 8 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer+ into your draw pile. Exhaust.</t>
-  </si>
-  <si>
     <t>Unplayable. When you draw this card, gain 8 Block. Recall: Shuffle a Magic Chant - Fall into your draw pile. Exhaust.</t>
   </si>
   <si>
-    <t>Unplayable. When you draw this card, gain 10 Block. Recall: Shuffle a Magic Chant - Fall+ into your draw pile. Exhaust.</t>
+    <t>Unplayable. When you draw this card, deal 10 damage to a ALL enemies. Recall: Shuffle a Magic Chant - Winter into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain an extra action at the end of your turn. Recall: Shuffle a Magic Chant - Spring+ into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, deal 9 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer+ into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, gain 12 Block. Recall: Shuffle a Magic Chant - Fall+ into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, deal 15 damage to a ALL enemies. Recall: Shuffle a Magic Chant - Winter+ into your draw pile. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -4588,7 +4588,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4646,7 +4646,7 @@
         <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>78</v>
@@ -4672,16 +4672,16 @@
         <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -4701,11 +4701,11 @@
         <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -4719,13 +4719,13 @@
         <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Only one magic chant can be active at a time
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B1F9E9-1985-E141-BA3A-2E1FAD37779E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42B61E0-2E12-554D-AEFE-8BF845C754EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="296">
   <si>
     <t>Card</t>
   </si>
@@ -637,12 +637,6 @@
     <t>Magic Chant - Spring</t>
   </si>
   <si>
-    <t>Deal 6 damage. Recall: Add a Magic Chant - Summer to your hand.</t>
-  </si>
-  <si>
-    <t>Deal 8 damage. Recall: Add a Magic Chant - Summer+ to your hand.</t>
-  </si>
-  <si>
     <t>Magic Chant - Summer</t>
   </si>
   <si>
@@ -935,6 +929,9 @@
   </si>
   <si>
     <t>Unplayable. When you draw this card, deal 15 damage to a ALL enemies. Recall: Shuffle a Magic Chant - Winter+ into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Unplayable. When you draw this card, deal 9 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer into your draw pile. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -2015,7 +2012,7 @@
         <v>77</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>77</v>
@@ -2038,13 +2035,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2206,7 +2203,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -2350,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2409,13 +2406,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -2438,13 +2435,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -2467,13 +2464,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -2496,13 +2493,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -2525,13 +2522,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
@@ -2641,13 +2638,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -2670,13 +2667,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>31</v>
@@ -2699,13 +2696,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -2728,13 +2725,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>29</v>
@@ -2757,13 +2754,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -2815,13 +2812,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -2844,13 +2841,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -2902,13 +2899,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H19" t="s">
         <v>30</v>
@@ -2931,13 +2928,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>30</v>
@@ -2960,13 +2957,13 @@
         <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>38</v>
@@ -2989,13 +2986,13 @@
         <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H22" t="s">
         <v>31</v>
@@ -3018,13 +3015,13 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>33</v>
@@ -3047,13 +3044,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>29</v>
@@ -3091,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -3105,13 +3102,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>197</v>
+        <v>288</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>198</v>
+        <v>295</v>
       </c>
       <c r="H26" t="s">
         <v>30</v>
@@ -3163,13 +3160,13 @@
         <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H28" t="s">
         <v>31</v>
@@ -3192,13 +3189,13 @@
         <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>33</v>
@@ -3291,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -3314,13 +3311,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -3343,13 +3340,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -3372,13 +3369,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -3430,13 +3427,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -3517,13 +3514,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -3575,13 +3572,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -3633,13 +3630,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F14" s="10">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -3720,13 +3717,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H17" t="s">
         <v>30</v>
@@ -3778,7 +3775,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
@@ -3813,7 +3810,7 @@
         <v>77</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>38</v>
@@ -3836,13 +3833,13 @@
         <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H21" t="s">
         <v>31</v>
@@ -3865,13 +3862,13 @@
         <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>33</v>
@@ -3882,7 +3879,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3894,13 +3891,13 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
@@ -3923,13 +3920,13 @@
         <v>77</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -3952,13 +3949,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
@@ -3969,7 +3966,7 @@
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3981,13 +3978,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F26" s="10">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>34</v>
@@ -4010,13 +4007,13 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H27" t="s">
         <v>32</v>
@@ -4039,13 +4036,13 @@
         <v>78</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>51</v>
@@ -4126,13 +4123,13 @@
         <v>77</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>31</v>
@@ -4155,13 +4152,13 @@
         <v>77</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
@@ -4270,13 +4267,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -4328,13 +4325,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -4386,13 +4383,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -4415,13 +4412,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -4444,13 +4441,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>30</v>
@@ -4588,7 +4585,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4646,13 +4643,13 @@
         <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4660,7 +4657,7 @@
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4672,18 +4669,18 @@
         <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -4695,19 +4692,19 @@
         <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -4719,13 +4716,13 @@
         <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Rework predestination and rewind
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42B61E0-2E12-554D-AEFE-8BF845C754EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B147F701-243F-924B-AA88-9A829B5900A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="295">
   <si>
     <t>Card</t>
   </si>
@@ -742,15 +742,6 @@
     <t>Gain 2 E and draw 1 card at the start of your next X turns.</t>
   </si>
   <si>
-    <t>Shuffle X random cost X cards into your draw pile. They are free to play once. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 11 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 15 Block at the start of your next X+1 turns. Gain 1 Jade. Exhaust.</t>
-  </si>
-  <si>
     <t>Recall: Gain 1 E and draw 1 card.</t>
   </si>
   <si>
@@ -796,9 +787,6 @@
     <t>Deal 16 damage. Repeat your next Recall effect.</t>
   </si>
   <si>
-    <t>Repeat your next Recall effect twice. Gain 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 5 damage. Gain 1 E and 1 Jade.</t>
   </si>
   <si>
@@ -907,9 +895,6 @@
     <t>Play the last card that you played this turn.</t>
   </si>
   <si>
-    <t>Shuffle X random cost X cards into your draw pile. Exhaust.</t>
-  </si>
-  <si>
     <t>Unplayable. When you draw this card, deal 6 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer into your draw pile. Exhaust.</t>
   </si>
   <si>
@@ -932,6 +917,18 @@
   </si>
   <si>
     <t>Unplayable. When you draw this card, deal 9 damage to a random enemy. Recall: Shuffle a Magic Chant - Summer into your draw pile. Exhaust.</t>
+  </si>
+  <si>
+    <t>Repeat ALL your Recall effects. Gain 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 11 Block at the start of your next X turns. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 15 Block at the start of your next X turns. Exhaust.</t>
+  </si>
+  <si>
+    <t>Add a random cost X card into your hand. It is free to play once. Gain 1 Jade. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1036,10 @@
   </cellStyles>
   <dxfs count="45">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1410,8 +1407,8 @@
     <tableColumn id="3" xr3:uid="{37E6D650-B23D-6A40-B02E-90A20F9D2691}" name="Rarity"/>
     <tableColumn id="4" xr3:uid="{A1DBCF33-51FA-9649-BFB9-3D2518B80229}" name="Cost" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{AEA37D5C-0344-6941-8456-C3B687F58AF2}" name="Effect" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F7C6D4FE-ABB0-5B45-9A6E-F5507258C202}" name="Cost+" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{D67A734E-BEC8-E54A-810D-E8F4724DA1B3}" name="Effect+" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F7C6D4FE-ABB0-5B45-9A6E-F5507258C202}" name="Cost+" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{D67A734E-BEC8-E54A-810D-E8F4724DA1B3}" name="Effect+" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{63355E4D-239A-0146-8A40-2DD33EE2AAFD}" name="Archtype"/>
     <tableColumn id="9" xr3:uid="{A359FB33-E6A7-E147-9926-FA66877A5753}" name="Done"/>
   </tableColumns>
@@ -1874,7 +1871,7 @@
       </c>
       <c r="C8" s="9">
         <f>COUNTIF(Attack!D:D, 1) + COUNTIF(Skill!D:D, 1) + COUNTIF(Power!D:D, 1) + 2</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9">
         <f>COUNTIF(Attack!D:D, 2) + COUNTIF(Skill!D:D, 2) + COUNTIF(Power!D:D, 2)</f>
@@ -1890,7 +1887,7 @@
       </c>
       <c r="G8" s="9">
         <f>COUNTIF(Attack!D:D, "X") + COUNTIF(Skill!D:D, "X") + COUNTIF(Power!D:D, "X") + 1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="9">
         <f>COUNTIF(Attack!D:D, "-") + COUNTIF(Skill!D:D, "-") + COUNTIF(Power!D:D, "-")</f>
@@ -2035,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2406,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -2435,13 +2432,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -2470,7 +2467,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -2493,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -2638,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -2667,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>31</v>
@@ -2696,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -2725,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>29</v>
@@ -2754,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -2812,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -2899,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H19" t="s">
         <v>30</v>
@@ -2928,13 +2925,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>30</v>
@@ -3044,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>29</v>
@@ -3102,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H26" t="s">
         <v>30</v>
@@ -3189,13 +3186,13 @@
         <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>33</v>
@@ -3223,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3311,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -3340,13 +3337,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -3369,13 +3366,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -3427,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -3531,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3543,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="2">
+        <v>262</v>
+      </c>
+      <c r="F11" s="10">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
@@ -3560,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3572,13 +3569,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F12" s="10">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>267</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -3587,9 +3584,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3601,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>170</v>
+        <v>239</v>
       </c>
       <c r="F13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>170</v>
+        <v>240</v>
       </c>
       <c r="H13" t="s">
         <v>32</v>
@@ -3616,9 +3613,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3630,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>242</v>
+        <v>170</v>
       </c>
       <c r="F14" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>243</v>
+        <v>170</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -3821,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3833,15 +3830,15 @@
         <v>77</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>230</v>
+        <v>292</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="H21" t="s">
+        <v>293</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I21" t="b">
@@ -3850,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3862,16 +3859,16 @@
         <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>33</v>
+        <v>231</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -3891,13 +3888,13 @@
         <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
@@ -3906,9 +3903,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3916,20 +3913,20 @@
       <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>240</v>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -3964,9 +3961,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>268</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,27 +3972,27 @@
         <v>36</v>
       </c>
       <c r="D26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="F26" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>34</v>
+        <v>282</v>
+      </c>
+      <c r="H26" t="s">
+        <v>32</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4003,20 +4000,20 @@
       <c r="C27" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="2">
-        <v>2</v>
+      <c r="D27" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F27" s="10">
-        <v>1</v>
+        <v>234</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H27" t="s">
-        <v>32</v>
+        <v>235</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -4024,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4032,20 +4029,20 @@
       <c r="C28" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>78</v>
+      <c r="D28" s="2">
+        <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>78</v>
+        <v>166</v>
+      </c>
+      <c r="F28" s="10">
+        <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>51</v>
+        <v>167</v>
+      </c>
+      <c r="H28" t="s">
+        <v>30</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -4053,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4062,18 +4059,18 @@
         <v>36</v>
       </c>
       <c r="D29" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="F29" s="10">
         <v>2</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I29" t="b">
@@ -4082,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4091,27 +4088,27 @@
         <v>36</v>
       </c>
       <c r="D30" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>291</v>
       </c>
       <c r="F30" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>24</v>
+        <v>291</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4122,14 +4119,14 @@
       <c r="D31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>287</v>
+      <c r="E31" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>232</v>
+      <c r="G31" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>31</v>
@@ -4152,13 +4149,13 @@
         <v>77</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>77</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
@@ -4412,13 +4409,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -4584,7 +4581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC080DC-CAAA-624E-86CF-D08125A60CBC}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -4643,13 +4640,13 @@
         <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4669,13 +4666,13 @@
         <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4692,13 +4689,13 @@
         <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -4716,13 +4713,13 @@
         <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add chemical xx and fix mystic shift bug
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B147F701-243F-924B-AA88-9A829B5900A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58CA089-71B4-6248-A275-E4480FC42272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
@@ -928,7 +928,7 @@
     <t>Gain 15 Block at the start of your next X turns. Exhaust.</t>
   </si>
   <si>
-    <t>Add a random cost X card into your hand. It is free to play once. Gain 1 Jade. Exhaust.</t>
+    <t>Choose 1 of 3 random cost X card to add to your hand. It is free to play once. Gain 1 Jade. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3903,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
Balance change for some cards
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58CA089-71B4-6248-A275-E4480FC42272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F550DCBB-3541-7242-95AE-B65CD535BF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="4" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="5" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Deal 6 damage. Recall: Gain 6 Block.</t>
   </si>
   <si>
-    <t>Deal 9 damage. Recall: Gain 9 Block.</t>
-  </si>
-  <si>
     <t>Relic</t>
   </si>
   <si>
@@ -187,15 +184,6 @@
   </si>
   <si>
     <t>Gain 1 Blur. Recall: Deal damage to ALL enemies equal to your Block.</t>
-  </si>
-  <si>
-    <t>Recall your Block. Gain 8 Block X times.</t>
-  </si>
-  <si>
-    <t>Deal 6 damage. Put a card from your discard pile into your hand.</t>
-  </si>
-  <si>
-    <t>Deal 4 damage. Put a random card from your discard pile into your hand.</t>
   </si>
   <si>
     <t>Manipulation
@@ -238,9 +226,6 @@
     <t>Deal 4 damage. Increase this card's cost by 1 and double its damage this combat.</t>
   </si>
   <si>
-    <t>Deal 6 damage. Increase this card's cost by 1 and double its damage this combat.</t>
-  </si>
-  <si>
     <t>Recall: If the enemy intends to attack, apply 3 Weak. Otherwise apply 3 Vulnerable.</t>
   </si>
   <si>
@@ -253,12 +238,6 @@
     <t>Gain 12 Block. Recall: Gain 12 Block.</t>
   </si>
   <si>
-    <t>Recall: Deal 5 damage twice X times.</t>
-  </si>
-  <si>
-    <t>Recall: Deal 7 damage twice X times.</t>
-  </si>
-  <si>
     <t>Type Distribution</t>
   </si>
   <si>
@@ -550,15 +529,6 @@
     <t>Recall: If any of the enemies intend to attack, gain 28 Block. Otherwise gain 3 Artifact.</t>
   </si>
   <si>
-    <t>Deal 9 damage. Trigger all Recall effects this turn.</t>
-  </si>
-  <si>
-    <t>Deal 13 damage. Trigger all Recall effects this turn.</t>
-  </si>
-  <si>
-    <t>Retain a card. Recall: It costs 0 this turn.</t>
-  </si>
-  <si>
     <t>Deal 6 damage 2 times. When you draw this card, increase its number of hits by 1 this combat and gain 1 Jade.</t>
   </si>
   <si>
@@ -661,12 +631,6 @@
     <t>Deal 10 damage. Put a random Attack card from your discard pile into your hand. It costs 0 this turn.</t>
   </si>
   <si>
-    <t>Recall: Deal 9 damage to a random enemy X times.</t>
-  </si>
-  <si>
-    <t>Recall: Deal 12 damage to a random enemy X times.</t>
-  </si>
-  <si>
     <t>Draw 4 cards. Gain 1 Jade.</t>
   </si>
   <si>
@@ -679,18 +643,9 @@
     <t>Discard your draw pile. Trigger all Recall effects this turn.</t>
   </si>
   <si>
-    <t>If the enemy intends to attack, gain 7X Block. Otherwise, deal 7X damage.</t>
-  </si>
-  <si>
-    <t>If the enemy intends to attack, gain 10X Block. Otherwise, deal 10X damage.</t>
-  </si>
-  <si>
     <t>Deal 9X damage. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Recall your Block. Gain 11 Block X times.</t>
-  </si>
-  <si>
     <t>Deal 8 damage. Deal 3 additional damage for each Jade you have.</t>
   </si>
   <si>
@@ -700,9 +655,6 @@
     <t>Deal 7 damage to ALL enemies X times. If X is 3 or more, apply 3 Vulnerable and 3 Weak to ALL enemies and gain 1 Jade.</t>
   </si>
   <si>
-    <t>Deal 7 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
     <t>Double your Jade and gain E equal to your Jade. Your Attack deals double damage this turn. Exhaust.</t>
   </si>
   <si>
@@ -721,18 +673,6 @@
     <t>Gain E equals to the cost of the first card you play each combat.</t>
   </si>
   <si>
-    <t>Deal 12 damage. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Deal 16 damage. Place this card onto the top of your draw pile.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 12 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
-    <t>Require 3 E. Deal 16 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
-  </si>
-  <si>
     <t>Gain 9 Block. Recall: Gain 9 Block.</t>
   </si>
   <si>
@@ -748,12 +688,6 @@
     <t>Draw 1 card. Recall: Gain 1 E and draw 1 card.</t>
   </si>
   <si>
-    <t>Ethereal. Unplayable. When you draw this card, gain 1 Intangible and 2 Jade.</t>
-  </si>
-  <si>
-    <t>Ethereal. Unplayable. When you draw this card, gain 1 Intangible and 1 Jade.</t>
-  </si>
-  <si>
     <t>Draw X cards. They cost 0 this turn. Exhaust.</t>
   </si>
   <si>
@@ -787,9 +721,6 @@
     <t>Deal 16 damage. Repeat your next Recall effect.</t>
   </si>
   <si>
-    <t>Deal 5 damage. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
     <t>Deal 8 damage and apply 1 Vulnerable. Gain 1 Jade.</t>
   </si>
   <si>
@@ -808,12 +739,6 @@
     <t>Deal 14 damage to ALL enemies. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Gain 2 Jade. Deal 9 damage for each Jade you have.</t>
-  </si>
-  <si>
-    <t>Gain 2 Jade. Deal 11 damage for each Jade you have.</t>
-  </si>
-  <si>
     <t>Deal 15X damage. Gain X Jade. Exhaust.</t>
   </si>
   <si>
@@ -826,12 +751,6 @@
     <t>Gain 8 Block. Gain 3 additional Block for each Jade that you have.</t>
   </si>
   <si>
-    <t>Gain 4 Block. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
-    <t>Gain 6 Block. Gain 1 E and 1 Jade.</t>
-  </si>
-  <si>
     <t>Gain 11 Block. Gain 1 Jade.</t>
   </si>
   <si>
@@ -868,12 +787,6 @@
     <t>Whenever you spend at least 2 E on a cost X card, gain 1 Strength and 1 Dexterity.</t>
   </si>
   <si>
-    <t>Deal 11 damage. Draw 3 cards and discard them.</t>
-  </si>
-  <si>
-    <t>Deal 14 damage. Draw 3 cards and discard them.</t>
-  </si>
-  <si>
     <t>Deal 12 damage and draw 1 card. Gain 1 Jade.</t>
   </si>
   <si>
@@ -922,13 +835,100 @@
     <t>Repeat ALL your Recall effects. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Gain 11 Block at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
-    <t>Gain 15 Block at the start of your next X turns. Exhaust.</t>
-  </si>
-  <si>
     <t>Choose 1 of 3 random cost X card to add to your hand. It is free to play once. Gain 1 Jade. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deal 5 damage. Increase this card's cost by 1 and double its damage this combat.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Draw 3 cards and discard them.</t>
+  </si>
+  <si>
+    <t>Deal 13 damage. Draw 3 cards and discard them.</t>
+  </si>
+  <si>
+    <t>Deal 11 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 15 damage. Place this card onto the top of your draw pile.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage. Put a random card from your discard pile into your hand.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Put a card from your discard pile into your hand.</t>
+  </si>
+  <si>
+    <t>Deal 8 damage. Recall: Gain 8 Block.</t>
+  </si>
+  <si>
+    <t>Deal 14 damage. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Deal 10 damage. Trigger all Recall effects this turn.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 8 damage to a random enemy X times.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 11 damage to a random enemy X times.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 8 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Gain 2 Jade. Deal 10 damage for each Jade you have.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 4 damage twice X times.</t>
+  </si>
+  <si>
+    <t>Recall: Deal 6 damage twice X times.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 10 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Require 3 E. Deal 14 damage to a random enemy X times. Gain 1 E for each enemy killed this way.</t>
+  </si>
+  <si>
+    <t>Deal 6 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Deal 9 damage. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 5 Block. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Gain 8 Block. Gain 1 E and 1 Jade.</t>
+  </si>
+  <si>
+    <t>Retain a card. Recall: It is free to play once.</t>
+  </si>
+  <si>
+    <t>Recall your Block. Gain 7 Block X times.</t>
+  </si>
+  <si>
+    <t>Recall your Block. Gain 10 Block X times.</t>
+  </si>
+  <si>
+    <t>If the enemy intends to attack, gain 6X Block. Otherwise, deal 6X damage.</t>
+  </si>
+  <si>
+    <t>If the enemy intends to attack, gain 9X Block. Otherwise, deal 9X damage.</t>
+  </si>
+  <si>
+    <t>Gain 10 Block at the start of your next X turns. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 14 Block at the start of your next X turns. Exhaust.</t>
+  </si>
+  <si>
+    <t>Exhaust. Unplayable. When you draw this card, gain 1 Intangible and 2 Jade.</t>
+  </si>
+  <si>
+    <t>Exhaust. Unplayable. When you draw this card, gain 1 Intangible and 1 Jade.</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>19</v>
@@ -1795,7 +1795,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1836,31 +1836,31 @@
     </row>
     <row r="7" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1997,7 +1997,7 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2006,13 +2006,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" ht="34" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2075,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -2084,24 +2084,24 @@
         <v>4</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2109,16 +2109,16 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -2126,16 +2126,16 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2143,16 +2143,16 @@
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2194,16 +2194,16 @@
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -2211,16 +2211,16 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2228,16 +2228,16 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -2245,16 +2245,16 @@
     </row>
     <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -2262,16 +2262,16 @@
     </row>
     <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -2279,16 +2279,16 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -2296,16 +2296,16 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -2313,16 +2313,16 @@
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2386,12 @@
         <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>247</v>
+        <v>282</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>218</v>
+        <v>283</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -2432,13 +2432,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -2461,13 +2461,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>238</v>
+        <v>216</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2548,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>269</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>270</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -2577,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -2612,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>271</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -2635,13 +2635,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="F10" s="10">
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -2664,13 +2664,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
       <c r="F11" s="10">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>31</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -2722,13 +2722,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>29</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -2751,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -2780,13 +2780,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>64</v>
+        <v>264</v>
       </c>
       <c r="H15" t="s">
         <v>32</v>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>32</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>168</v>
+        <v>273</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>169</v>
+        <v>272</v>
       </c>
       <c r="H18" t="s">
         <v>30</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -2896,13 +2896,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="F19" s="2">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>244</v>
+        <v>222</v>
       </c>
       <c r="H19" t="s">
         <v>30</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -2925,13 +2925,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="F20" s="10">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>30</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -2951,16 +2951,16 @@
         <v>37</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>206</v>
+        <v>275</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>38</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -2980,16 +2980,16 @@
         <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>211</v>
+        <v>289</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>212</v>
+        <v>290</v>
       </c>
       <c r="H22" t="s">
         <v>31</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -3009,16 +3009,16 @@
         <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>33</v>
@@ -3029,7 +3029,7 @@
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -3041,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>29</v>
@@ -3058,7 +3058,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -3070,16 +3070,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F25" s="10">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -3087,7 +3087,7 @@
     </row>
     <row r="26" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -3099,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>283</v>
+        <v>254</v>
       </c>
       <c r="F26" s="2">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="H26" t="s">
         <v>30</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -3125,16 +3125,16 @@
         <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>69</v>
+        <v>278</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>70</v>
+        <v>279</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>38</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3154,16 +3154,16 @@
         <v>36</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>228</v>
+        <v>281</v>
       </c>
       <c r="H28" t="s">
         <v>31</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -3183,16 +3183,16 @@
         <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>33</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3262,12 +3262,12 @@
         <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -3325,7 +3325,7 @@
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -3337,13 +3337,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -3366,13 +3366,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3395,13 +3395,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
@@ -3412,7 +3412,7 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -3424,13 +3424,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3453,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H8" t="s">
         <v>30</v>
@@ -3470,7 +3470,7 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -3482,13 +3482,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -3511,13 +3511,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H10" t="s">
         <v>31</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -3540,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="F11" s="10">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="H13" t="s">
         <v>32</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>170</v>
+        <v>286</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>170</v>
+        <v>286</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -3653,16 +3653,16 @@
         <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
         <v>32</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -3685,16 +3685,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F16" s="10">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -3714,13 +3714,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="H17" t="s">
         <v>30</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -3743,13 +3743,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="10">
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
         <v>30</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -3772,13 +3772,13 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="F19" s="10">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>30</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -3798,16 +3798,16 @@
         <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>287</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>214</v>
+        <v>288</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>38</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -3827,16 +3827,16 @@
         <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>31</v>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
@@ -3856,16 +3856,16 @@
         <v>37</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="H22" t="s">
         <v>31</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -3885,16 +3885,16 @@
         <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>272</v>
+        <v>245</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
@@ -3917,13 +3917,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -3934,7 +3934,7 @@
     </row>
     <row r="25" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -3946,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="F25" s="10">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -3975,13 +3975,13 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="F26" s="10">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -4001,19 +4001,19 @@
         <v>36</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>234</v>
+        <v>293</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>235</v>
+        <v>294</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -4033,13 +4033,13 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F28" s="10">
         <v>2</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H28" t="s">
         <v>30</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -4091,13 +4091,13 @@
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="F30" s="10">
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>34</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -4117,16 +4117,16 @@
         <v>36</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>237</v>
+        <v>215</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>31</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
@@ -4146,16 +4146,16 @@
         <v>36</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>270</v>
+        <v>243</v>
       </c>
       <c r="H32" t="s">
         <v>31</v>
@@ -4176,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5B952-69A0-F942-8DAF-554172FF53C0}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4218,12 +4218,12 @@
         <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -4235,13 +4235,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -4264,13 +4264,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -4293,13 +4293,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>29</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -4322,13 +4322,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>32</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -4351,13 +4351,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -4380,13 +4380,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4409,13 +4409,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4438,13 +4438,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>30</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -4467,13 +4467,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
         <v>30</v>
@@ -4484,7 +4484,7 @@
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -4496,13 +4496,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>29</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -4554,7 +4554,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -4623,12 +4623,12 @@
         <v>28</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -4637,16 +4637,16 @@
         <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>283</v>
+        <v>254</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -4663,21 +4663,21 @@
         <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>284</v>
+        <v>255</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -4686,22 +4686,22 @@
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>289</v>
+        <v>260</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -4710,16 +4710,16 @@
         <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="H5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change predestination and fix bugs
</commit_message>
<xml_diff>
--- a/Chronomancer.xlsx
+++ b/Chronomancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Slay the Spire Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE1A313-13E5-5845-9146-E26823225C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856AAF7A-783A-8D42-B28F-609BC3587731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="3" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{B58693F6-773A-8B4E-93F7-98C244145AC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="9" r:id="rId1"/>
@@ -820,9 +820,6 @@
     <t>Repeat ALL your Recall effects. Gain 1 Jade.</t>
   </si>
   <si>
-    <t>Choose 1 of 3 random cost X card to add to your hand. It is free to play once. Gain 1 Jade. Exhaust.</t>
-  </si>
-  <si>
     <t>Deal 5 damage. Increase this card's cost by 1 and double its damage this combat.</t>
   </si>
   <si>
@@ -929,6 +926,9 @@
   </si>
   <si>
     <t>Deal 8 damage. When you draw this card, increase its damage by 4 this combat.</t>
+  </si>
+  <si>
+    <t>Add a random cost X card to your hand. It is free to play once. Gain 1 Jade. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2396E-0670-B44C-B534-C216CC78A82B}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2197,7 +2197,7 @@
         <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>207</v>
@@ -2248,7 +2248,7 @@
         <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>179</v>
@@ -2344,7 +2344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469964C-8B5F-4244-8A02-3931FFBF20CD}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2403,13 +2403,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
@@ -2490,13 +2490,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
@@ -2519,13 +2519,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="F6" s="10">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
@@ -2548,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
@@ -2612,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H9" t="s">
         <v>30</v>
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H15" t="s">
         <v>32</v>
@@ -2809,13 +2809,13 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F16" s="10">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H16" t="s">
         <v>32</v>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F18" s="10">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H18" t="s">
         <v>30</v>
@@ -2954,13 +2954,13 @@
         <v>70</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>70</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>38</v>
@@ -2983,13 +2983,13 @@
         <v>70</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H22" t="s">
         <v>31</v>
@@ -3041,13 +3041,13 @@
         <v>0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>29</v>
@@ -3128,13 +3128,13 @@
         <v>70</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>38</v>
@@ -3157,13 +3157,13 @@
         <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H28" t="s">
         <v>31</v>
@@ -3220,8 +3220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD9CBC4-7F6E-494D-B5D8-9E8D7F427803}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3308,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -3598,13 +3598,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F13" s="10">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H13" t="s">
         <v>32</v>
@@ -3627,13 +3627,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H14" t="s">
         <v>32</v>
@@ -3801,13 +3801,13 @@
         <v>70</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>38</v>
@@ -3830,13 +3830,13 @@
         <v>70</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>70</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>31</v>
@@ -3903,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -3917,13 +3917,13 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>33</v>
@@ -4004,13 +4004,13 @@
         <v>71</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>71</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>47</v>

</xml_diff>